<commit_message>
GDE-9197 - Addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -22,18 +22,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -174,70 +167,70 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1484,8 +1477,8 @@
     <col width="18.85546875" bestFit="1" customWidth="1" style="31" min="42" max="42"/>
     <col width="14.28515625" bestFit="1" customWidth="1" style="31" min="43" max="43"/>
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
-    <col width="9.140625" customWidth="1" style="31" min="45" max="49"/>
-    <col width="9.140625" customWidth="1" style="31" min="50" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="45" max="51"/>
+    <col width="9.140625" customWidth="1" style="31" min="52" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">
@@ -1995,7 +1988,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2003,7 +1996,7 @@
     <col width="6.140625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="38.140625" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="24.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="27" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13.140625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="24.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="16.85546875" bestFit="1" customWidth="1" min="7" max="7"/>
@@ -2460,15 +2453,15 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
     <col width="6.140625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="38.140625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="27" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="13.140625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="24.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
@@ -2597,12 +2590,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>REVOLVER_FAC_</t>
+          <t>REV_CASH_ADVANCE_FAC_</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>REVOLVER_FAC_21124</t>
+          <t>REV_CASH_ADVANCE_FAC_12122</t>
         </is>
       </c>
       <c r="E2" s="35" t="inlineStr">

</xml_diff>

<commit_message>
GDE-9199 - initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C4E4E4-9748-4F12-8BE3-3C16C723D387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DF7B3-9D5F-4471-8EAC-D6A6DB934859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="CRED08_OngoingFeeSetup_A" sheetId="4" r:id="rId4"/>
     <sheet name="CRED02_FacilitySetup_B" sheetId="5" r:id="rId5"/>
     <sheet name="CRED08_OngoingFeeSetup_B" sheetId="6" r:id="rId6"/>
+    <sheet name="SYND02_PrimaryAllocation" sheetId="7" r:id="rId7"/>
+    <sheet name="CRED01_DealPricingSetup" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="340">
   <si>
     <t>rowid</t>
   </si>
@@ -970,6 +972,81 @@
   </si>
   <si>
     <t>01-Oct-2019</t>
+  </si>
+  <si>
+    <t>Setup Primaries</t>
+  </si>
+  <si>
+    <t>Technology, Media, Health and Education</t>
+  </si>
+  <si>
+    <t>Primary_RiskBook</t>
+  </si>
+  <si>
+    <t>Primaries_TransactionType</t>
+  </si>
+  <si>
+    <t>Origination</t>
+  </si>
+  <si>
+    <t>Primary_PctOfDeal</t>
+  </si>
+  <si>
+    <t>Primary_ExpectedCloseDate</t>
+  </si>
+  <si>
+    <t>Primary_Contact</t>
+  </si>
+  <si>
+    <t>Primary_SGAlias</t>
+  </si>
+  <si>
+    <t>Primary_CircledDate</t>
+  </si>
+  <si>
+    <t>Lender_Hostbank</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Primary_Portfolio</t>
+  </si>
+  <si>
+    <t>Primary_PortfolioBranch</t>
+  </si>
+  <si>
+    <t>Hold for Investment - Australia</t>
+  </si>
+  <si>
+    <t>Primary_ExpenseCode</t>
+  </si>
+  <si>
+    <t>Primary_BuySellPrice</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>ApproveDate</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
+  </si>
+  <si>
+    <t>02-Apr-2007</t>
+  </si>
+  <si>
+    <t>Update Deal Pricing</t>
+  </si>
+  <si>
+    <t>InterestPricingOption</t>
+  </si>
+  <si>
+    <t>Pricing_MatrixChangeAppMethod</t>
+  </si>
+  <si>
+    <t>Next repricing date</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1207,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1192,6 +1269,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -2104,10 +2182,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,11 +2234,13 @@
     <col min="42" max="42" width="18.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="24" style="31" bestFit="1" customWidth="1"/>
-    <col min="45" max="52" width="9.140625" style="31" customWidth="1"/>
+    <col min="45" max="45" width="13.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="47" max="52" width="9.140625" style="31" customWidth="1"/>
     <col min="53" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2293,8 +2373,14 @@
       <c r="AR1" s="22" t="s">
         <v>164</v>
       </c>
+      <c r="AS1" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>334</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>72</v>
       </c>
@@ -2427,8 +2513,14 @@
       <c r="AR2" s="33" t="s">
         <v>191</v>
       </c>
+      <c r="AS2" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="AT2" s="47" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
@@ -2474,7 +2566,7 @@
       <c r="AQ3" s="29"/>
       <c r="AR3" s="29"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="Y7" s="28"/>
     </row>
   </sheetData>
@@ -2491,7 +2583,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2636,7 +2728,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Date Format" prompt="ddmmyy" sqref="H2:J2" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2651,8 +2743,8 @@
   </sheetPr>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2963,8 +3055,8 @@
   </sheetPr>
   <dimension ref="A1:BB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3364,4 +3456,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDA1AD9-F354-4449-91AD-50ABFD2BD297}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102FC4BF-C81B-4322-9974-08C0D13FC4A2}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GDE-9201 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BDD877-2FAB-429F-AB80-01CE229E3772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F77CE4-CE32-47D4-BFD7-BD6B7CF71063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,25 @@
     <sheet name="CRED07_UpfrontFee_Payment" sheetId="9" r:id="rId9"/>
     <sheet name="Correspondence" sheetId="10" r:id="rId10"/>
     <sheet name="SERV01_LoanDrawdown" sheetId="11" r:id="rId11"/>
+    <sheet name="TRPO12_PortfolioSettledDisc" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="496">
   <si>
     <t>rowid</t>
   </si>
@@ -1076,9 +1088,6 @@
     <t>Charge Upfront fee</t>
   </si>
   <si>
-    <t>275,750</t>
-  </si>
-  <si>
     <t>27-Dec-2019</t>
   </si>
   <si>
@@ -1470,6 +1479,57 @@
   </si>
   <si>
     <t>Expctd_Loan_IntCycleFrequency</t>
+  </si>
+  <si>
+    <t>CashFlow_BeforeStatus</t>
+  </si>
+  <si>
+    <t>CashFlow_BeforeMethod</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>PEND</t>
+  </si>
+  <si>
+    <t>GLShortName</t>
+  </si>
+  <si>
+    <t>Special Acc't Pay.</t>
+  </si>
+  <si>
+    <t>Should be 27-Dec-2019</t>
+  </si>
+  <si>
+    <t>01-Nov-2022</t>
+  </si>
+  <si>
+    <t>CashFlow_AfterStatus</t>
+  </si>
+  <si>
+    <t>CashFlow_AfterMethod</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>GL_ShortName</t>
+  </si>
+  <si>
+    <t>GL_Offset_Type</t>
+  </si>
+  <si>
+    <t>Fees Held Awaiting Dispos.</t>
+  </si>
+  <si>
+    <t>Existing WIP</t>
+  </si>
+  <si>
+    <t>Portfolio Settled Discount Change</t>
+  </si>
+  <si>
+    <t>AdjustmentSelection</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1540,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
     <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1552,6 +1612,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1687,7 +1754,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1780,6 +1847,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -2781,196 +2852,196 @@
         <v>125</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E1" s="49" t="s">
         <v>197</v>
       </c>
       <c r="F1" s="49" t="s">
+        <v>354</v>
+      </c>
+      <c r="G1" s="58" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="H1" s="58" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="I1" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="J1" s="58" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="K1" s="60" t="s">
         <v>359</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="L1" s="58" t="s">
         <v>360</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="M1" s="61" t="s">
         <v>361</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="N1" s="61" t="s">
         <v>362</v>
       </c>
-      <c r="N1" s="61" t="s">
+      <c r="O1" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="P1" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="Q1" s="58" t="s">
         <v>365</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="R1" s="58" t="s">
         <v>366</v>
       </c>
-      <c r="R1" s="58" t="s">
+      <c r="S1" s="48" t="s">
         <v>367</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>368</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="U1" s="48" t="s">
         <v>369</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>370</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="W1" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>372</v>
       </c>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48" t="s">
         <v>374</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="AA1" s="48" t="s">
         <v>375</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AB1" s="48" t="s">
         <v>376</v>
       </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="AC1" s="50" t="s">
+      <c r="AD1" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="AD1" s="50" t="s">
+      <c r="AE1" s="50" t="s">
         <v>379</v>
       </c>
-      <c r="AE1" s="50" t="s">
+      <c r="AF1" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="AF1" s="51" t="s">
+      <c r="AG1" s="50" t="s">
         <v>381</v>
       </c>
-      <c r="AG1" s="50" t="s">
+      <c r="AH1" s="48" t="s">
         <v>382</v>
       </c>
-      <c r="AH1" s="48" t="s">
+      <c r="AI1" s="48" t="s">
         <v>383</v>
       </c>
-      <c r="AI1" s="48" t="s">
+      <c r="AJ1" s="49" t="s">
         <v>384</v>
       </c>
-      <c r="AJ1" s="49" t="s">
+      <c r="AK1" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="AK1" s="49" t="s">
+      <c r="AL1" s="48" t="s">
         <v>386</v>
       </c>
-      <c r="AL1" s="48" t="s">
+      <c r="AM1" s="48" t="s">
         <v>387</v>
       </c>
-      <c r="AM1" s="48" t="s">
+      <c r="AN1" s="48" t="s">
         <v>388</v>
       </c>
-      <c r="AN1" s="48" t="s">
+      <c r="AO1" s="48" t="s">
         <v>389</v>
-      </c>
-      <c r="AO1" s="48" t="s">
-        <v>390</v>
       </c>
       <c r="AP1" s="49" t="s">
         <v>227</v>
       </c>
       <c r="AQ1" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="AR1" s="52" t="s">
         <v>391</v>
       </c>
-      <c r="AR1" s="52" t="s">
+      <c r="AS1" s="48" t="s">
         <v>392</v>
       </c>
-      <c r="AS1" s="48" t="s">
+      <c r="AT1" s="52" t="s">
         <v>393</v>
       </c>
-      <c r="AT1" s="52" t="s">
+      <c r="AU1" s="48" t="s">
         <v>394</v>
       </c>
-      <c r="AU1" s="48" t="s">
+      <c r="AV1" s="48" t="s">
         <v>395</v>
       </c>
-      <c r="AV1" s="48" t="s">
+      <c r="AW1" s="48" t="s">
         <v>396</v>
       </c>
-      <c r="AW1" s="48" t="s">
+      <c r="AX1" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="AX1" s="48" t="s">
+      <c r="AY1" s="48" t="s">
         <v>398</v>
       </c>
-      <c r="AY1" s="48" t="s">
+      <c r="AZ1" s="48" t="s">
         <v>399</v>
       </c>
-      <c r="AZ1" s="48" t="s">
+      <c r="BA1" s="48" t="s">
         <v>400</v>
       </c>
-      <c r="BA1" s="48" t="s">
+      <c r="BB1" s="48" t="s">
         <v>401</v>
       </c>
-      <c r="BB1" s="48" t="s">
+      <c r="BC1" s="48" t="s">
         <v>402</v>
       </c>
-      <c r="BC1" s="48" t="s">
+      <c r="BD1" s="48" t="s">
         <v>403</v>
       </c>
-      <c r="BD1" s="48" t="s">
+      <c r="BE1" s="48" t="s">
         <v>404</v>
       </c>
-      <c r="BE1" s="48" t="s">
+      <c r="BF1" s="48" t="s">
         <v>405</v>
       </c>
-      <c r="BF1" s="48" t="s">
+      <c r="BG1" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="BG1" s="48" t="s">
+      <c r="BH1" s="48" t="s">
         <v>407</v>
       </c>
-      <c r="BH1" s="48" t="s">
+      <c r="BI1" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="BI1" s="48" t="s">
+      <c r="BJ1" s="58" t="s">
         <v>409</v>
-      </c>
-      <c r="BJ1" s="58" t="s">
-        <v>410</v>
       </c>
       <c r="BK1" s="58" t="s">
         <v>340</v>
       </c>
       <c r="BL1" s="58" t="s">
+        <v>410</v>
+      </c>
+      <c r="BM1" s="58" t="s">
         <v>411</v>
-      </c>
-      <c r="BM1" s="58" t="s">
-        <v>412</v>
       </c>
       <c r="BN1" s="58" t="s">
         <v>342</v>
       </c>
       <c r="BO1" s="58" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2978,127 +3049,127 @@
         <v>72</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>414</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>415</v>
       </c>
       <c r="D2" s="70" t="s">
         <v>99</v>
       </c>
       <c r="E2" s="63" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2" s="63" t="s">
         <v>416</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="G2" s="70" t="s">
         <v>417</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="H2" s="66" t="s">
         <v>418</v>
       </c>
-      <c r="H2" s="66" t="s">
+      <c r="I2" s="70" t="s">
         <v>419</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="J2" s="70" t="s">
         <v>420</v>
       </c>
-      <c r="J2" s="70" t="s">
+      <c r="K2" s="70" t="s">
         <v>421</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="L2" s="70" t="s">
         <v>422</v>
-      </c>
-      <c r="L2" s="70" t="s">
-        <v>423</v>
       </c>
       <c r="M2" s="66">
         <v>5</v>
       </c>
       <c r="N2" s="66" t="s">
+        <v>423</v>
+      </c>
+      <c r="O2" s="67" t="s">
         <v>424</v>
-      </c>
-      <c r="O2" s="67" t="s">
-        <v>425</v>
       </c>
       <c r="P2" s="67" t="s">
         <v>107</v>
       </c>
       <c r="Q2" s="70" t="s">
+        <v>425</v>
+      </c>
+      <c r="R2" s="70" t="s">
+        <v>425</v>
+      </c>
+      <c r="S2" s="67" t="s">
         <v>426</v>
       </c>
-      <c r="R2" s="70" t="s">
-        <v>426</v>
-      </c>
-      <c r="S2" s="67" t="s">
+      <c r="T2" s="67" t="s">
         <v>427</v>
       </c>
-      <c r="T2" s="67" t="s">
+      <c r="U2" s="67" t="s">
         <v>428</v>
       </c>
-      <c r="U2" s="67" t="s">
+      <c r="V2" s="67" t="s">
         <v>429</v>
       </c>
-      <c r="V2" s="67" t="s">
+      <c r="W2" s="68" t="s">
         <v>430</v>
       </c>
-      <c r="W2" s="68" t="s">
+      <c r="X2" s="68" t="s">
         <v>431</v>
       </c>
-      <c r="X2" s="68" t="s">
+      <c r="Y2" s="68" t="s">
         <v>432</v>
       </c>
-      <c r="Y2" s="68" t="s">
+      <c r="Z2" s="68" t="s">
         <v>433</v>
       </c>
-      <c r="Z2" s="68" t="s">
+      <c r="AA2" s="68" t="s">
         <v>434</v>
       </c>
-      <c r="AA2" s="68" t="s">
+      <c r="AB2" s="68" t="s">
         <v>435</v>
-      </c>
-      <c r="AB2" s="68" t="s">
-        <v>436</v>
       </c>
       <c r="AC2" s="63"/>
       <c r="AD2" s="68" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AE2" s="68"/>
       <c r="AF2" s="69"/>
       <c r="AG2" s="63"/>
       <c r="AH2" s="67" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AI2" s="63"/>
       <c r="AJ2" s="66" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AK2" s="63"/>
       <c r="AL2" s="64" t="s">
+        <v>439</v>
+      </c>
+      <c r="AM2" s="64" t="s">
         <v>440</v>
       </c>
-      <c r="AM2" s="64" t="s">
+      <c r="AN2" s="64" t="s">
         <v>441</v>
       </c>
-      <c r="AN2" s="64" t="s">
+      <c r="AO2" s="64" t="s">
         <v>442</v>
-      </c>
-      <c r="AO2" s="64" t="s">
-        <v>443</v>
       </c>
       <c r="AP2" s="63"/>
       <c r="AQ2" s="63"/>
       <c r="AR2" s="65"/>
       <c r="AS2" s="64" t="s">
+        <v>443</v>
+      </c>
+      <c r="AT2" s="64" t="s">
         <v>444</v>
       </c>
-      <c r="AT2" s="64" t="s">
+      <c r="AU2" s="64" t="s">
         <v>445</v>
       </c>
-      <c r="AU2" s="64" t="s">
+      <c r="AV2" s="64" t="s">
         <v>446</v>
-      </c>
-      <c r="AV2" s="64" t="s">
-        <v>447</v>
       </c>
       <c r="AW2" s="64"/>
       <c r="AX2" s="64"/>
@@ -3114,10 +3185,10 @@
       <c r="BH2" s="64"/>
       <c r="BI2" s="64"/>
       <c r="BJ2" s="62" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BK2" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BL2" s="62" t="s">
         <v>93</v>
@@ -3126,7 +3197,7 @@
         <v>113</v>
       </c>
       <c r="BN2" s="62" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BO2" s="62" t="s">
         <v>172</v>
@@ -3134,7 +3205,7 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="C3" s="53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D3" s="59"/>
       <c r="G3" s="57"/>
@@ -3173,8 +3244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3215,37 +3286,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D1" s="71" t="s">
+        <v>449</v>
+      </c>
+      <c r="E1" s="71" t="s">
         <v>450</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="F1" s="71" t="s">
         <v>451</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="G1" s="71" t="s">
         <v>452</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="H1" s="71" t="s">
+        <v>392</v>
+      </c>
+      <c r="I1" s="71" t="s">
+        <v>393</v>
+      </c>
+      <c r="J1" s="71" t="s">
         <v>453</v>
       </c>
-      <c r="H1" s="71" t="s">
-        <v>393</v>
-      </c>
-      <c r="I1" s="71" t="s">
-        <v>394</v>
-      </c>
-      <c r="J1" s="71" t="s">
+      <c r="K1" s="71" t="s">
+        <v>464</v>
+      </c>
+      <c r="L1" s="71" t="s">
         <v>454</v>
       </c>
-      <c r="K1" s="71" t="s">
-        <v>465</v>
-      </c>
-      <c r="L1" s="71" t="s">
-        <v>455</v>
-      </c>
       <c r="M1" s="71" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N1" s="71" t="s">
         <v>345</v>
@@ -3254,37 +3325,37 @@
         <v>346</v>
       </c>
       <c r="P1" s="71" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q1" s="71" t="s">
         <v>456</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="R1" s="71" t="s">
         <v>457</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="S1" s="71" t="s">
         <v>458</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="T1" s="71" t="s">
         <v>459</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="U1" s="71" t="s">
         <v>460</v>
       </c>
-      <c r="U1" s="71" t="s">
+      <c r="V1" s="71" t="s">
         <v>461</v>
       </c>
-      <c r="V1" s="71" t="s">
+      <c r="W1" s="71" t="s">
         <v>462</v>
       </c>
-      <c r="W1" s="71" t="s">
+      <c r="X1" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="X1" s="71" t="s">
-        <v>464</v>
-      </c>
       <c r="Y1" s="71" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Z1" s="71" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -3292,10 +3363,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" s="35" t="s">
         <v>466</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>467</v>
       </c>
       <c r="D2" t="s">
         <v>221</v>
@@ -3307,7 +3378,7 @@
         <v>113</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H2" s="37" t="s">
         <v>218</v>
@@ -3316,56 +3387,123 @@
         <v>220</v>
       </c>
       <c r="J2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K2" s="46" t="s">
         <v>105</v>
       </c>
       <c r="L2" t="s">
+        <v>468</v>
+      </c>
+      <c r="M2" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="N2" t="s">
+        <v>351</v>
+      </c>
+      <c r="O2" t="s">
         <v>470</v>
       </c>
-      <c r="N2" t="s">
-        <v>352</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>471</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="U2" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="Q2" s="37" t="s">
-        <v>448</v>
-      </c>
-      <c r="R2" s="37" t="s">
-        <v>448</v>
-      </c>
-      <c r="S2" s="37" t="s">
-        <v>448</v>
-      </c>
-      <c r="T2" s="37" t="s">
-        <v>448</v>
-      </c>
-      <c r="U2" s="37" t="s">
+      <c r="V2" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="W2" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="X2" t="s">
         <v>475</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>476</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>477</v>
       </c>
       <c r="Z2" t="s">
         <v>105</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDCF721-02DF-47DA-B0C7-58C5A045C4B7}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="75" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="75" customWidth="1"/>
+    <col min="6" max="19" width="8.7109375" style="75" customWidth="1"/>
+    <col min="20" max="16384" width="8.7109375" style="75"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="74" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>495</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>494</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>492</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3380,8 +3518,8 @@
   </sheetPr>
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,8 +3916,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3924,7 +4062,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Date Format" prompt="ddmmyy" sqref="H2:J2" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3939,9 +4077,7 @@
   </sheetPr>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4655,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4673,7 +4809,7 @@
     <col min="11" max="11" width="16.85546875" style="46" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.28515625" style="46" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" style="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -4820,10 +4956,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4836,9 +4972,14 @@
     <col min="7" max="7" width="33.140625" style="46" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="46" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="49.42578125" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4866,8 +5007,23 @@
       <c r="I1" s="22" t="s">
         <v>346</v>
       </c>
+      <c r="J1" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>488</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>72</v>
       </c>
@@ -4875,28 +5031,49 @@
         <v>347</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>348</v>
+        <v>447</v>
       </c>
       <c r="D2" s="37" t="s">
+        <v>486</v>
+      </c>
+      <c r="E2" t="s">
         <v>349</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>350</v>
-      </c>
-      <c r="F2" t="s">
-        <v>351</v>
       </c>
       <c r="G2" t="s">
         <v>107</v>
       </c>
       <c r="H2" t="s">
+        <v>351</v>
+      </c>
+      <c r="I2" t="s">
         <v>352</v>
       </c>
-      <c r="I2" t="s">
-        <v>353</v>
+      <c r="J2" t="s">
+        <v>482</v>
+      </c>
+      <c r="K2" t="s">
+        <v>481</v>
+      </c>
+      <c r="L2" t="s">
+        <v>484</v>
+      </c>
+      <c r="M2" s="46" t="s">
+        <v>489</v>
+      </c>
+      <c r="N2" s="46" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D3" s="72" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GDE-9402 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -244,7 +244,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -305,7 +305,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -717,22 +716,22 @@
     <col width="33" bestFit="1" customWidth="1" style="9" min="54" max="54"/>
     <col width="24.85546875" customWidth="1" style="9" min="55" max="55"/>
     <col width="20" customWidth="1" style="9" min="56" max="56"/>
-    <col width="22.5703125" bestFit="1" customWidth="1" style="77" min="57" max="57"/>
-    <col width="16" bestFit="1" customWidth="1" style="77" min="58" max="58"/>
-    <col width="26" bestFit="1" customWidth="1" style="77" min="59" max="59"/>
-    <col width="26.42578125" bestFit="1" customWidth="1" style="77" min="60" max="60"/>
-    <col width="21.5703125" bestFit="1" customWidth="1" style="77" min="61" max="61"/>
-    <col width="19.140625" bestFit="1" customWidth="1" style="77" min="62" max="62"/>
-    <col width="32.5703125" bestFit="1" customWidth="1" style="77" min="63" max="63"/>
-    <col width="34.28515625" bestFit="1" customWidth="1" style="77" min="64" max="64"/>
-    <col width="31.7109375" bestFit="1" customWidth="1" style="77" min="65" max="65"/>
-    <col width="22" bestFit="1" customWidth="1" style="77" min="66" max="66"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="77" min="67" max="67"/>
-    <col width="18.140625" bestFit="1" customWidth="1" style="77" min="68" max="68"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="77" min="69" max="69"/>
-    <col width="25.85546875" bestFit="1" customWidth="1" style="77" min="70" max="70"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="77" min="71" max="71"/>
-    <col width="25.7109375" bestFit="1" customWidth="1" style="77" min="72" max="72"/>
+    <col width="22.5703125" bestFit="1" customWidth="1" style="76" min="57" max="57"/>
+    <col width="16" bestFit="1" customWidth="1" style="76" min="58" max="58"/>
+    <col width="26" bestFit="1" customWidth="1" style="76" min="59" max="59"/>
+    <col width="26.42578125" bestFit="1" customWidth="1" style="76" min="60" max="60"/>
+    <col width="21.5703125" bestFit="1" customWidth="1" style="76" min="61" max="61"/>
+    <col width="19.140625" bestFit="1" customWidth="1" style="76" min="62" max="62"/>
+    <col width="32.5703125" bestFit="1" customWidth="1" style="76" min="63" max="63"/>
+    <col width="34.28515625" bestFit="1" customWidth="1" style="76" min="64" max="64"/>
+    <col width="31.7109375" bestFit="1" customWidth="1" style="76" min="65" max="65"/>
+    <col width="22" bestFit="1" customWidth="1" style="76" min="66" max="66"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="76" min="67" max="67"/>
+    <col width="18.140625" bestFit="1" customWidth="1" style="76" min="68" max="68"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="76" min="69" max="69"/>
+    <col width="25.85546875" bestFit="1" customWidth="1" style="76" min="70" max="70"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="71" max="71"/>
+    <col width="25.7109375" bestFit="1" customWidth="1" style="76" min="72" max="72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="5">
@@ -1543,690 +1542,690 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="6.5703125" customWidth="1" style="55" min="1" max="1"/>
-    <col width="22" bestFit="1" customWidth="1" style="55" min="2" max="2"/>
-    <col width="27.42578125" bestFit="1" customWidth="1" style="53" min="3" max="3"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="55" min="4" max="4"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="53" min="5" max="5"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="53" min="6" max="6"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" style="53" min="7" max="7"/>
-    <col width="20" customWidth="1" style="53" min="8" max="8"/>
-    <col width="16.42578125" customWidth="1" style="55" min="9" max="9"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="53" min="10" max="10"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="55" min="11" max="12"/>
-    <col width="13.85546875" bestFit="1" customWidth="1" style="55" min="13" max="13"/>
-    <col width="50.7109375" bestFit="1" customWidth="1" style="55" min="14" max="14"/>
-    <col width="16.42578125" customWidth="1" style="55" min="15" max="15"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="55" min="16" max="16"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="55" min="17" max="18"/>
-    <col width="23" bestFit="1" customWidth="1" style="53" min="19" max="19"/>
-    <col width="39" bestFit="1" customWidth="1" style="53" min="20" max="20"/>
-    <col width="65.28515625" bestFit="1" customWidth="1" style="53" min="21" max="21"/>
-    <col width="14" customWidth="1" style="53" min="22" max="22"/>
-    <col width="20" customWidth="1" style="53" min="23" max="23"/>
-    <col width="20.5703125" customWidth="1" style="53" min="24" max="24"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" style="53" min="25" max="25"/>
-    <col width="66.7109375" bestFit="1" customWidth="1" style="53" min="26" max="26"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="53" min="27" max="27"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="53" min="28" max="28"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="53" min="29" max="29"/>
-    <col width="16" customWidth="1" style="53" min="30" max="30"/>
-    <col width="17" customWidth="1" style="53" min="31" max="31"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="56" min="32" max="32"/>
-    <col width="16.7109375" customWidth="1" style="53" min="33" max="33"/>
-    <col width="13.85546875" bestFit="1" customWidth="1" style="53" min="34" max="34"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="53" min="35" max="35"/>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="53" min="36" max="36"/>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="53" min="37" max="37"/>
-    <col width="15.42578125" bestFit="1" customWidth="1" style="53" min="38" max="38"/>
-    <col width="13.42578125" customWidth="1" style="53" min="39" max="39"/>
-    <col width="16.140625" customWidth="1" style="53" min="40" max="40"/>
-    <col width="15.42578125" customWidth="1" style="53" min="41" max="41"/>
-    <col width="18.140625" bestFit="1" customWidth="1" style="53" min="42" max="42"/>
-    <col width="16.7109375" bestFit="1" customWidth="1" style="53" min="43" max="43"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="53" min="44" max="44"/>
-    <col width="19" bestFit="1" customWidth="1" style="53" min="45" max="45"/>
-    <col width="18.5703125" bestFit="1" customWidth="1" style="53" min="46" max="46"/>
-    <col width="20.140625" bestFit="1" customWidth="1" style="53" min="47" max="47"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="53" min="48" max="48"/>
-    <col width="19.85546875" bestFit="1" customWidth="1" style="53" min="49" max="49"/>
-    <col width="30.85546875" bestFit="1" customWidth="1" style="53" min="50" max="50"/>
-    <col width="30.28515625" bestFit="1" customWidth="1" style="53" min="51" max="51"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="53" min="52" max="52"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="53" min="53" max="53"/>
-    <col width="18.85546875" bestFit="1" customWidth="1" style="53" min="54" max="54"/>
-    <col width="18" bestFit="1" customWidth="1" style="53" min="55" max="55"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="53" min="56" max="56"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="53" min="57" max="57"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="53" min="58" max="58"/>
-    <col width="17.140625" bestFit="1" customWidth="1" style="53" min="59" max="59"/>
-    <col width="14.140625" bestFit="1" customWidth="1" style="53" min="60" max="60"/>
-    <col width="17.140625" bestFit="1" customWidth="1" style="53" min="61" max="61"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="53" min="62" max="62"/>
-    <col width="20.140625" bestFit="1" customWidth="1" style="53" min="63" max="63"/>
-    <col width="40.7109375" bestFit="1" customWidth="1" style="53" min="64" max="64"/>
-    <col width="9.7109375" bestFit="1" customWidth="1" style="53" min="65" max="65"/>
-    <col width="26" bestFit="1" customWidth="1" style="53" min="66" max="66"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="53" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="53" min="68" max="126"/>
-    <col width="9.140625" customWidth="1" style="53" min="127" max="16384"/>
+    <col width="6.5703125" customWidth="1" style="54" min="1" max="1"/>
+    <col width="22" bestFit="1" customWidth="1" style="54" min="2" max="2"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="52" min="3" max="3"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="54" min="4" max="4"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="52" min="5" max="5"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" style="52" min="6" max="6"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" style="52" min="7" max="7"/>
+    <col width="20" customWidth="1" style="52" min="8" max="8"/>
+    <col width="16.42578125" customWidth="1" style="54" min="9" max="9"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="52" min="10" max="10"/>
+    <col width="22.140625" bestFit="1" customWidth="1" style="54" min="11" max="12"/>
+    <col width="13.85546875" bestFit="1" customWidth="1" style="54" min="13" max="13"/>
+    <col width="50.7109375" bestFit="1" customWidth="1" style="54" min="14" max="14"/>
+    <col width="16.42578125" customWidth="1" style="54" min="15" max="15"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="54" min="16" max="16"/>
+    <col width="22.140625" bestFit="1" customWidth="1" style="54" min="17" max="18"/>
+    <col width="23" bestFit="1" customWidth="1" style="52" min="19" max="19"/>
+    <col width="39" bestFit="1" customWidth="1" style="52" min="20" max="20"/>
+    <col width="65.28515625" bestFit="1" customWidth="1" style="52" min="21" max="21"/>
+    <col width="14" customWidth="1" style="52" min="22" max="22"/>
+    <col width="20" customWidth="1" style="52" min="23" max="23"/>
+    <col width="20.5703125" customWidth="1" style="52" min="24" max="24"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" style="52" min="25" max="25"/>
+    <col width="66.7109375" bestFit="1" customWidth="1" style="52" min="26" max="26"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="52" min="27" max="27"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="52" min="28" max="28"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" style="52" min="29" max="29"/>
+    <col width="16" customWidth="1" style="52" min="30" max="30"/>
+    <col width="17" customWidth="1" style="52" min="31" max="31"/>
+    <col width="14.7109375" bestFit="1" customWidth="1" style="55" min="32" max="32"/>
+    <col width="16.7109375" customWidth="1" style="52" min="33" max="33"/>
+    <col width="13.85546875" bestFit="1" customWidth="1" style="52" min="34" max="34"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="52" min="35" max="35"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="52" min="36" max="36"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="52" min="37" max="37"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" style="52" min="38" max="38"/>
+    <col width="13.42578125" customWidth="1" style="52" min="39" max="39"/>
+    <col width="16.140625" customWidth="1" style="52" min="40" max="40"/>
+    <col width="15.42578125" customWidth="1" style="52" min="41" max="41"/>
+    <col width="18.140625" bestFit="1" customWidth="1" style="52" min="42" max="42"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" style="52" min="43" max="43"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" style="52" min="44" max="44"/>
+    <col width="19" bestFit="1" customWidth="1" style="52" min="45" max="45"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="52" min="46" max="46"/>
+    <col width="20.140625" bestFit="1" customWidth="1" style="52" min="47" max="47"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="52" min="48" max="48"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="52" min="49" max="49"/>
+    <col width="30.85546875" bestFit="1" customWidth="1" style="52" min="50" max="50"/>
+    <col width="30.28515625" bestFit="1" customWidth="1" style="52" min="51" max="51"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="52" min="52" max="52"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="52" min="53" max="53"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="52" min="54" max="54"/>
+    <col width="18" bestFit="1" customWidth="1" style="52" min="55" max="55"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="52" min="56" max="56"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="52" min="57" max="57"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="52" min="58" max="58"/>
+    <col width="17.140625" bestFit="1" customWidth="1" style="52" min="59" max="59"/>
+    <col width="14.140625" bestFit="1" customWidth="1" style="52" min="60" max="60"/>
+    <col width="17.140625" bestFit="1" customWidth="1" style="52" min="61" max="61"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" style="52" min="62" max="62"/>
+    <col width="20.140625" bestFit="1" customWidth="1" style="52" min="63" max="63"/>
+    <col width="40.7109375" bestFit="1" customWidth="1" style="52" min="64" max="64"/>
+    <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
+    <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="127"/>
+    <col width="9.140625" customWidth="1" style="52" min="128" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.15" customHeight="1" s="77">
-      <c r="A1" s="48" t="inlineStr">
+    <row r="1" ht="13.15" customHeight="1" s="76">
+      <c r="A1" s="47" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="48" t="inlineStr">
+      <c r="B1" s="47" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="49" t="inlineStr">
+      <c r="C1" s="48" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="58" t="inlineStr">
+      <c r="D1" s="57" t="inlineStr">
         <is>
           <t>Notice_Customer_LegalName</t>
         </is>
       </c>
-      <c r="E1" s="49" t="inlineStr">
+      <c r="E1" s="48" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="F1" s="49" t="inlineStr">
+      <c r="F1" s="48" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="G1" s="58" t="inlineStr">
+      <c r="G1" s="57" t="inlineStr">
         <is>
           <t>Contact</t>
         </is>
       </c>
-      <c r="H1" s="58" t="inlineStr">
+      <c r="H1" s="57" t="inlineStr">
         <is>
           <t>NoticeGroup_UserID</t>
         </is>
       </c>
-      <c r="I1" s="58" t="inlineStr">
+      <c r="I1" s="57" t="inlineStr">
         <is>
           <t>Notice_Identifier</t>
         </is>
       </c>
-      <c r="J1" s="58" t="inlineStr">
+      <c r="J1" s="57" t="inlineStr">
         <is>
           <t>Correlation_ID</t>
         </is>
       </c>
-      <c r="K1" s="60" t="inlineStr">
+      <c r="K1" s="59" t="inlineStr">
         <is>
           <t>Thru_Date</t>
         </is>
       </c>
-      <c r="L1" s="58" t="inlineStr">
+      <c r="L1" s="57" t="inlineStr">
         <is>
           <t>From_Date</t>
         </is>
       </c>
-      <c r="M1" s="61" t="inlineStr">
+      <c r="M1" s="60" t="inlineStr">
         <is>
           <t>SubAdd_Days</t>
         </is>
       </c>
-      <c r="N1" s="61" t="inlineStr">
+      <c r="N1" s="60" t="inlineStr">
         <is>
           <t>Notice_Type</t>
         </is>
       </c>
-      <c r="O1" s="48" t="inlineStr">
+      <c r="O1" s="47" t="inlineStr">
         <is>
           <t>Search_By</t>
         </is>
       </c>
-      <c r="P1" s="48" t="inlineStr">
+      <c r="P1" s="47" t="inlineStr">
         <is>
           <t>Notice_Method</t>
         </is>
       </c>
-      <c r="Q1" s="58" t="inlineStr">
+      <c r="Q1" s="57" t="inlineStr">
         <is>
           <t>BEO_StartDate</t>
         </is>
       </c>
-      <c r="R1" s="58" t="inlineStr">
+      <c r="R1" s="57" t="inlineStr">
         <is>
           <t>BEO_EndDate</t>
         </is>
       </c>
-      <c r="S1" s="48" t="inlineStr">
+      <c r="S1" s="47" t="inlineStr">
         <is>
           <t>Customer_IdentifiedBy</t>
         </is>
       </c>
-      <c r="T1" s="48" t="inlineStr">
+      <c r="T1" s="47" t="inlineStr">
         <is>
           <t>Zero_TempPath</t>
         </is>
       </c>
-      <c r="U1" s="48" t="inlineStr">
+      <c r="U1" s="47" t="inlineStr">
         <is>
           <t>InputFilePath</t>
         </is>
       </c>
-      <c r="V1" s="48" t="inlineStr">
+      <c r="V1" s="47" t="inlineStr">
         <is>
           <t>XML_File</t>
         </is>
       </c>
-      <c r="W1" s="48" t="inlineStr">
+      <c r="W1" s="47" t="inlineStr">
         <is>
           <t>Temp_File</t>
         </is>
       </c>
-      <c r="X1" s="48" t="inlineStr">
+      <c r="X1" s="47" t="inlineStr">
         <is>
           <t>InputJson</t>
         </is>
       </c>
-      <c r="Y1" s="48" t="inlineStr">
+      <c r="Y1" s="47" t="inlineStr">
         <is>
           <t>ExpectedJson</t>
         </is>
       </c>
-      <c r="Z1" s="48" t="inlineStr">
+      <c r="Z1" s="47" t="inlineStr">
         <is>
           <t>OutputFilePath</t>
         </is>
       </c>
-      <c r="AA1" s="48" t="inlineStr">
+      <c r="AA1" s="47" t="inlineStr">
         <is>
           <t>Field_Name</t>
         </is>
       </c>
-      <c r="AB1" s="48" t="inlineStr">
+      <c r="AB1" s="47" t="inlineStr">
         <is>
           <t>OutputAPIResponse</t>
         </is>
       </c>
-      <c r="AC1" s="50" t="inlineStr">
+      <c r="AC1" s="49" t="inlineStr">
         <is>
           <t>messageId</t>
         </is>
       </c>
-      <c r="AD1" s="50" t="inlineStr">
+      <c r="AD1" s="49" t="inlineStr">
         <is>
           <t>CallBack_Status</t>
         </is>
       </c>
-      <c r="AE1" s="50" t="inlineStr">
+      <c r="AE1" s="49" t="inlineStr">
         <is>
           <t>CallBack_Status2</t>
         </is>
       </c>
-      <c r="AF1" s="51" t="inlineStr">
+      <c r="AF1" s="50" t="inlineStr">
         <is>
           <t>errorMessage</t>
         </is>
       </c>
-      <c r="AG1" s="50" t="inlineStr">
+      <c r="AG1" s="49" t="inlineStr">
         <is>
           <t>errorMessage_2</t>
         </is>
       </c>
-      <c r="AH1" s="48" t="inlineStr">
+      <c r="AH1" s="47" t="inlineStr">
         <is>
           <t>Notice_Status</t>
         </is>
       </c>
-      <c r="AI1" s="48" t="inlineStr">
+      <c r="AI1" s="47" t="inlineStr">
         <is>
           <t>WIP_ExceptionQueueDescription</t>
         </is>
       </c>
-      <c r="AJ1" s="49" t="inlineStr">
+      <c r="AJ1" s="48" t="inlineStr">
         <is>
           <t>XML_NoticeType</t>
         </is>
       </c>
-      <c r="AK1" s="49" t="inlineStr">
+      <c r="AK1" s="48" t="inlineStr">
         <is>
           <t>Loan_PricingOption</t>
         </is>
       </c>
-      <c r="AL1" s="48" t="inlineStr">
+      <c r="AL1" s="47" t="inlineStr">
         <is>
           <t>Loan_BaseRate</t>
         </is>
       </c>
-      <c r="AM1" s="48" t="inlineStr">
+      <c r="AM1" s="47" t="inlineStr">
         <is>
           <t>Loan_Spread</t>
         </is>
       </c>
-      <c r="AN1" s="48" t="inlineStr">
+      <c r="AN1" s="47" t="inlineStr">
         <is>
           <t>Notice_AllInRate</t>
         </is>
       </c>
-      <c r="AO1" s="48" t="inlineStr">
+      <c r="AO1" s="47" t="inlineStr">
         <is>
           <t>Notice_Amount</t>
         </is>
       </c>
-      <c r="AP1" s="49" t="inlineStr">
+      <c r="AP1" s="48" t="inlineStr">
         <is>
           <t>OngoingFee_Type</t>
         </is>
       </c>
-      <c r="AQ1" s="48" t="inlineStr">
+      <c r="AQ1" s="47" t="inlineStr">
         <is>
           <t>Balance_Amount</t>
         </is>
       </c>
-      <c r="AR1" s="52" t="inlineStr">
+      <c r="AR1" s="51" t="inlineStr">
         <is>
           <t>Rate_Basis</t>
         </is>
       </c>
-      <c r="AS1" s="48" t="inlineStr">
+      <c r="AS1" s="47" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="AT1" s="52" t="inlineStr">
+      <c r="AT1" s="51" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="AU1" s="48" t="inlineStr">
+      <c r="AU1" s="47" t="inlineStr">
         <is>
           <t>Loan_GlobalOriginal</t>
         </is>
       </c>
-      <c r="AV1" s="48" t="inlineStr">
+      <c r="AV1" s="47" t="inlineStr">
         <is>
           <t>Loan_RateSetting_DueDate</t>
         </is>
       </c>
-      <c r="AW1" s="48" t="inlineStr">
+      <c r="AW1" s="47" t="inlineStr">
         <is>
           <t>Loan_RepricingDate</t>
         </is>
       </c>
-      <c r="AX1" s="48" t="inlineStr">
+      <c r="AX1" s="47" t="inlineStr">
         <is>
           <t>EffectiveDate_PrincipalPayment</t>
         </is>
       </c>
-      <c r="AY1" s="48" t="inlineStr">
+      <c r="AY1" s="47" t="inlineStr">
         <is>
           <t>Outstanding_PrincipalPayment</t>
         </is>
       </c>
-      <c r="AZ1" s="48" t="inlineStr">
+      <c r="AZ1" s="47" t="inlineStr">
         <is>
           <t>EffectiveDate_InterestPayment</t>
         </is>
       </c>
-      <c r="BA1" s="48" t="inlineStr">
+      <c r="BA1" s="47" t="inlineStr">
         <is>
           <t>ProjectedCycleDue_InterestPayment</t>
         </is>
       </c>
-      <c r="BB1" s="48" t="inlineStr">
+      <c r="BB1" s="47" t="inlineStr">
         <is>
           <t>StartDate_Principal</t>
         </is>
       </c>
-      <c r="BC1" s="48" t="inlineStr">
+      <c r="BC1" s="47" t="inlineStr">
         <is>
           <t>EndDate_Principal</t>
         </is>
       </c>
-      <c r="BD1" s="48" t="inlineStr">
+      <c r="BD1" s="47" t="inlineStr">
         <is>
           <t>Days_Principal</t>
         </is>
       </c>
-      <c r="BE1" s="48" t="inlineStr">
+      <c r="BE1" s="47" t="inlineStr">
         <is>
           <t>Principal_Amount</t>
         </is>
       </c>
-      <c r="BF1" s="48" t="inlineStr">
+      <c r="BF1" s="47" t="inlineStr">
         <is>
           <t>StartDate_Interest</t>
         </is>
       </c>
-      <c r="BG1" s="48" t="inlineStr">
+      <c r="BG1" s="47" t="inlineStr">
         <is>
           <t>EndDate_Interest</t>
         </is>
       </c>
-      <c r="BH1" s="48" t="inlineStr">
+      <c r="BH1" s="47" t="inlineStr">
         <is>
           <t>Days_Interest</t>
         </is>
       </c>
-      <c r="BI1" s="48" t="inlineStr">
+      <c r="BI1" s="47" t="inlineStr">
         <is>
           <t>Interest_Amount</t>
         </is>
       </c>
-      <c r="BJ1" s="58" t="inlineStr">
+      <c r="BJ1" s="57" t="inlineStr">
         <is>
           <t>Effective_Date</t>
         </is>
       </c>
-      <c r="BK1" s="58" t="inlineStr">
+      <c r="BK1" s="57" t="inlineStr">
         <is>
           <t>UpfrontFee_Amount</t>
         </is>
       </c>
-      <c r="BL1" s="58" t="inlineStr">
+      <c r="BL1" s="57" t="inlineStr">
         <is>
           <t>Branch_Description</t>
         </is>
       </c>
-      <c r="BM1" s="58" t="inlineStr">
+      <c r="BM1" s="57" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="BN1" s="58" t="inlineStr">
+      <c r="BN1" s="57" t="inlineStr">
         <is>
           <t>Fee_Type</t>
         </is>
       </c>
-      <c r="BO1" s="58" t="inlineStr">
+      <c r="BO1" s="57" t="inlineStr">
         <is>
           <t>Account_Name</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="77">
-      <c r="A2" s="53" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="76">
+      <c r="A2" s="52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="54" t="inlineStr">
+      <c r="B2" s="53" t="inlineStr">
         <is>
           <t>Upfront Fee Intent Notice</t>
         </is>
       </c>
-      <c r="C2" s="64" t="inlineStr">
+      <c r="C2" s="63" t="inlineStr">
         <is>
           <t>CBANLD_03112020160326YZJ</t>
         </is>
       </c>
-      <c r="D2" s="70" t="inlineStr">
+      <c r="D2" s="69" t="inlineStr">
         <is>
           <t>CH EDU Limited 1710818</t>
         </is>
       </c>
-      <c r="E2" s="63" t="inlineStr">
+      <c r="E2" s="62" t="inlineStr">
         <is>
           <t>CBANLDNAFAC03112020161931</t>
         </is>
       </c>
-      <c r="F2" s="63" t="inlineStr">
+      <c r="F2" s="62" t="inlineStr">
         <is>
           <t>60000035</t>
         </is>
       </c>
-      <c r="G2" s="70" t="inlineStr">
+      <c r="G2" s="69" t="inlineStr">
         <is>
           <t>Linda Chu</t>
         </is>
       </c>
-      <c r="H2" s="66" t="inlineStr">
+      <c r="H2" s="65" t="inlineStr">
         <is>
           <t>LOANIQ01</t>
         </is>
       </c>
-      <c r="I2" s="70" t="inlineStr">
+      <c r="I2" s="69" t="inlineStr">
         <is>
           <t>@1EL8J83</t>
         </is>
       </c>
-      <c r="J2" s="70" t="inlineStr">
+      <c r="J2" s="69" t="inlineStr">
         <is>
           <t>LIQ-@1EL8J83-@1EL8J61-3</t>
         </is>
       </c>
-      <c r="K2" s="70" t="inlineStr">
+      <c r="K2" s="69" t="inlineStr">
         <is>
           <t>2020-12-20 00:00:00.000</t>
         </is>
       </c>
-      <c r="L2" s="70" t="inlineStr">
+      <c r="L2" s="69" t="inlineStr">
         <is>
           <t>2020-12-10 00:00:00.000</t>
         </is>
       </c>
-      <c r="M2" s="66" t="n">
+      <c r="M2" s="65" t="n">
         <v>5</v>
       </c>
-      <c r="N2" s="66" t="inlineStr">
+      <c r="N2" s="65" t="inlineStr">
         <is>
           <t>Upfront Fee From Borrower/Agent/Third Party Intent Notice</t>
         </is>
       </c>
-      <c r="O2" s="67" t="inlineStr">
+      <c r="O2" s="66" t="inlineStr">
         <is>
           <t>Notice Identifier</t>
         </is>
       </c>
-      <c r="P2" s="67" t="inlineStr">
+      <c r="P2" s="66" t="inlineStr">
         <is>
           <t>CBA Email with PDF Attachment</t>
         </is>
       </c>
-      <c r="Q2" s="70" t="inlineStr">
+      <c r="Q2" s="69" t="inlineStr">
         <is>
           <t>2020-12-15 18:00:33.362</t>
         </is>
       </c>
-      <c r="R2" s="70" t="inlineStr">
+      <c r="R2" s="69" t="inlineStr">
         <is>
           <t>2020-12-15 18:00:33.362</t>
         </is>
       </c>
-      <c r="S2" s="67" t="inlineStr">
+      <c r="S2" s="66" t="inlineStr">
         <is>
           <t>Legal Name</t>
         </is>
       </c>
-      <c r="T2" s="67" t="inlineStr">
+      <c r="T2" s="66" t="inlineStr">
         <is>
           <t>C:\Users\u720589\AppData\Local\Temp\</t>
         </is>
       </c>
-      <c r="U2" s="67" t="inlineStr">
+      <c r="U2" s="66" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
         </is>
       </c>
-      <c r="V2" s="67" t="inlineStr">
+      <c r="V2" s="66" t="inlineStr">
         <is>
           <t>API_COR_TC02</t>
         </is>
       </c>
-      <c r="W2" s="68" t="inlineStr">
+      <c r="W2" s="67" t="inlineStr">
         <is>
           <t>TEMP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="X2" s="68" t="inlineStr">
+      <c r="X2" s="67" t="inlineStr">
         <is>
           <t>INPUT_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Y2" s="68" t="inlineStr">
+      <c r="Y2" s="67" t="inlineStr">
         <is>
           <t>EXP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Z2" s="68" t="inlineStr">
+      <c r="Z2" s="67" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
         </is>
       </c>
-      <c r="AA2" s="68" t="inlineStr">
+      <c r="AA2" s="67" t="inlineStr">
         <is>
           <t>correlationId</t>
         </is>
       </c>
-      <c r="AB2" s="68" t="inlineStr">
+      <c r="AB2" s="67" t="inlineStr">
         <is>
           <t>API_COR_RESPONSE_TC2</t>
         </is>
       </c>
-      <c r="AC2" s="63" t="n"/>
-      <c r="AD2" s="68" t="inlineStr">
+      <c r="AC2" s="62" t="n"/>
+      <c r="AD2" s="67" t="inlineStr">
         <is>
           <t>SENT</t>
         </is>
       </c>
-      <c r="AE2" s="68" t="n"/>
-      <c r="AF2" s="69" t="n"/>
-      <c r="AG2" s="63" t="n"/>
-      <c r="AH2" s="67" t="inlineStr">
+      <c r="AE2" s="67" t="n"/>
+      <c r="AF2" s="68" t="n"/>
+      <c r="AG2" s="62" t="n"/>
+      <c r="AH2" s="66" t="inlineStr">
         <is>
           <t>Sent</t>
         </is>
       </c>
-      <c r="AI2" s="63" t="n"/>
-      <c r="AJ2" s="66" t="inlineStr">
+      <c r="AI2" s="62" t="n"/>
+      <c r="AJ2" s="65" t="inlineStr">
         <is>
           <t>FEE INVOICE</t>
         </is>
       </c>
-      <c r="AK2" s="63" t="n"/>
-      <c r="AL2" s="64" t="inlineStr">
+      <c r="AK2" s="62" t="n"/>
+      <c r="AL2" s="63" t="inlineStr">
         <is>
           <t>10.000000%</t>
         </is>
       </c>
-      <c r="AM2" s="64" t="inlineStr">
+      <c r="AM2" s="63" t="inlineStr">
         <is>
           <t>5.000000%</t>
         </is>
       </c>
-      <c r="AN2" s="64" t="inlineStr">
+      <c r="AN2" s="63" t="inlineStr">
         <is>
           <t>15.000000%</t>
         </is>
       </c>
-      <c r="AO2" s="64" t="inlineStr">
+      <c r="AO2" s="63" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AP2" s="63" t="n"/>
-      <c r="AQ2" s="63" t="n"/>
-      <c r="AR2" s="65" t="n"/>
-      <c r="AS2" s="64" t="inlineStr">
+      <c r="AP2" s="62" t="n"/>
+      <c r="AQ2" s="62" t="n"/>
+      <c r="AR2" s="64" t="n"/>
+      <c r="AS2" s="63" t="inlineStr">
         <is>
           <t>27-May-2020</t>
         </is>
       </c>
-      <c r="AT2" s="64" t="inlineStr">
+      <c r="AT2" s="63" t="inlineStr">
         <is>
           <t>28-Jun-2021</t>
         </is>
       </c>
-      <c r="AU2" s="64" t="inlineStr">
+      <c r="AU2" s="63" t="inlineStr">
         <is>
           <t>10,000.00</t>
         </is>
       </c>
-      <c r="AV2" s="64" t="inlineStr">
+      <c r="AV2" s="63" t="inlineStr">
         <is>
           <t>25-May-2020</t>
         </is>
       </c>
-      <c r="AW2" s="64" t="n"/>
-      <c r="AX2" s="64" t="n"/>
-      <c r="AY2" s="64" t="n"/>
-      <c r="AZ2" s="64" t="n"/>
-      <c r="BA2" s="64" t="n"/>
-      <c r="BB2" s="64" t="n"/>
-      <c r="BC2" s="64" t="n"/>
-      <c r="BD2" s="64" t="n"/>
-      <c r="BE2" s="64" t="n"/>
-      <c r="BF2" s="64" t="n"/>
-      <c r="BG2" s="64" t="n"/>
-      <c r="BH2" s="64" t="n"/>
-      <c r="BI2" s="64" t="n"/>
-      <c r="BJ2" s="62" t="inlineStr">
+      <c r="AW2" s="63" t="n"/>
+      <c r="AX2" s="63" t="n"/>
+      <c r="AY2" s="63" t="n"/>
+      <c r="AZ2" s="63" t="n"/>
+      <c r="BA2" s="63" t="n"/>
+      <c r="BB2" s="63" t="n"/>
+      <c r="BC2" s="63" t="n"/>
+      <c r="BD2" s="63" t="n"/>
+      <c r="BE2" s="63" t="n"/>
+      <c r="BF2" s="63" t="n"/>
+      <c r="BG2" s="63" t="n"/>
+      <c r="BH2" s="63" t="n"/>
+      <c r="BI2" s="63" t="n"/>
+      <c r="BJ2" s="61" t="inlineStr">
         <is>
           <t>27-Dec-2019</t>
         </is>
       </c>
-      <c r="BK2" s="62" t="inlineStr">
+      <c r="BK2" s="61" t="inlineStr">
         <is>
           <t>275,750.00</t>
         </is>
       </c>
-      <c r="BL2" s="62" t="inlineStr">
+      <c r="BL2" s="61" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="BM2" s="62" t="inlineStr">
+      <c r="BM2" s="61" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BN2" s="62" t="inlineStr">
+      <c r="BN2" s="61" t="inlineStr">
         <is>
           <t>Establishment/Extension Fee</t>
         </is>
       </c>
-      <c r="BO2" s="62" t="inlineStr">
+      <c r="BO2" s="61" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="53" t="inlineStr">
+      <c r="C3" s="52" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="D3" s="59" t="n"/>
-      <c r="G3" s="57" t="n"/>
-      <c r="H3" s="57" t="n"/>
-      <c r="I3" s="59" t="n"/>
-      <c r="J3" s="57" t="n"/>
-      <c r="K3" s="59" t="n"/>
-      <c r="L3" s="59" t="n"/>
-      <c r="M3" s="59" t="n"/>
-      <c r="N3" s="59" t="n"/>
-      <c r="O3" s="59" t="n"/>
-      <c r="P3" s="59" t="n"/>
-      <c r="Q3" s="59" t="n"/>
-      <c r="R3" s="59" t="n"/>
-      <c r="S3" s="57" t="n"/>
-      <c r="T3" s="57" t="n"/>
-      <c r="U3" s="57" t="n"/>
-      <c r="V3" s="57" t="n"/>
-      <c r="AH3" s="57" t="n"/>
-      <c r="AJ3" s="57" t="n"/>
-      <c r="BJ3" s="57" t="n"/>
-      <c r="BK3" s="57" t="n"/>
-      <c r="BL3" s="57" t="n"/>
-      <c r="BM3" s="57" t="n"/>
-      <c r="BN3" s="57" t="n"/>
-      <c r="BO3" s="57" t="n"/>
+      <c r="D3" s="58" t="n"/>
+      <c r="G3" s="56" t="n"/>
+      <c r="H3" s="56" t="n"/>
+      <c r="I3" s="58" t="n"/>
+      <c r="J3" s="56" t="n"/>
+      <c r="K3" s="58" t="n"/>
+      <c r="L3" s="58" t="n"/>
+      <c r="M3" s="58" t="n"/>
+      <c r="N3" s="58" t="n"/>
+      <c r="O3" s="58" t="n"/>
+      <c r="P3" s="58" t="n"/>
+      <c r="Q3" s="58" t="n"/>
+      <c r="R3" s="58" t="n"/>
+      <c r="S3" s="56" t="n"/>
+      <c r="T3" s="56" t="n"/>
+      <c r="U3" s="56" t="n"/>
+      <c r="V3" s="56" t="n"/>
+      <c r="AH3" s="56" t="n"/>
+      <c r="AJ3" s="56" t="n"/>
+      <c r="BJ3" s="56" t="n"/>
+      <c r="BK3" s="56" t="n"/>
+      <c r="BL3" s="56" t="n"/>
+      <c r="BM3" s="56" t="n"/>
+      <c r="BN3" s="56" t="n"/>
+      <c r="BO3" s="56" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2241,41 +2240,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="77" min="1" max="1"/>
-    <col width="51.28515625" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="11" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="77" min="6" max="6"/>
-    <col width="23.5703125" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="25.28515625" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="23.85546875" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="21" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
-    <col width="37.7109375" bestFit="1" customWidth="1" style="77" min="15" max="15"/>
-    <col width="23.85546875" bestFit="1" customWidth="1" style="77" min="16" max="16"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="77" min="17" max="17"/>
-    <col width="26" bestFit="1" customWidth="1" style="77" min="18" max="18"/>
-    <col width="26.7109375" bestFit="1" customWidth="1" style="77" min="19" max="19"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="77" min="20" max="20"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="77" min="21" max="21"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="77" min="22" max="22"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="77" min="23" max="23"/>
-    <col width="19.85546875" bestFit="1" customWidth="1" style="77" min="24" max="24"/>
-    <col width="31.28515625" bestFit="1" customWidth="1" style="77" min="25" max="25"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="77" min="26" max="26"/>
-    <col width="29.140625" bestFit="1" customWidth="1" style="77" min="27" max="27"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
+    <col width="51.28515625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="11" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="25.28515625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="21" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="37.7109375" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
+    <col width="26" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="76" min="20" max="20"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="76" min="21" max="21"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="76" min="22" max="22"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="23" max="23"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="76" min="24" max="24"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" style="76" min="25" max="25"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="26" max="26"/>
+    <col width="29.140625" bestFit="1" customWidth="1" style="76" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2294,122 +2293,122 @@
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="D1" s="71" t="inlineStr">
+      <c r="D1" s="70" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="E1" s="71" t="inlineStr">
+      <c r="E1" s="70" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="F1" s="71" t="inlineStr">
+      <c r="F1" s="70" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="G1" s="71" t="inlineStr">
+      <c r="G1" s="70" t="inlineStr">
         <is>
           <t>Loan_RequestedAmount</t>
         </is>
       </c>
-      <c r="H1" s="71" t="inlineStr">
+      <c r="H1" s="70" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="I1" s="71" t="inlineStr">
+      <c r="I1" s="70" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="J1" s="71" t="inlineStr">
+      <c r="J1" s="70" t="inlineStr">
         <is>
           <t>Loan_RepricingFrequency</t>
         </is>
       </c>
-      <c r="K1" s="71" t="inlineStr">
+      <c r="K1" s="70" t="inlineStr">
         <is>
           <t>Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="L1" s="71" t="inlineStr">
+      <c r="L1" s="70" t="inlineStr">
         <is>
           <t>Loan_Accrue</t>
         </is>
       </c>
-      <c r="M1" s="71" t="inlineStr">
+      <c r="M1" s="70" t="inlineStr">
         <is>
           <t>Loan_RepricingDate</t>
         </is>
       </c>
-      <c r="N1" s="71" t="inlineStr">
+      <c r="N1" s="70" t="inlineStr">
         <is>
           <t>Notice_Subject</t>
         </is>
       </c>
-      <c r="O1" s="71" t="inlineStr">
+      <c r="O1" s="70" t="inlineStr">
         <is>
           <t>Notice_Comment</t>
         </is>
       </c>
-      <c r="P1" s="71" t="inlineStr">
+      <c r="P1" s="70" t="inlineStr">
         <is>
           <t>AcceptRate_FromPricing</t>
         </is>
       </c>
-      <c r="Q1" s="71" t="inlineStr">
+      <c r="Q1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalOriginal</t>
         </is>
       </c>
-      <c r="R1" s="71" t="inlineStr">
+      <c r="R1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalCurrent</t>
         </is>
       </c>
-      <c r="S1" s="71" t="inlineStr">
+      <c r="S1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankGross</t>
         </is>
       </c>
-      <c r="T1" s="71" t="inlineStr">
+      <c r="T1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankNet</t>
         </is>
       </c>
-      <c r="U1" s="71" t="inlineStr">
+      <c r="U1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanCurrentBaseRate</t>
         </is>
       </c>
-      <c r="V1" s="71" t="inlineStr">
+      <c r="V1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanSpread</t>
         </is>
       </c>
-      <c r="W1" s="71" t="inlineStr">
+      <c r="W1" s="70" t="inlineStr">
         <is>
           <t>Expctd_LoanAllInRate</t>
         </is>
       </c>
-      <c r="X1" s="71" t="inlineStr">
+      <c r="X1" s="70" t="inlineStr">
         <is>
           <t>Loan_PaymentMode</t>
         </is>
       </c>
-      <c r="Y1" s="71" t="inlineStr">
+      <c r="Y1" s="70" t="inlineStr">
         <is>
           <t>Expctd_Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="Z1" s="71" t="inlineStr">
+      <c r="Z1" s="70" t="inlineStr">
         <is>
           <t>BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="AA1" s="71" t="inlineStr">
+      <c r="AA1" s="70" t="inlineStr">
         <is>
           <t>AcceptRate_FromInterpolation</t>
         </is>
@@ -2546,7 +2545,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="AA2" s="76" t="n"/>
+      <c r="AA2" s="75" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="37" t="inlineStr">
@@ -2614,9 +2613,9 @@
           <t>16-Mar-2020</t>
         </is>
       </c>
-      <c r="N3" s="76" t="n"/>
-      <c r="O3" s="76" t="n"/>
-      <c r="P3" s="76" t="n"/>
+      <c r="N3" s="75" t="n"/>
+      <c r="O3" s="75" t="n"/>
+      <c r="P3" s="75" t="n"/>
       <c r="Q3" s="37" t="inlineStr">
         <is>
           <t>36,500,000.00</t>
@@ -2673,7 +2672,7 @@
         </is>
       </c>
     </row>
-    <row r="4" s="77">
+    <row r="4">
       <c r="A4" s="37" t="inlineStr">
         <is>
           <t>3</t>
@@ -2739,8 +2738,8 @@
           <t>03-Jan-2020</t>
         </is>
       </c>
-      <c r="N4" s="76" t="n"/>
-      <c r="O4" s="76" t="n"/>
+      <c r="N4" s="75" t="n"/>
+      <c r="O4" s="75" t="n"/>
       <c r="P4" t="inlineStr">
         <is>
           <t>Y</t>
@@ -2796,7 +2795,132 @@
           <t>None</t>
         </is>
       </c>
-      <c r="AA4" s="76" t="n"/>
+      <c r="AA4" s="75" t="n"/>
+    </row>
+    <row r="5" s="76">
+      <c r="A5" s="37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" s="35" t="inlineStr">
+        <is>
+          <t>Create Drawdown for Capitalization Facility - Outstanding B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>60002074</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="G5" s="37" t="inlineStr">
+        <is>
+          <t>2,900,000.00</t>
+        </is>
+      </c>
+      <c r="H5" s="37" t="inlineStr">
+        <is>
+          <t>18-Dec-2019</t>
+        </is>
+      </c>
+      <c r="I5" s="37" t="inlineStr">
+        <is>
+          <t>29-Aug-2023</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>to the adjusted due date</t>
+        </is>
+      </c>
+      <c r="M5" s="37" t="inlineStr">
+        <is>
+          <t>03-Jan-2020</t>
+        </is>
+      </c>
+      <c r="N5" s="75" t="n"/>
+      <c r="O5" s="75" t="n"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="Q5" s="37" t="inlineStr">
+        <is>
+          <t>2,900,000.00</t>
+        </is>
+      </c>
+      <c r="R5" s="37" t="inlineStr">
+        <is>
+          <t>2,900,000.00</t>
+        </is>
+      </c>
+      <c r="S5" s="37" t="inlineStr">
+        <is>
+          <t>2,900,000.00</t>
+        </is>
+      </c>
+      <c r="T5" s="37" t="inlineStr">
+        <is>
+          <t>2,900,000.00</t>
+        </is>
+      </c>
+      <c r="U5" s="37" t="inlineStr">
+        <is>
+          <t>0.842300%</t>
+        </is>
+      </c>
+      <c r="V5" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="W5" s="37" t="inlineStr">
+        <is>
+          <t>1.567300%</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AA5" s="75" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2819,37 +2943,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="75" min="1" max="1"/>
-    <col width="29.42578125" bestFit="1" customWidth="1" style="75" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="75" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="75" min="4" max="4"/>
-    <col width="20.5703125" customWidth="1" style="75" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="75" min="6" max="20"/>
-    <col width="8.7109375" customWidth="1" style="75" min="21" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="29.42578125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="29.42578125" customWidth="1" style="74" min="3" max="3"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="20.5703125" customWidth="1" style="74" min="5" max="5"/>
+    <col width="8.7109375" customWidth="1" style="74" min="6" max="21"/>
+    <col width="8.7109375" customWidth="1" style="74" min="22" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="74">
-      <c r="A1" s="73" t="inlineStr">
+    <row r="1" customFormat="1" s="73">
+      <c r="A1" s="72" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="73" t="inlineStr">
+      <c r="B1" s="72" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="73" t="inlineStr">
+      <c r="C1" s="72" t="inlineStr">
         <is>
           <t>AdjustmentSelection</t>
         </is>
       </c>
-      <c r="D1" s="74" t="inlineStr">
+      <c r="D1" s="73" t="inlineStr">
         <is>
           <t>GL_ShortName</t>
         </is>
       </c>
-      <c r="E1" s="74" t="inlineStr">
+      <c r="E1" s="73" t="inlineStr">
         <is>
           <t>GL_Offset_Type</t>
         </is>
@@ -2871,12 +2995,12 @@
           <t>Portfolio Settled Discount Change</t>
         </is>
       </c>
-      <c r="D2" s="75" t="inlineStr">
+      <c r="D2" s="74" t="inlineStr">
         <is>
           <t>Fees Held Awaiting Dispos.</t>
         </is>
       </c>
-      <c r="E2" s="75" t="inlineStr">
+      <c r="E2" s="74" t="inlineStr">
         <is>
           <t>Existing WIP</t>
         </is>
@@ -2954,8 +3078,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="57"/>
-    <col width="9.140625" customWidth="1" style="31" min="58" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="58"/>
+    <col width="9.140625" customWidth="1" style="31" min="59" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">
@@ -3407,18 +3531,18 @@
           <t>30-Jun-2019</t>
         </is>
       </c>
-      <c r="AS2" s="47" t="inlineStr">
+      <c r="AS2" s="46" t="inlineStr">
         <is>
           <t>02-Apr-2007</t>
         </is>
       </c>
-      <c r="AT2" s="47" t="inlineStr">
+      <c r="AT2" s="46" t="inlineStr">
         <is>
           <t>02-Apr-2007</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1" s="77">
+    <row r="3" ht="30" customHeight="1" s="76">
       <c r="C3" s="29" t="n"/>
       <c r="D3" s="29" t="n"/>
       <c r="E3" s="29" t="n"/>
@@ -3490,25 +3614,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="77" min="1" max="1"/>
-    <col width="38.140625" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="27" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="6" max="6"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="23.140625" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="20.7109375" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="18" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="77" min="15" max="15"/>
-    <col width="32" bestFit="1" customWidth="1" style="77" min="16" max="16"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" style="77" min="17" max="17"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" style="77" min="18" max="18"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="19" max="19"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="27" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="18" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
+    <col width="32" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
+    <col width="24.42578125" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3729,23 +3853,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="77" min="1" max="1"/>
-    <col width="27.5703125" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" style="77" min="6" max="7"/>
-    <col width="15.7109375" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="19.140625" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="77" min="15" max="15"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="77" min="16" max="16"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="77" min="17" max="17"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="77" min="18" max="18"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="76" min="6" max="7"/>
+    <col width="15.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="19.140625" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3956,25 +4080,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="77" min="1" max="1"/>
-    <col width="38.140625" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="32.42578125" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="27" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="6" max="6"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="23.140625" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="20.7109375" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="18" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="77" min="15" max="15"/>
-    <col width="32" bestFit="1" customWidth="1" style="77" min="16" max="16"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" style="77" min="17" max="17"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" style="77" min="18" max="18"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="19" max="19"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="27" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="18" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
+    <col width="32" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
+    <col width="24.42578125" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4195,60 +4319,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="77" min="1" max="1"/>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" style="77" min="6" max="6"/>
-    <col width="22" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
-    <col width="27.42578125" bestFit="1" customWidth="1" style="77" min="15" max="15"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="77" min="16" max="16"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="77" min="17" max="17"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="77" min="18" max="18"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="77" min="19" max="19"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="77" min="20" max="20"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="77" min="21" max="21"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="77" min="22" max="22"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="77" min="23" max="23"/>
-    <col width="27.42578125" bestFit="1" customWidth="1" style="77" min="24" max="24"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="77" min="25" max="25"/>
-    <col width="16.7109375" bestFit="1" customWidth="1" style="77" min="26" max="26"/>
-    <col width="22.5703125" bestFit="1" customWidth="1" style="77" min="27" max="27"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="77" min="28" max="28"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="77" min="29" max="29"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="77" min="30" max="30"/>
-    <col width="38.5703125" bestFit="1" customWidth="1" style="77" min="31" max="31"/>
-    <col width="39.140625" bestFit="1" customWidth="1" style="77" min="32" max="32"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="77" min="33" max="33"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="77" min="34" max="34"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="77" min="35" max="35"/>
-    <col width="18.85546875" bestFit="1" customWidth="1" style="77" min="36" max="36"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="37" max="37"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="38" max="38"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="77" min="39" max="39"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="77" min="40" max="40"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="77" min="41" max="41"/>
-    <col width="38.5703125" bestFit="1" customWidth="1" style="77" min="42" max="42"/>
-    <col width="39.140625" bestFit="1" customWidth="1" style="77" min="43" max="43"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="77" min="44" max="44"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="77" min="45" max="45"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="77" min="46" max="46"/>
-    <col width="18.85546875" bestFit="1" customWidth="1" style="77" min="47" max="47"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="77" min="48" max="48"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="77" min="49" max="49"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="77" min="50" max="50"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="77" min="51" max="51"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="77" min="52" max="52"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="77" min="53" max="53"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="77" min="54" max="54"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
+    <col width="22" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="31.140625" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="76" min="20" max="20"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="76" min="21" max="21"/>
+    <col width="31.140625" bestFit="1" customWidth="1" style="76" min="22" max="22"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="23" max="23"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="76" min="24" max="24"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="76" min="25" max="25"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" style="76" min="26" max="26"/>
+    <col width="22.5703125" bestFit="1" customWidth="1" style="76" min="27" max="27"/>
+    <col width="39.85546875" bestFit="1" customWidth="1" style="76" min="28" max="28"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="29" max="29"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="30" max="30"/>
+    <col width="38.5703125" bestFit="1" customWidth="1" style="76" min="31" max="31"/>
+    <col width="39.140625" bestFit="1" customWidth="1" style="76" min="32" max="32"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="33" max="33"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="34" max="34"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="35" max="35"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="76" min="36" max="36"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="37" max="37"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="38" max="38"/>
+    <col width="39.85546875" bestFit="1" customWidth="1" style="76" min="39" max="39"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="40" max="40"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="41" max="41"/>
+    <col width="38.5703125" bestFit="1" customWidth="1" style="76" min="42" max="42"/>
+    <col width="39.140625" bestFit="1" customWidth="1" style="76" min="43" max="43"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="44" max="44"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="45" max="45"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="46" max="46"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="76" min="47" max="47"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="48" max="48"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="49" max="49"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="50" max="50"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="76" min="51" max="51"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="52" max="52"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="53" max="53"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="54" max="54"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4801,19 +4925,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="26.28515625" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="18.42578125" customWidth="1" style="77" min="6" max="6"/>
-    <col width="27.28515625" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="20" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="26.28515625" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="34.85546875" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="22" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="18.42578125" customWidth="1" style="76" min="6" max="6"/>
+    <col width="27.28515625" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="20" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="34.85546875" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="22" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4980,9 +5104,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="38.140625" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="32.140625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5048,19 +5172,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="38.140625" bestFit="1" customWidth="1" style="77" min="2" max="2"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" style="77" min="3" max="3"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="77" min="4" max="4"/>
-    <col width="26" bestFit="1" customWidth="1" style="77" min="5" max="5"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="77" min="6" max="6"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="77" min="7" max="7"/>
-    <col width="21" bestFit="1" customWidth="1" style="77" min="8" max="8"/>
-    <col width="49.42578125" bestFit="1" customWidth="1" style="77" min="9" max="9"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="77" min="10" max="10"/>
-    <col width="24" bestFit="1" customWidth="1" style="77" min="11" max="11"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="77" min="12" max="12"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="77" min="13" max="13"/>
-    <col width="24" bestFit="1" customWidth="1" style="77" min="14" max="14"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
+    <col width="32.140625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="26" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
+    <col width="21" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
+    <col width="49.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
+    <col width="24" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
+    <col width="24" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5208,7 +5332,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="72" t="inlineStr">
+      <c r="D3" s="71" t="inlineStr">
         <is>
           <t>Should be 27-Dec-2019</t>
         </is>

</xml_diff>

<commit_message>
GDE-9406 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A06E0BB-B141-4BFF-B5EA-674C51EB61E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55572205-DAC5-42A7-AF7F-F4D3F70C892F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="SERV01_LoanDrawdown" sheetId="11" r:id="rId11"/>
     <sheet name="TRPO12_PortfolioSettledDisc" sheetId="12" r:id="rId12"/>
     <sheet name="AMCH04_DealChangeTransaction" sheetId="13" r:id="rId13"/>
+    <sheet name="SERV29_PaymentFees" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="537">
   <si>
     <t>rowid</t>
   </si>
@@ -1619,6 +1620,30 @@
   </si>
   <si>
     <t>0.355</t>
+  </si>
+  <si>
+    <t>Collect line fee in arrears</t>
+  </si>
+  <si>
+    <t>Cycle_Number</t>
+  </si>
+  <si>
+    <t>Expected_CycleDueAmt</t>
+  </si>
+  <si>
+    <t>204,668.49</t>
+  </si>
+  <si>
+    <t>Cycle_StartDate</t>
+  </si>
+  <si>
+    <t>Cycle_EndDate</t>
+  </si>
+  <si>
+    <t>Cycle_DueDate</t>
+  </si>
+  <si>
+    <t>ProjectedCycleDue</t>
   </si>
 </sst>
 </file>
@@ -3845,7 +3870,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3909,6 +3934,107 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE15980-6AE5-4307-A6B8-E504D31085CE}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="74" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="74" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="24.28515625" style="74" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" style="74" customWidth="1"/>
+    <col min="11" max="11" width="24" style="74" bestFit="1" customWidth="1"/>
+    <col min="12" max="27" width="8.7109375" style="74" customWidth="1"/>
+    <col min="28" max="16384" width="8.7109375" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>530</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>533</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>534</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>535</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>536</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>420</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>529</v>
+      </c>
+      <c r="C2" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="77">
+        <v>1</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="77" t="s">
+        <v>251</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2" s="77" t="s">
+        <v>251</v>
+      </c>
+      <c r="J2" s="77" t="s">
+        <v>532</v>
+      </c>
+      <c r="K2" s="77"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>

</xml_diff>

<commit_message>
GDE-9407 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55572205-DAC5-42A7-AF7F-F4D3F70C892F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2494A22C-D08A-4D89-AD2D-8ED8D7E9A858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,14 @@
     <sheet name="SERV01_LoanDrawdown" sheetId="11" r:id="rId11"/>
     <sheet name="TRPO12_PortfolioSettledDisc" sheetId="12" r:id="rId12"/>
     <sheet name="AMCH04_DealChangeTransaction" sheetId="13" r:id="rId13"/>
-    <sheet name="SERV29_PaymentFees" sheetId="15" r:id="rId14"/>
+    <sheet name="SERV29_PaymentFees" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="544">
   <si>
     <t>rowid</t>
   </si>
@@ -1412,6 +1412,30 @@
     <t>27-Dec-2019</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Ongoing Fee Payment Intent Notice</t>
+  </si>
+  <si>
+    <t>9HEMMY3A</t>
+  </si>
+  <si>
+    <t>LIQ-9HEMMY3A-9HEMMY1R-2</t>
+  </si>
+  <si>
+    <t>2021-01-23 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-01-03 00:00:00.000</t>
+  </si>
+  <si>
+    <t>Fee Payment Notice</t>
+  </si>
+  <si>
+    <t>2021-01-13 18:45:16.775</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
@@ -1508,9 +1532,6 @@
     <t>Quarterly</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Create Drawdown for Capitalization Facility - Outstanding Z</t>
   </si>
   <si>
@@ -1601,49 +1622,49 @@
     <t>Deal_RatioType</t>
   </si>
   <si>
+    <t>NewFinancial_Ratio</t>
+  </si>
+  <si>
+    <t>DealEventStatus1</t>
+  </si>
+  <si>
+    <t>DealEventStatus2</t>
+  </si>
+  <si>
     <t>Update LVR for CH EDU Bilateral Deal</t>
   </si>
   <si>
-    <t>NewFinancial_Ratio</t>
+    <t>0.355</t>
+  </si>
+  <si>
+    <t>Deal Change Transaction Released</t>
   </si>
   <si>
     <t>Financial Ratio Changed</t>
   </si>
   <si>
-    <t>DealEventStatus1</t>
-  </si>
-  <si>
-    <t>DealEventStatus2</t>
-  </si>
-  <si>
-    <t>Deal Change Transaction Released</t>
-  </si>
-  <si>
-    <t>0.355</t>
+    <t>Cycle_Number</t>
+  </si>
+  <si>
+    <t>Cycle_StartDate</t>
+  </si>
+  <si>
+    <t>Cycle_EndDate</t>
+  </si>
+  <si>
+    <t>Cycle_DueDate</t>
+  </si>
+  <si>
+    <t>ProjectedCycleDue</t>
+  </si>
+  <si>
+    <t>Expected_CycleDueAmt</t>
   </si>
   <si>
     <t>Collect line fee in arrears</t>
   </si>
   <si>
-    <t>Cycle_Number</t>
-  </si>
-  <si>
-    <t>Expected_CycleDueAmt</t>
-  </si>
-  <si>
     <t>204,668.49</t>
-  </si>
-  <si>
-    <t>Cycle_StartDate</t>
-  </si>
-  <si>
-    <t>Cycle_EndDate</t>
-  </si>
-  <si>
-    <t>Cycle_DueDate</t>
-  </si>
-  <si>
-    <t>ProjectedCycleDue</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1889,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1967,6 +1988,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -2879,17 +2901,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO3"/>
+  <dimension ref="A1:BO4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M15" sqref="M15"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="54" customWidth="1"/>
-    <col min="2" max="2" width="22" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="52" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" style="52" bestFit="1" customWidth="1"/>
@@ -2953,8 +2975,8 @@
     <col min="65" max="65" width="9.7109375" style="52" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="26" style="52" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="17.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="68" max="128" width="9.140625" style="52" customWidth="1"/>
-    <col min="129" max="16384" width="9.140625" style="52"/>
+    <col min="68" max="129" width="9.140625" style="52" customWidth="1"/>
+    <col min="130" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3319,35 +3341,194 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="C3" s="52" t="s">
+    <row r="3" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="78" t="s">
         <v>459</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="AH3" s="56"/>
-      <c r="AJ3" s="56"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="56"/>
-      <c r="BO3" s="56"/>
+      <c r="B3" s="53" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>425</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>426</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>428</v>
+      </c>
+      <c r="H3" s="65" t="s">
+        <v>429</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>461</v>
+      </c>
+      <c r="J3" s="69" t="s">
+        <v>462</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>463</v>
+      </c>
+      <c r="L3" s="69" t="s">
+        <v>464</v>
+      </c>
+      <c r="M3" s="65">
+        <v>5</v>
+      </c>
+      <c r="N3" s="65" t="s">
+        <v>465</v>
+      </c>
+      <c r="O3" s="66" t="s">
+        <v>435</v>
+      </c>
+      <c r="P3" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" s="69" t="s">
+        <v>466</v>
+      </c>
+      <c r="R3" s="69" t="s">
+        <v>466</v>
+      </c>
+      <c r="S3" s="66" t="s">
+        <v>437</v>
+      </c>
+      <c r="T3" s="66" t="s">
+        <v>438</v>
+      </c>
+      <c r="U3" s="66" t="s">
+        <v>439</v>
+      </c>
+      <c r="V3" s="66" t="s">
+        <v>440</v>
+      </c>
+      <c r="W3" s="67" t="s">
+        <v>441</v>
+      </c>
+      <c r="X3" s="67" t="s">
+        <v>442</v>
+      </c>
+      <c r="Y3" s="67" t="s">
+        <v>443</v>
+      </c>
+      <c r="Z3" s="67" t="s">
+        <v>444</v>
+      </c>
+      <c r="AA3" s="67" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB3" s="67" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="67" t="s">
+        <v>447</v>
+      </c>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="62"/>
+      <c r="AH3" s="66" t="s">
+        <v>448</v>
+      </c>
+      <c r="AI3" s="62"/>
+      <c r="AJ3" s="65" t="s">
+        <v>449</v>
+      </c>
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="63" t="s">
+        <v>450</v>
+      </c>
+      <c r="AM3" s="63" t="s">
+        <v>451</v>
+      </c>
+      <c r="AN3" s="63" t="s">
+        <v>452</v>
+      </c>
+      <c r="AO3" s="63" t="s">
+        <v>453</v>
+      </c>
+      <c r="AP3" s="62"/>
+      <c r="AQ3" s="62"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="63" t="s">
+        <v>454</v>
+      </c>
+      <c r="AT3" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="AU3" s="63" t="s">
+        <v>456</v>
+      </c>
+      <c r="AV3" s="63" t="s">
+        <v>457</v>
+      </c>
+      <c r="AW3" s="63"/>
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="63"/>
+      <c r="AZ3" s="63"/>
+      <c r="BA3" s="63"/>
+      <c r="BB3" s="63"/>
+      <c r="BC3" s="63"/>
+      <c r="BD3" s="63"/>
+      <c r="BE3" s="63"/>
+      <c r="BF3" s="63"/>
+      <c r="BG3" s="63"/>
+      <c r="BH3" s="63"/>
+      <c r="BI3" s="63"/>
+      <c r="BJ3" s="75" t="s">
+        <v>458</v>
+      </c>
+      <c r="BK3" s="75" t="s">
+        <v>353</v>
+      </c>
+      <c r="BL3" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM3" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="BN3" s="75" t="s">
+        <v>355</v>
+      </c>
+      <c r="BO3" s="61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="C4" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="D4" s="58"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="AH4" s="56"/>
+      <c r="AJ4" s="56"/>
+      <c r="BJ4" s="56"/>
+      <c r="BK4" s="56"/>
+      <c r="BL4" s="56"/>
+      <c r="BM4" s="56"/>
+      <c r="BN4" s="56"/>
+      <c r="BO4" s="56"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -3406,16 +3587,16 @@
         <v>365</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="E1" s="70" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="G1" s="70" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="H1" s="70" t="s">
         <v>403</v>
@@ -3424,13 +3605,13 @@
         <v>404</v>
       </c>
       <c r="J1" s="70" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K1" s="70" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="L1" s="70" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="M1" s="70" t="s">
         <v>407</v>
@@ -3442,40 +3623,40 @@
         <v>346</v>
       </c>
       <c r="P1" s="70" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="Q1" s="70" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="R1" s="70" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="S1" s="70" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="T1" s="70" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="U1" s="70" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="V1" s="70" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="W1" s="70" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="X1" s="70" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="Y1" s="70" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="Z1" s="70" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="AA1" s="70" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -3483,10 +3664,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="D2" t="s">
         <v>221</v>
@@ -3507,25 +3688,25 @@
         <v>220</v>
       </c>
       <c r="J2" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="K2" t="s">
         <v>105</v>
       </c>
       <c r="L2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="N2" t="s">
         <v>357</v>
       </c>
       <c r="O2" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="P2" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="Q2" s="37" t="s">
         <v>353</v>
@@ -3540,19 +3721,19 @@
         <v>353</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="V2" s="37" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="X2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="Y2" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="Z2" t="s">
         <v>105</v>
@@ -3561,13 +3742,13 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>491</v>
+        <v>459</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="C3" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="D3" t="s">
         <v>221</v>
@@ -3579,72 +3760,72 @@
         <v>113</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="I3" s="37" t="s">
         <v>220</v>
       </c>
       <c r="J3" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="K3" t="s">
         <v>105</v>
       </c>
       <c r="L3" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="N3" s="75"/>
       <c r="O3" s="75"/>
       <c r="P3" s="75"/>
       <c r="Q3" s="37" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="R3" s="37" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="T3" s="37" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="U3" s="37" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="V3" s="37" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="W3" s="37" t="s">
+        <v>504</v>
+      </c>
+      <c r="X3" t="s">
         <v>497</v>
       </c>
-      <c r="X3" t="s">
-        <v>489</v>
-      </c>
       <c r="Y3" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="Z3" t="s">
         <v>105</v>
       </c>
       <c r="AA3" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="C4" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="D4" t="s">
         <v>221</v>
@@ -3656,57 +3837,57 @@
         <v>113</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="I4" s="37" t="s">
         <v>261</v>
       </c>
       <c r="J4" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="K4" t="s">
         <v>105</v>
       </c>
       <c r="L4" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="N4" s="75"/>
       <c r="O4" s="75"/>
       <c r="P4" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="Q4" s="37" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="R4" s="37" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="S4" s="37" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="V4" s="37" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="W4" s="37" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="X4" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="Y4" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="Z4" t="s">
         <v>105</v>
@@ -3715,13 +3896,13 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C5" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="D5" t="s">
         <v>221</v>
@@ -3733,57 +3914,57 @@
         <v>113</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>261</v>
       </c>
       <c r="J5" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="K5" t="s">
         <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="N5" s="75"/>
       <c r="O5" s="75"/>
       <c r="P5" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="R5" s="37" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="S5" s="37" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="T5" s="37" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="U5" s="37" t="s">
+        <v>520</v>
+      </c>
+      <c r="V5" s="37" t="s">
         <v>513</v>
       </c>
-      <c r="V5" s="37" t="s">
-        <v>506</v>
-      </c>
       <c r="W5" s="37" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="X5" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="Y5" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="Z5" t="s">
         <v>105</v>
@@ -3814,8 +3995,8 @@
     <col min="3" max="3" width="29.42578125" style="74" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="74" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="74" customWidth="1"/>
-    <col min="6" max="22" width="8.7109375" style="74" customWidth="1"/>
-    <col min="23" max="16384" width="8.7109375" style="74"/>
+    <col min="6" max="23" width="8.7109375" style="74" customWidth="1"/>
+    <col min="24" max="16384" width="8.7109375" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -3826,13 +4007,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3840,16 +4021,16 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C2" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="E2" s="74" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3864,7 +4045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EA4661-728F-4481-A052-F31AE93E892B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
@@ -3883,8 +4064,8 @@
     <col min="5" max="5" width="30.140625" style="74" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" style="74" customWidth="1"/>
     <col min="7" max="7" width="24" style="74" bestFit="1" customWidth="1"/>
-    <col min="8" max="23" width="8.7109375" style="74" customWidth="1"/>
-    <col min="24" max="16384" width="8.7109375" style="74"/>
+    <col min="8" max="24" width="8.7109375" style="74" customWidth="1"/>
+    <col min="25" max="16384" width="8.7109375" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -3895,16 +4076,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="G1" s="73" t="s">
         <v>164</v>
@@ -3914,20 +4095,20 @@
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="76" t="s">
-        <v>522</v>
-      </c>
-      <c r="C2" s="76" t="s">
+      <c r="B2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="E2" s="74" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="F2" s="74" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="G2" s="77" t="s">
         <v>253</v>
@@ -3945,13 +4126,13 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE15980-6AE5-4307-A6B8-E504D31085CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -3965,8 +4146,8 @@
     <col min="9" max="9" width="30.140625" style="74" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.140625" style="74" customWidth="1"/>
     <col min="11" max="11" width="24" style="74" bestFit="1" customWidth="1"/>
-    <col min="12" max="27" width="8.7109375" style="74" customWidth="1"/>
-    <col min="28" max="16384" width="8.7109375" style="74"/>
+    <col min="12" max="28" width="8.7109375" style="74" customWidth="1"/>
+    <col min="29" max="16384" width="8.7109375" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -3980,35 +4161,35 @@
         <v>342</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="I1" s="73" t="s">
         <v>420</v>
       </c>
       <c r="J1" s="73" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="76" t="s">
-        <v>529</v>
-      </c>
-      <c r="C2" s="76" t="s">
+      <c r="B2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C2" t="s">
         <v>189</v>
       </c>
       <c r="D2" s="77">
@@ -4024,13 +4205,13 @@
         <v>251</v>
       </c>
       <c r="H2" s="77" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="I2" s="77" t="s">
         <v>251</v>
       </c>
       <c r="J2" s="77" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="K2" s="77"/>
     </row>
@@ -4104,8 +4285,8 @@
     <col min="44" max="44" width="24" style="31" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="47" max="59" width="9.140625" style="31" customWidth="1"/>
-    <col min="60" max="16384" width="9.140625" style="31"/>
+    <col min="47" max="60" width="9.140625" style="31" customWidth="1"/>
+    <col min="61" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
GDE-9410 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -322,9 +322,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -722,22 +720,22 @@
     <col width="33" bestFit="1" customWidth="1" style="9" min="54" max="54"/>
     <col width="24.85546875" customWidth="1" style="9" min="55" max="55"/>
     <col width="20" customWidth="1" style="9" min="56" max="56"/>
-    <col width="22.5703125" bestFit="1" customWidth="1" style="76" min="57" max="57"/>
-    <col width="16" bestFit="1" customWidth="1" style="76" min="58" max="58"/>
-    <col width="26" bestFit="1" customWidth="1" style="76" min="59" max="59"/>
-    <col width="26.42578125" bestFit="1" customWidth="1" style="76" min="60" max="60"/>
-    <col width="21.5703125" bestFit="1" customWidth="1" style="76" min="61" max="61"/>
-    <col width="19.140625" bestFit="1" customWidth="1" style="76" min="62" max="62"/>
-    <col width="32.5703125" bestFit="1" customWidth="1" style="76" min="63" max="63"/>
-    <col width="34.28515625" bestFit="1" customWidth="1" style="76" min="64" max="64"/>
-    <col width="31.7109375" bestFit="1" customWidth="1" style="76" min="65" max="65"/>
-    <col width="22" bestFit="1" customWidth="1" style="76" min="66" max="66"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="76" min="67" max="67"/>
-    <col width="18.140625" bestFit="1" customWidth="1" style="76" min="68" max="68"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="76" min="69" max="69"/>
-    <col width="25.85546875" bestFit="1" customWidth="1" style="76" min="70" max="70"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="71" max="71"/>
-    <col width="25.7109375" bestFit="1" customWidth="1" style="76" min="72" max="72"/>
+    <col width="22.5703125" bestFit="1" customWidth="1" style="74" min="57" max="57"/>
+    <col width="16" bestFit="1" customWidth="1" style="74" min="58" max="58"/>
+    <col width="26" bestFit="1" customWidth="1" style="74" min="59" max="59"/>
+    <col width="26.42578125" bestFit="1" customWidth="1" style="74" min="60" max="60"/>
+    <col width="21.5703125" bestFit="1" customWidth="1" style="74" min="61" max="61"/>
+    <col width="19.140625" bestFit="1" customWidth="1" style="74" min="62" max="62"/>
+    <col width="32.5703125" bestFit="1" customWidth="1" style="74" min="63" max="63"/>
+    <col width="34.28515625" bestFit="1" customWidth="1" style="74" min="64" max="64"/>
+    <col width="31.7109375" bestFit="1" customWidth="1" style="74" min="65" max="65"/>
+    <col width="22" bestFit="1" customWidth="1" style="74" min="66" max="66"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="74" min="67" max="67"/>
+    <col width="18.140625" bestFit="1" customWidth="1" style="74" min="68" max="68"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="74" min="69" max="69"/>
+    <col width="25.85546875" bestFit="1" customWidth="1" style="74" min="70" max="70"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="74" min="71" max="71"/>
+    <col width="25.7109375" bestFit="1" customWidth="1" style="74" min="72" max="72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="5">
@@ -1541,15 +1539,15 @@
   </sheetPr>
   <dimension ref="A1:BO4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6.5703125" customWidth="1" style="54" min="1" max="1"/>
-    <col width="31.28515625" bestFit="1" customWidth="1" style="54" min="2" max="2"/>
+    <col width="39.85546875" bestFit="1" customWidth="1" style="54" min="2" max="2"/>
     <col width="27.42578125" bestFit="1" customWidth="1" style="52" min="3" max="3"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="54" min="4" max="4"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="52" min="5" max="5"/>
@@ -1612,12 +1610,12 @@
     <col width="40.7109375" bestFit="1" customWidth="1" style="52" min="64" max="64"/>
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="133"/>
-    <col width="9.140625" customWidth="1" style="52" min="134" max="16384"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="135"/>
+    <col width="9.140625" customWidth="1" style="52" min="136" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.15" customHeight="1" s="76">
+    <row r="1" ht="13.15" customHeight="1" s="74">
       <c r="A1" s="47" t="inlineStr">
         <is>
           <t>rowid</t>
@@ -1633,7 +1631,7 @@
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="57" t="inlineStr">
+      <c r="D1" s="56" t="inlineStr">
         <is>
           <t>Notice_Customer_LegalName</t>
         </is>
@@ -1648,42 +1646,42 @@
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="G1" s="57" t="inlineStr">
+      <c r="G1" s="56" t="inlineStr">
         <is>
           <t>Contact</t>
         </is>
       </c>
-      <c r="H1" s="57" t="inlineStr">
+      <c r="H1" s="58" t="inlineStr">
         <is>
           <t>NoticeGroup_UserID</t>
         </is>
       </c>
-      <c r="I1" s="57" t="inlineStr">
+      <c r="I1" s="56" t="inlineStr">
         <is>
           <t>Notice_Identifier</t>
         </is>
       </c>
-      <c r="J1" s="57" t="inlineStr">
+      <c r="J1" s="56" t="inlineStr">
         <is>
           <t>Correlation_ID</t>
         </is>
       </c>
-      <c r="K1" s="59" t="inlineStr">
+      <c r="K1" s="57" t="inlineStr">
         <is>
           <t>Thru_Date</t>
         </is>
       </c>
-      <c r="L1" s="57" t="inlineStr">
+      <c r="L1" s="56" t="inlineStr">
         <is>
           <t>From_Date</t>
         </is>
       </c>
-      <c r="M1" s="60" t="inlineStr">
+      <c r="M1" s="58" t="inlineStr">
         <is>
           <t>SubAdd_Days</t>
         </is>
       </c>
-      <c r="N1" s="60" t="inlineStr">
+      <c r="N1" s="58" t="inlineStr">
         <is>
           <t>Notice_Type</t>
         </is>
@@ -1698,12 +1696,12 @@
           <t>Notice_Method</t>
         </is>
       </c>
-      <c r="Q1" s="57" t="inlineStr">
+      <c r="Q1" s="56" t="inlineStr">
         <is>
           <t>BEO_StartDate</t>
         </is>
       </c>
-      <c r="R1" s="57" t="inlineStr">
+      <c r="R1" s="56" t="inlineStr">
         <is>
           <t>BEO_EndDate</t>
         </is>
@@ -1923,38 +1921,38 @@
           <t>Interest_Amount</t>
         </is>
       </c>
-      <c r="BJ1" s="57" t="inlineStr">
+      <c r="BJ1" s="56" t="inlineStr">
         <is>
           <t>Effective_Date</t>
         </is>
       </c>
-      <c r="BK1" s="57" t="inlineStr">
+      <c r="BK1" s="56" t="inlineStr">
         <is>
           <t>UpfrontFee_Amount</t>
         </is>
       </c>
-      <c r="BL1" s="57" t="inlineStr">
+      <c r="BL1" s="56" t="inlineStr">
         <is>
           <t>Branch_Description</t>
         </is>
       </c>
-      <c r="BM1" s="57" t="inlineStr">
+      <c r="BM1" s="56" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="BN1" s="57" t="inlineStr">
+      <c r="BN1" s="56" t="inlineStr">
         <is>
           <t>Fee_Type</t>
         </is>
       </c>
-      <c r="BO1" s="57" t="inlineStr">
+      <c r="BO1" s="56" t="inlineStr">
         <is>
           <t>Account_Name</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="76">
+    <row r="2" ht="15" customHeight="1" s="74">
       <c r="A2" s="52" t="inlineStr">
         <is>
           <t>1</t>
@@ -1965,244 +1963,232 @@
           <t>Upfront Fee Intent Notice</t>
         </is>
       </c>
-      <c r="C2" s="63" t="inlineStr">
-        <is>
-          <t>CBANLD_03112020160326YZJ</t>
-        </is>
-      </c>
-      <c r="D2" s="69" t="inlineStr">
+      <c r="C2" s="61" t="n"/>
+      <c r="D2" s="67" t="inlineStr">
         <is>
           <t>CH EDU Limited 1710818</t>
         </is>
       </c>
-      <c r="E2" s="62" t="inlineStr">
-        <is>
-          <t>CBANLDNAFAC03112020161931</t>
-        </is>
-      </c>
-      <c r="F2" s="62" t="inlineStr">
-        <is>
-          <t>60000035</t>
-        </is>
-      </c>
-      <c r="G2" s="69" t="inlineStr">
+      <c r="E2" s="60" t="n"/>
+      <c r="F2" s="60" t="n"/>
+      <c r="G2" s="67" t="inlineStr">
         <is>
           <t>Linda Chu</t>
         </is>
       </c>
-      <c r="H2" s="65" t="inlineStr">
+      <c r="H2" s="63" t="inlineStr">
         <is>
           <t>LOANIQ01</t>
         </is>
       </c>
-      <c r="I2" s="69" t="inlineStr">
+      <c r="I2" s="67" t="inlineStr">
         <is>
           <t>@1EL8J83</t>
         </is>
       </c>
-      <c r="J2" s="69" t="inlineStr">
+      <c r="J2" s="67" t="inlineStr">
         <is>
           <t>LIQ-@1EL8J83-@1EL8J61-3</t>
         </is>
       </c>
-      <c r="K2" s="69" t="inlineStr">
+      <c r="K2" s="67" t="inlineStr">
         <is>
           <t>2020-12-20 00:00:00.000</t>
         </is>
       </c>
-      <c r="L2" s="69" t="inlineStr">
+      <c r="L2" s="67" t="inlineStr">
         <is>
           <t>2020-12-10 00:00:00.000</t>
         </is>
       </c>
-      <c r="M2" s="65" t="n">
+      <c r="M2" s="63" t="n">
         <v>5</v>
       </c>
-      <c r="N2" s="65" t="inlineStr">
+      <c r="N2" s="63" t="inlineStr">
         <is>
           <t>Upfront Fee From Borrower/Agent/Third Party Intent Notice</t>
         </is>
       </c>
-      <c r="O2" s="66" t="inlineStr">
+      <c r="O2" s="64" t="inlineStr">
         <is>
           <t>Notice Identifier</t>
         </is>
       </c>
-      <c r="P2" s="66" t="inlineStr">
+      <c r="P2" s="64" t="inlineStr">
         <is>
           <t>CBA Email with PDF Attachment</t>
         </is>
       </c>
-      <c r="Q2" s="69" t="inlineStr">
+      <c r="Q2" s="67" t="inlineStr">
         <is>
           <t>2020-12-15 18:00:33.362</t>
         </is>
       </c>
-      <c r="R2" s="69" t="inlineStr">
+      <c r="R2" s="67" t="inlineStr">
         <is>
           <t>2020-12-15 18:00:33.362</t>
         </is>
       </c>
-      <c r="S2" s="66" t="inlineStr">
+      <c r="S2" s="64" t="inlineStr">
         <is>
           <t>Legal Name</t>
         </is>
       </c>
-      <c r="T2" s="66" t="inlineStr">
+      <c r="T2" s="64" t="inlineStr">
         <is>
           <t>C:\Users\u720589\AppData\Local\Temp\</t>
         </is>
       </c>
-      <c r="U2" s="66" t="inlineStr">
+      <c r="U2" s="64" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
         </is>
       </c>
-      <c r="V2" s="66" t="inlineStr">
+      <c r="V2" s="64" t="inlineStr">
         <is>
           <t>API_COR_TC02</t>
         </is>
       </c>
-      <c r="W2" s="67" t="inlineStr">
+      <c r="W2" s="65" t="inlineStr">
         <is>
           <t>TEMP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="X2" s="67" t="inlineStr">
+      <c r="X2" s="65" t="inlineStr">
         <is>
           <t>INPUT_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Y2" s="67" t="inlineStr">
+      <c r="Y2" s="65" t="inlineStr">
         <is>
           <t>EXP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Z2" s="67" t="inlineStr">
+      <c r="Z2" s="65" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
         </is>
       </c>
-      <c r="AA2" s="67" t="inlineStr">
+      <c r="AA2" s="65" t="inlineStr">
         <is>
           <t>correlationId</t>
         </is>
       </c>
-      <c r="AB2" s="67" t="inlineStr">
+      <c r="AB2" s="65" t="inlineStr">
         <is>
           <t>API_COR_RESPONSE_TC2</t>
         </is>
       </c>
-      <c r="AC2" s="62" t="n"/>
-      <c r="AD2" s="67" t="inlineStr">
+      <c r="AC2" s="60" t="n"/>
+      <c r="AD2" s="65" t="inlineStr">
         <is>
           <t>SENT</t>
         </is>
       </c>
-      <c r="AE2" s="67" t="n"/>
-      <c r="AF2" s="68" t="n"/>
-      <c r="AG2" s="62" t="n"/>
-      <c r="AH2" s="66" t="inlineStr">
+      <c r="AE2" s="65" t="n"/>
+      <c r="AF2" s="66" t="n"/>
+      <c r="AG2" s="60" t="n"/>
+      <c r="AH2" s="64" t="inlineStr">
         <is>
           <t>Sent</t>
         </is>
       </c>
-      <c r="AI2" s="62" t="n"/>
-      <c r="AJ2" s="65" t="inlineStr">
+      <c r="AI2" s="60" t="n"/>
+      <c r="AJ2" s="63" t="inlineStr">
         <is>
           <t>FEE INVOICE</t>
         </is>
       </c>
-      <c r="AK2" s="62" t="n"/>
-      <c r="AL2" s="63" t="inlineStr">
+      <c r="AK2" s="60" t="n"/>
+      <c r="AL2" s="61" t="inlineStr">
         <is>
           <t>10.000000%</t>
         </is>
       </c>
-      <c r="AM2" s="63" t="inlineStr">
+      <c r="AM2" s="61" t="inlineStr">
         <is>
           <t>5.000000%</t>
         </is>
       </c>
-      <c r="AN2" s="63" t="inlineStr">
+      <c r="AN2" s="61" t="inlineStr">
         <is>
           <t>15.000000%</t>
         </is>
       </c>
-      <c r="AO2" s="63" t="inlineStr">
+      <c r="AO2" s="61" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AP2" s="62" t="n"/>
-      <c r="AQ2" s="62" t="n"/>
-      <c r="AR2" s="64" t="n"/>
-      <c r="AS2" s="63" t="inlineStr">
+      <c r="AP2" s="60" t="n"/>
+      <c r="AQ2" s="60" t="n"/>
+      <c r="AR2" s="62" t="n"/>
+      <c r="AS2" s="61" t="inlineStr">
         <is>
           <t>27-May-2020</t>
         </is>
       </c>
-      <c r="AT2" s="63" t="inlineStr">
+      <c r="AT2" s="61" t="inlineStr">
         <is>
           <t>28-Jun-2021</t>
         </is>
       </c>
-      <c r="AU2" s="63" t="inlineStr">
+      <c r="AU2" s="61" t="inlineStr">
         <is>
           <t>10,000.00</t>
         </is>
       </c>
-      <c r="AV2" s="63" t="inlineStr">
+      <c r="AV2" s="61" t="inlineStr">
         <is>
           <t>25-May-2020</t>
         </is>
       </c>
-      <c r="AW2" s="63" t="n"/>
-      <c r="AX2" s="63" t="n"/>
-      <c r="AY2" s="63" t="n"/>
-      <c r="AZ2" s="63" t="n"/>
-      <c r="BA2" s="63" t="n"/>
-      <c r="BB2" s="63" t="n"/>
-      <c r="BC2" s="63" t="n"/>
-      <c r="BD2" s="63" t="n"/>
-      <c r="BE2" s="63" t="n"/>
-      <c r="BF2" s="63" t="n"/>
-      <c r="BG2" s="63" t="n"/>
-      <c r="BH2" s="63" t="n"/>
-      <c r="BI2" s="63" t="n"/>
-      <c r="BJ2" s="61" t="inlineStr">
+      <c r="AW2" s="61" t="n"/>
+      <c r="AX2" s="61" t="n"/>
+      <c r="AY2" s="61" t="n"/>
+      <c r="AZ2" s="61" t="n"/>
+      <c r="BA2" s="61" t="n"/>
+      <c r="BB2" s="61" t="n"/>
+      <c r="BC2" s="61" t="n"/>
+      <c r="BD2" s="61" t="n"/>
+      <c r="BE2" s="61" t="n"/>
+      <c r="BF2" s="61" t="n"/>
+      <c r="BG2" s="61" t="n"/>
+      <c r="BH2" s="61" t="n"/>
+      <c r="BI2" s="61" t="n"/>
+      <c r="BJ2" s="59" t="inlineStr">
         <is>
           <t>27-Dec-2019</t>
         </is>
       </c>
-      <c r="BK2" s="61" t="inlineStr">
+      <c r="BK2" s="59" t="inlineStr">
         <is>
           <t>275,750.00</t>
         </is>
       </c>
-      <c r="BL2" s="61" t="inlineStr">
+      <c r="BL2" s="59" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="BM2" s="61" t="inlineStr">
+      <c r="BM2" s="59" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BN2" s="61" t="inlineStr">
+      <c r="BN2" s="59" t="inlineStr">
         <is>
           <t>Establishment/Extension Fee</t>
         </is>
       </c>
-      <c r="BO2" s="61" t="inlineStr">
+      <c r="BO2" s="59" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="76">
-      <c r="A3" s="78" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="74">
+      <c r="A3" s="76" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2212,273 +2198,464 @@
           <t>Ongoing Fee Payment Intent Notice</t>
         </is>
       </c>
-      <c r="C3" s="63" t="inlineStr">
-        <is>
-          <t>CBANLD_03112020160326YZJ</t>
-        </is>
-      </c>
-      <c r="D3" s="69" t="inlineStr">
+      <c r="C3" s="61" t="n"/>
+      <c r="D3" s="67" t="inlineStr">
         <is>
           <t>CH EDU Limited 1710818</t>
         </is>
       </c>
-      <c r="E3" s="62" t="inlineStr">
-        <is>
-          <t>CBANLDNAFAC03112020161931</t>
-        </is>
-      </c>
-      <c r="F3" s="62" t="inlineStr">
-        <is>
-          <t>60000035</t>
-        </is>
-      </c>
-      <c r="G3" s="69" t="inlineStr">
+      <c r="E3" s="60" t="n"/>
+      <c r="F3" s="60" t="n"/>
+      <c r="G3" s="67" t="inlineStr">
         <is>
           <t>Linda Chu</t>
         </is>
       </c>
-      <c r="H3" s="65" t="inlineStr">
+      <c r="H3" s="63" t="inlineStr">
         <is>
           <t>LOANIQ01</t>
         </is>
       </c>
-      <c r="I3" s="69" t="inlineStr">
+      <c r="I3" s="67" t="inlineStr">
         <is>
           <t>9HEMMY3A</t>
         </is>
       </c>
-      <c r="J3" s="69" t="inlineStr">
+      <c r="J3" s="67" t="inlineStr">
         <is>
           <t>LIQ-9HEMMY3A-9HEMMY1R-2</t>
         </is>
       </c>
-      <c r="K3" s="69" t="inlineStr">
+      <c r="K3" s="67" t="inlineStr">
         <is>
           <t>2021-01-23 00:00:00.000</t>
         </is>
       </c>
-      <c r="L3" s="69" t="inlineStr">
+      <c r="L3" s="67" t="inlineStr">
         <is>
           <t>2021-01-03 00:00:00.000</t>
         </is>
       </c>
-      <c r="M3" s="65" t="n">
+      <c r="M3" s="63" t="n">
         <v>5</v>
       </c>
-      <c r="N3" s="65" t="inlineStr">
+      <c r="N3" s="63" t="inlineStr">
         <is>
           <t>Fee Payment Notice</t>
         </is>
       </c>
-      <c r="O3" s="66" t="inlineStr">
+      <c r="O3" s="64" t="inlineStr">
         <is>
           <t>Notice Identifier</t>
         </is>
       </c>
-      <c r="P3" s="66" t="inlineStr">
+      <c r="P3" s="64" t="inlineStr">
         <is>
           <t>CBA Email with PDF Attachment</t>
         </is>
       </c>
-      <c r="Q3" s="69" t="inlineStr">
+      <c r="Q3" s="67" t="inlineStr">
         <is>
           <t>2021-01-13 18:45:16.775</t>
         </is>
       </c>
-      <c r="R3" s="69" t="inlineStr">
+      <c r="R3" s="67" t="inlineStr">
         <is>
           <t>2021-01-13 18:45:16.775</t>
         </is>
       </c>
-      <c r="S3" s="66" t="inlineStr">
+      <c r="S3" s="64" t="inlineStr">
         <is>
           <t>Legal Name</t>
         </is>
       </c>
-      <c r="T3" s="66" t="inlineStr">
+      <c r="T3" s="64" t="inlineStr">
         <is>
           <t>C:\Users\u720589\AppData\Local\Temp\</t>
         </is>
       </c>
-      <c r="U3" s="66" t="inlineStr">
+      <c r="U3" s="64" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
         </is>
       </c>
-      <c r="V3" s="66" t="inlineStr">
+      <c r="V3" s="64" t="inlineStr">
         <is>
           <t>API_COR_TC02</t>
         </is>
       </c>
-      <c r="W3" s="67" t="inlineStr">
+      <c r="W3" s="65" t="inlineStr">
         <is>
           <t>TEMP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="X3" s="67" t="inlineStr">
+      <c r="X3" s="65" t="inlineStr">
         <is>
           <t>INPUT_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Y3" s="67" t="inlineStr">
+      <c r="Y3" s="65" t="inlineStr">
         <is>
           <t>EXP_API_COR_TC02</t>
         </is>
       </c>
-      <c r="Z3" s="67" t="inlineStr">
+      <c r="Z3" s="65" t="inlineStr">
         <is>
           <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
         </is>
       </c>
-      <c r="AA3" s="67" t="inlineStr">
+      <c r="AA3" s="65" t="inlineStr">
         <is>
           <t>correlationId</t>
         </is>
       </c>
-      <c r="AB3" s="67" t="inlineStr">
+      <c r="AB3" s="65" t="inlineStr">
         <is>
           <t>API_COR_RESPONSE_TC2</t>
         </is>
       </c>
-      <c r="AC3" s="62" t="n"/>
-      <c r="AD3" s="67" t="inlineStr">
+      <c r="AC3" s="60" t="n"/>
+      <c r="AD3" s="65" t="inlineStr">
         <is>
           <t>SENT</t>
         </is>
       </c>
-      <c r="AE3" s="67" t="n"/>
-      <c r="AF3" s="68" t="n"/>
-      <c r="AG3" s="62" t="n"/>
-      <c r="AH3" s="66" t="inlineStr">
+      <c r="AE3" s="65" t="n"/>
+      <c r="AF3" s="66" t="n"/>
+      <c r="AG3" s="60" t="n"/>
+      <c r="AH3" s="64" t="inlineStr">
         <is>
           <t>Sent</t>
         </is>
       </c>
-      <c r="AI3" s="62" t="n"/>
-      <c r="AJ3" s="65" t="inlineStr">
+      <c r="AI3" s="60" t="n"/>
+      <c r="AJ3" s="63" t="inlineStr">
         <is>
           <t>FEE INVOICE</t>
         </is>
       </c>
-      <c r="AK3" s="62" t="n"/>
-      <c r="AL3" s="63" t="inlineStr">
+      <c r="AK3" s="60" t="n"/>
+      <c r="AL3" s="61" t="inlineStr">
         <is>
           <t>10.000000%</t>
         </is>
       </c>
-      <c r="AM3" s="63" t="inlineStr">
+      <c r="AM3" s="61" t="inlineStr">
         <is>
           <t>5.000000%</t>
         </is>
       </c>
-      <c r="AN3" s="63" t="inlineStr">
+      <c r="AN3" s="61" t="inlineStr">
         <is>
           <t>15.000000%</t>
         </is>
       </c>
-      <c r="AO3" s="63" t="inlineStr">
+      <c r="AO3" s="61" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AP3" s="62" t="n"/>
-      <c r="AQ3" s="62" t="n"/>
-      <c r="AR3" s="64" t="n"/>
-      <c r="AS3" s="63" t="inlineStr">
+      <c r="AP3" s="60" t="n"/>
+      <c r="AQ3" s="60" t="n"/>
+      <c r="AR3" s="62" t="n"/>
+      <c r="AS3" s="61" t="inlineStr">
         <is>
           <t>27-May-2020</t>
         </is>
       </c>
-      <c r="AT3" s="63" t="inlineStr">
+      <c r="AT3" s="61" t="inlineStr">
         <is>
           <t>28-Jun-2021</t>
         </is>
       </c>
-      <c r="AU3" s="63" t="inlineStr">
+      <c r="AU3" s="61" t="inlineStr">
         <is>
           <t>10,000.00</t>
         </is>
       </c>
-      <c r="AV3" s="63" t="inlineStr">
+      <c r="AV3" s="61" t="inlineStr">
         <is>
           <t>25-May-2020</t>
         </is>
       </c>
-      <c r="AW3" s="63" t="n"/>
-      <c r="AX3" s="63" t="n"/>
-      <c r="AY3" s="63" t="n"/>
-      <c r="AZ3" s="63" t="n"/>
-      <c r="BA3" s="63" t="n"/>
-      <c r="BB3" s="63" t="n"/>
-      <c r="BC3" s="63" t="n"/>
-      <c r="BD3" s="63" t="n"/>
-      <c r="BE3" s="63" t="n"/>
-      <c r="BF3" s="63" t="n"/>
-      <c r="BG3" s="63" t="n"/>
-      <c r="BH3" s="63" t="n"/>
-      <c r="BI3" s="63" t="n"/>
-      <c r="BJ3" s="75" t="inlineStr">
+      <c r="AW3" s="61" t="n"/>
+      <c r="AX3" s="61" t="n"/>
+      <c r="AY3" s="61" t="n"/>
+      <c r="AZ3" s="61" t="n"/>
+      <c r="BA3" s="61" t="n"/>
+      <c r="BB3" s="61" t="n"/>
+      <c r="BC3" s="61" t="n"/>
+      <c r="BD3" s="61" t="n"/>
+      <c r="BE3" s="61" t="n"/>
+      <c r="BF3" s="61" t="n"/>
+      <c r="BG3" s="61" t="n"/>
+      <c r="BH3" s="61" t="n"/>
+      <c r="BI3" s="61" t="n"/>
+      <c r="BJ3" s="73" t="inlineStr">
         <is>
           <t>27-Dec-2019</t>
         </is>
       </c>
-      <c r="BK3" s="75" t="inlineStr">
+      <c r="BK3" s="73" t="inlineStr">
         <is>
           <t>275,750.00</t>
         </is>
       </c>
-      <c r="BL3" s="75" t="inlineStr">
+      <c r="BL3" s="73" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="BM3" s="75" t="inlineStr">
+      <c r="BM3" s="73" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BN3" s="75" t="inlineStr">
+      <c r="BN3" s="73" t="inlineStr">
         <is>
           <t>Establishment/Extension Fee</t>
         </is>
       </c>
-      <c r="BO3" s="61" t="inlineStr">
+      <c r="BO3" s="59" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" s="52" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D4" s="58" t="n"/>
-      <c r="G4" s="56" t="n"/>
-      <c r="H4" s="56" t="n"/>
-      <c r="I4" s="58" t="n"/>
-      <c r="J4" s="56" t="n"/>
-      <c r="K4" s="58" t="n"/>
-      <c r="L4" s="58" t="n"/>
-      <c r="M4" s="58" t="n"/>
-      <c r="N4" s="58" t="n"/>
-      <c r="O4" s="58" t="n"/>
-      <c r="P4" s="58" t="n"/>
-      <c r="Q4" s="58" t="n"/>
-      <c r="R4" s="58" t="n"/>
-      <c r="S4" s="56" t="n"/>
-      <c r="T4" s="56" t="n"/>
-      <c r="U4" s="56" t="n"/>
-      <c r="V4" s="56" t="n"/>
-      <c r="AH4" s="56" t="n"/>
-      <c r="AJ4" s="56" t="n"/>
-      <c r="BJ4" s="56" t="n"/>
-      <c r="BK4" s="56" t="n"/>
-      <c r="BL4" s="56" t="n"/>
-      <c r="BM4" s="56" t="n"/>
-      <c r="BN4" s="56" t="n"/>
-      <c r="BO4" s="56" t="n"/>
+    <row r="4" ht="15" customHeight="1" s="74">
+      <c r="A4" s="76" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" s="53" t="inlineStr">
+        <is>
+          <t>Loan Repricing Intent Notice - Combine A &amp; B</t>
+        </is>
+      </c>
+      <c r="C4" s="61" t="n"/>
+      <c r="D4" s="67" t="inlineStr">
+        <is>
+          <t>CH EDU Limited 1710818</t>
+        </is>
+      </c>
+      <c r="E4" s="60" t="n"/>
+      <c r="F4" s="60" t="n"/>
+      <c r="G4" s="67" t="inlineStr">
+        <is>
+          <t>Linda Chu</t>
+        </is>
+      </c>
+      <c r="H4" s="63" t="inlineStr">
+        <is>
+          <t>LOANIQ01</t>
+        </is>
+      </c>
+      <c r="I4" s="67" t="inlineStr">
+        <is>
+          <t>G9EN1EIM</t>
+        </is>
+      </c>
+      <c r="J4" s="67" t="inlineStr">
+        <is>
+          <t>LIQ-G9EN1EIM-G4EN1D8I-2</t>
+        </is>
+      </c>
+      <c r="K4" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-25 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="L4" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-15 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="M4" s="63" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" s="63" t="inlineStr">
+        <is>
+          <t>Repricing Intent Notice</t>
+        </is>
+      </c>
+      <c r="O4" s="64" t="inlineStr">
+        <is>
+          <t>Notice Identifier</t>
+        </is>
+      </c>
+      <c r="P4" s="64" t="inlineStr">
+        <is>
+          <t>CBA Email with PDF Attachment</t>
+        </is>
+      </c>
+      <c r="Q4" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-20 16:24:41.211</t>
+        </is>
+      </c>
+      <c r="R4" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-20 16:24:41.211</t>
+        </is>
+      </c>
+      <c r="S4" s="64" t="inlineStr">
+        <is>
+          <t>Legal Name</t>
+        </is>
+      </c>
+      <c r="T4" s="64" t="inlineStr">
+        <is>
+          <t>C:\Users\u720589\AppData\Local\Temp\</t>
+        </is>
+      </c>
+      <c r="U4" s="64" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
+        </is>
+      </c>
+      <c r="V4" s="64" t="inlineStr">
+        <is>
+          <t>API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="W4" s="65" t="inlineStr">
+        <is>
+          <t>TEMP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="X4" s="65" t="inlineStr">
+        <is>
+          <t>INPUT_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Y4" s="65" t="inlineStr">
+        <is>
+          <t>EXP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Z4" s="65" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
+        </is>
+      </c>
+      <c r="AA4" s="65" t="inlineStr">
+        <is>
+          <t>correlationId</t>
+        </is>
+      </c>
+      <c r="AB4" s="65" t="inlineStr">
+        <is>
+          <t>API_COR_RESPONSE_TC2</t>
+        </is>
+      </c>
+      <c r="AC4" s="60" t="n"/>
+      <c r="AD4" s="65" t="inlineStr">
+        <is>
+          <t>SENT</t>
+        </is>
+      </c>
+      <c r="AE4" s="65" t="n"/>
+      <c r="AF4" s="66" t="n"/>
+      <c r="AG4" s="60" t="n"/>
+      <c r="AH4" s="64" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="AI4" s="60" t="n"/>
+      <c r="AJ4" s="63" t="inlineStr">
+        <is>
+          <t>FEE INVOICE</t>
+        </is>
+      </c>
+      <c r="AK4" s="60" t="n"/>
+      <c r="AL4" s="61" t="inlineStr">
+        <is>
+          <t>10.000000%</t>
+        </is>
+      </c>
+      <c r="AM4" s="61" t="inlineStr">
+        <is>
+          <t>5.000000%</t>
+        </is>
+      </c>
+      <c r="AN4" s="61" t="inlineStr">
+        <is>
+          <t>15.000000%</t>
+        </is>
+      </c>
+      <c r="AO4" s="61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AP4" s="60" t="n"/>
+      <c r="AQ4" s="60" t="n"/>
+      <c r="AR4" s="62" t="n"/>
+      <c r="AS4" s="61" t="inlineStr">
+        <is>
+          <t>27-May-2020</t>
+        </is>
+      </c>
+      <c r="AT4" s="61" t="inlineStr">
+        <is>
+          <t>28-Jun-2021</t>
+        </is>
+      </c>
+      <c r="AU4" s="61" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="AV4" s="61" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="AW4" s="61" t="n"/>
+      <c r="AX4" s="61" t="n"/>
+      <c r="AY4" s="61" t="n"/>
+      <c r="AZ4" s="61" t="n"/>
+      <c r="BA4" s="61" t="n"/>
+      <c r="BB4" s="61" t="n"/>
+      <c r="BC4" s="61" t="n"/>
+      <c r="BD4" s="61" t="n"/>
+      <c r="BE4" s="61" t="n"/>
+      <c r="BF4" s="61" t="n"/>
+      <c r="BG4" s="61" t="n"/>
+      <c r="BH4" s="61" t="n"/>
+      <c r="BI4" s="61" t="n"/>
+      <c r="BJ4" s="73" t="inlineStr">
+        <is>
+          <t>27-Dec-2019</t>
+        </is>
+      </c>
+      <c r="BK4" s="73" t="inlineStr">
+        <is>
+          <t>275,750.00</t>
+        </is>
+      </c>
+      <c r="BL4" s="73" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BM4" s="73" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BN4" s="73" t="inlineStr">
+        <is>
+          <t>Establishment/Extension Fee</t>
+        </is>
+      </c>
+      <c r="BO4" s="59" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2501,33 +2678,33 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
-    <col width="51.28515625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="11" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
-    <col width="23.5703125" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="25.28515625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="23.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="21" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
-    <col width="37.7109375" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
-    <col width="23.85546875" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
-    <col width="26" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
-    <col width="26.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="76" min="20" max="20"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="76" min="21" max="21"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="76" min="22" max="22"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="23" max="23"/>
-    <col width="19.85546875" bestFit="1" customWidth="1" style="76" min="24" max="24"/>
-    <col width="31.28515625" bestFit="1" customWidth="1" style="76" min="25" max="25"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="26" max="26"/>
-    <col width="29.140625" bestFit="1" customWidth="1" style="76" min="27" max="27"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="51.28515625" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="11" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="74" min="6" max="6"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="25.28515625" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="21" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
+    <col width="37.7109375" bestFit="1" customWidth="1" style="74" min="15" max="15"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="74" min="16" max="16"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="74" min="17" max="17"/>
+    <col width="26" bestFit="1" customWidth="1" style="74" min="18" max="18"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" style="74" min="19" max="19"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="74" min="20" max="20"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="74" min="21" max="21"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="74" min="22" max="22"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="74" min="23" max="23"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="74" min="24" max="24"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" style="74" min="25" max="25"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="74" min="26" max="26"/>
+    <col width="29.140625" bestFit="1" customWidth="1" style="74" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2546,122 +2723,122 @@
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="D1" s="70" t="inlineStr">
+      <c r="D1" s="68" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
       </c>
-      <c r="E1" s="70" t="inlineStr">
+      <c r="E1" s="68" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="F1" s="70" t="inlineStr">
+      <c r="F1" s="68" t="inlineStr">
         <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="G1" s="70" t="inlineStr">
+      <c r="G1" s="68" t="inlineStr">
         <is>
           <t>Loan_RequestedAmount</t>
         </is>
       </c>
-      <c r="H1" s="70" t="inlineStr">
+      <c r="H1" s="68" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="I1" s="70" t="inlineStr">
+      <c r="I1" s="68" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="J1" s="70" t="inlineStr">
+      <c r="J1" s="68" t="inlineStr">
         <is>
           <t>Loan_RepricingFrequency</t>
         </is>
       </c>
-      <c r="K1" s="70" t="inlineStr">
+      <c r="K1" s="68" t="inlineStr">
         <is>
           <t>Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="L1" s="70" t="inlineStr">
+      <c r="L1" s="68" t="inlineStr">
         <is>
           <t>Loan_Accrue</t>
         </is>
       </c>
-      <c r="M1" s="70" t="inlineStr">
+      <c r="M1" s="68" t="inlineStr">
         <is>
           <t>Loan_RepricingDate</t>
         </is>
       </c>
-      <c r="N1" s="70" t="inlineStr">
+      <c r="N1" s="68" t="inlineStr">
         <is>
           <t>Notice_Subject</t>
         </is>
       </c>
-      <c r="O1" s="70" t="inlineStr">
+      <c r="O1" s="68" t="inlineStr">
         <is>
           <t>Notice_Comment</t>
         </is>
       </c>
-      <c r="P1" s="70" t="inlineStr">
+      <c r="P1" s="68" t="inlineStr">
         <is>
           <t>AcceptRate_FromPricing</t>
         </is>
       </c>
-      <c r="Q1" s="70" t="inlineStr">
+      <c r="Q1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalOriginal</t>
         </is>
       </c>
-      <c r="R1" s="70" t="inlineStr">
+      <c r="R1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalCurrent</t>
         </is>
       </c>
-      <c r="S1" s="70" t="inlineStr">
+      <c r="S1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankGross</t>
         </is>
       </c>
-      <c r="T1" s="70" t="inlineStr">
+      <c r="T1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankNet</t>
         </is>
       </c>
-      <c r="U1" s="70" t="inlineStr">
+      <c r="U1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanCurrentBaseRate</t>
         </is>
       </c>
-      <c r="V1" s="70" t="inlineStr">
+      <c r="V1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanSpread</t>
         </is>
       </c>
-      <c r="W1" s="70" t="inlineStr">
+      <c r="W1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanAllInRate</t>
         </is>
       </c>
-      <c r="X1" s="70" t="inlineStr">
+      <c r="X1" s="68" t="inlineStr">
         <is>
           <t>Loan_PaymentMode</t>
         </is>
       </c>
-      <c r="Y1" s="70" t="inlineStr">
+      <c r="Y1" s="68" t="inlineStr">
         <is>
           <t>Expctd_Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="Z1" s="70" t="inlineStr">
+      <c r="Z1" s="68" t="inlineStr">
         <is>
           <t>BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="AA1" s="70" t="inlineStr">
+      <c r="AA1" s="68" t="inlineStr">
         <is>
           <t>AcceptRate_FromInterpolation</t>
         </is>
@@ -2798,7 +2975,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="AA2" s="75" t="n"/>
+      <c r="AA2" s="73" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="37" t="inlineStr">
@@ -2866,9 +3043,9 @@
           <t>16-Mar-2020</t>
         </is>
       </c>
-      <c r="N3" s="75" t="n"/>
-      <c r="O3" s="75" t="n"/>
-      <c r="P3" s="75" t="n"/>
+      <c r="N3" s="73" t="n"/>
+      <c r="O3" s="73" t="n"/>
+      <c r="P3" s="73" t="n"/>
       <c r="Q3" s="37" t="inlineStr">
         <is>
           <t>36,500,000.00</t>
@@ -2991,8 +3168,8 @@
           <t>03-Jan-2020</t>
         </is>
       </c>
-      <c r="N4" s="75" t="n"/>
-      <c r="O4" s="75" t="n"/>
+      <c r="N4" s="73" t="n"/>
+      <c r="O4" s="73" t="n"/>
       <c r="P4" t="inlineStr">
         <is>
           <t>Y</t>
@@ -3048,7 +3225,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="AA4" s="75" t="n"/>
+      <c r="AA4" s="73" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="37" t="inlineStr">
@@ -3116,8 +3293,8 @@
           <t>03-Jan-2020</t>
         </is>
       </c>
-      <c r="N5" s="75" t="n"/>
-      <c r="O5" s="75" t="n"/>
+      <c r="N5" s="73" t="n"/>
+      <c r="O5" s="73" t="n"/>
       <c r="P5" t="inlineStr">
         <is>
           <t>Y</t>
@@ -3173,7 +3350,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="AA5" s="75" t="n"/>
+      <c r="AA5" s="73" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3196,37 +3373,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
-    <col width="29.42578125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="74" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
-    <col width="20.5703125" customWidth="1" style="74" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="74" min="6" max="27"/>
-    <col width="8.7109375" customWidth="1" style="74" min="28" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
+    <col width="29.42578125" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
+    <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
+    <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="29"/>
+    <col width="8.7109375" customWidth="1" style="72" min="30" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="73">
-      <c r="A1" s="72" t="inlineStr">
+    <row r="1" customFormat="1" s="71">
+      <c r="A1" s="70" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="72" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="72" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>AdjustmentSelection</t>
         </is>
       </c>
-      <c r="D1" s="73" t="inlineStr">
+      <c r="D1" s="71" t="inlineStr">
         <is>
           <t>GL_ShortName</t>
         </is>
       </c>
-      <c r="E1" s="73" t="inlineStr">
+      <c r="E1" s="71" t="inlineStr">
         <is>
           <t>GL_Offset_Type</t>
         </is>
@@ -3248,12 +3425,12 @@
           <t>Portfolio Settled Discount Change</t>
         </is>
       </c>
-      <c r="D2" s="74" t="inlineStr">
+      <c r="D2" s="72" t="inlineStr">
         <is>
           <t>Fees Held Awaiting Dispos.</t>
         </is>
       </c>
-      <c r="E2" s="74" t="inlineStr">
+      <c r="E2" s="72" t="inlineStr">
         <is>
           <t>Existing WIP</t>
         </is>
@@ -3285,49 +3462,49 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
-    <col width="33.42578125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="74" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
-    <col width="30.140625" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
-    <col width="30.140625" customWidth="1" style="74" min="6" max="6"/>
-    <col width="24" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="74" min="8" max="28"/>
-    <col width="8.7109375" customWidth="1" style="74" min="29" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
+    <col width="33.42578125" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
+    <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
+    <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
+    <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
+    <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="30"/>
+    <col width="8.7109375" customWidth="1" style="72" min="31" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="73">
-      <c r="A1" s="72" t="inlineStr">
+    <row r="1" customFormat="1" s="71">
+      <c r="A1" s="70" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="72" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="72" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>Deal_RatioType</t>
         </is>
       </c>
-      <c r="D1" s="73" t="inlineStr">
+      <c r="D1" s="71" t="inlineStr">
         <is>
           <t>NewFinancial_Ratio</t>
         </is>
       </c>
-      <c r="E1" s="73" t="inlineStr">
+      <c r="E1" s="71" t="inlineStr">
         <is>
           <t>DealEventStatus1</t>
         </is>
       </c>
-      <c r="F1" s="73" t="inlineStr">
+      <c r="F1" s="71" t="inlineStr">
         <is>
           <t>DealEventStatus2</t>
         </is>
       </c>
-      <c r="G1" s="73" t="inlineStr">
+      <c r="G1" s="71" t="inlineStr">
         <is>
           <t>FinancialRatio_StartDate</t>
         </is>
@@ -3349,22 +3526,22 @@
           <t>Leverage Ratio (LR)</t>
         </is>
       </c>
-      <c r="D2" s="77" t="inlineStr">
+      <c r="D2" s="75" t="inlineStr">
         <is>
           <t>0.355</t>
         </is>
       </c>
-      <c r="E2" s="74" t="inlineStr">
+      <c r="E2" s="72" t="inlineStr">
         <is>
           <t>Deal Change Transaction Released</t>
         </is>
       </c>
-      <c r="F2" s="74" t="inlineStr">
+      <c r="F2" s="72" t="inlineStr">
         <is>
           <t>Financial Ratio Changed</t>
         </is>
       </c>
-      <c r="G2" s="77" t="inlineStr">
+      <c r="G2" s="75" t="inlineStr">
         <is>
           <t>31-Dec-2019</t>
         </is>
@@ -3396,65 +3573,65 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
-    <col width="33.42578125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="74" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
-    <col width="24.28515625" customWidth="1" style="74" min="5" max="8"/>
-    <col width="30.140625" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
-    <col width="30.140625" customWidth="1" style="74" min="10" max="10"/>
-    <col width="24" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="74" min="12" max="32"/>
-    <col width="8.7109375" customWidth="1" style="74" min="33" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
+    <col width="33.42578125" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
+    <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
+    <col width="24.28515625" customWidth="1" style="72" min="5" max="8"/>
+    <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
+    <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
+    <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="34"/>
+    <col width="8.7109375" customWidth="1" style="72" min="35" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="73">
-      <c r="A1" s="72" t="inlineStr">
+    <row r="1" customFormat="1" s="71">
+      <c r="A1" s="70" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="72" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="72" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>Fee_Type</t>
         </is>
       </c>
-      <c r="D1" s="73" t="inlineStr">
+      <c r="D1" s="71" t="inlineStr">
         <is>
           <t>Cycle_Number</t>
         </is>
       </c>
-      <c r="E1" s="73" t="inlineStr">
+      <c r="E1" s="71" t="inlineStr">
         <is>
           <t>Cycle_StartDate</t>
         </is>
       </c>
-      <c r="F1" s="73" t="inlineStr">
+      <c r="F1" s="71" t="inlineStr">
         <is>
           <t>Cycle_EndDate</t>
         </is>
       </c>
-      <c r="G1" s="73" t="inlineStr">
+      <c r="G1" s="71" t="inlineStr">
         <is>
           <t>Cycle_DueDate</t>
         </is>
       </c>
-      <c r="H1" s="73" t="inlineStr">
+      <c r="H1" s="71" t="inlineStr">
         <is>
           <t>ProjectedCycleDue</t>
         </is>
       </c>
-      <c r="I1" s="73" t="inlineStr">
+      <c r="I1" s="71" t="inlineStr">
         <is>
           <t>Effective_Date</t>
         </is>
       </c>
-      <c r="J1" s="73" t="inlineStr">
+      <c r="J1" s="71" t="inlineStr">
         <is>
           <t>Expected_CycleDueAmt</t>
         </is>
@@ -3476,40 +3653,40 @@
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="D2" s="77" t="n">
+      <c r="D2" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="77" t="inlineStr">
+      <c r="E2" s="75" t="inlineStr">
         <is>
           <t>01-Oct-2019</t>
         </is>
       </c>
-      <c r="F2" s="77" t="inlineStr">
+      <c r="F2" s="75" t="inlineStr">
         <is>
           <t>31-Dec-2019</t>
         </is>
       </c>
-      <c r="G2" s="77" t="inlineStr">
+      <c r="G2" s="75" t="inlineStr">
         <is>
           <t>02-Jan-2020</t>
         </is>
       </c>
-      <c r="H2" s="77" t="inlineStr">
+      <c r="H2" s="75" t="inlineStr">
         <is>
           <t>204,668.49</t>
         </is>
       </c>
-      <c r="I2" s="77" t="inlineStr">
+      <c r="I2" s="75" t="inlineStr">
         <is>
           <t>02-Jan-2020</t>
         </is>
       </c>
-      <c r="J2" s="77" t="inlineStr">
+      <c r="J2" s="75" t="inlineStr">
         <is>
           <t>204,668.49</t>
         </is>
       </c>
-      <c r="K2" s="77" t="n"/>
+      <c r="K2" s="75" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
@@ -3531,94 +3708,94 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
-    <col width="33.42578125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="74" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
-    <col width="24.28515625" customWidth="1" style="74" min="5" max="8"/>
-    <col width="30.140625" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
-    <col width="30.140625" customWidth="1" style="74" min="10" max="10"/>
-    <col width="24" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
-    <col width="23.85546875" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="74" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="74" min="33" max="16384"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
+    <col width="33.42578125" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
+    <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
+    <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
+    <col width="24.28515625" customWidth="1" style="72" min="5" max="8"/>
+    <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
+    <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
+    <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="72" min="12" max="12"/>
+    <col width="23.85546875" bestFit="1" customWidth="1" style="72" min="13" max="13"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="72" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="72" min="15" max="34"/>
+    <col width="8.7109375" customWidth="1" style="72" min="35" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="73">
-      <c r="A1" s="72" t="inlineStr">
+    <row r="1" customFormat="1" s="71">
+      <c r="A1" s="70" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="72" t="inlineStr">
+      <c r="B1" s="70" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="72" t="inlineStr">
+      <c r="C1" s="70" t="inlineStr">
         <is>
           <t>OutstandingSelect_Type</t>
         </is>
       </c>
-      <c r="D1" s="72" t="inlineStr">
+      <c r="D1" s="70" t="inlineStr">
         <is>
           <t>Repricing_Type</t>
         </is>
       </c>
-      <c r="E1" s="73" t="inlineStr">
+      <c r="E1" s="71" t="inlineStr">
         <is>
           <t>Effective_Date</t>
         </is>
       </c>
-      <c r="F1" s="73" t="inlineStr">
+      <c r="F1" s="71" t="inlineStr">
         <is>
           <t>Repricing_Add_Option</t>
         </is>
       </c>
-      <c r="G1" s="79" t="inlineStr">
+      <c r="G1" s="77" t="inlineStr">
         <is>
           <t>LoanMerge_Amount</t>
         </is>
       </c>
-      <c r="H1" s="79" t="inlineStr">
+      <c r="H1" s="77" t="inlineStr">
         <is>
           <t>Alias_LoanMerge</t>
         </is>
       </c>
-      <c r="I1" s="73" t="inlineStr">
+      <c r="I1" s="71" t="inlineStr">
         <is>
           <t>BaseRate_Percentage</t>
         </is>
       </c>
-      <c r="J1" s="73" t="inlineStr">
+      <c r="J1" s="71" t="inlineStr">
         <is>
           <t>Outstanding_A_IntAmt</t>
         </is>
       </c>
-      <c r="K1" s="73" t="inlineStr">
+      <c r="K1" s="71" t="inlineStr">
         <is>
           <t>Outstanding_B_IntAmt</t>
         </is>
       </c>
-      <c r="L1" s="70" t="inlineStr">
+      <c r="L1" s="68" t="inlineStr">
         <is>
           <t>BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="M1" s="73" t="inlineStr">
+      <c r="M1" s="71" t="inlineStr">
         <is>
           <t>AcceptRate_FromPricing</t>
         </is>
       </c>
-      <c r="N1" s="70" t="inlineStr">
+      <c r="N1" s="68" t="inlineStr">
         <is>
           <t>Outstanding_Type</t>
         </is>
@@ -3645,37 +3822,37 @@
           <t>Comprehensive Repricing</t>
         </is>
       </c>
-      <c r="E2" s="77" t="inlineStr">
+      <c r="E2" s="75" t="inlineStr">
         <is>
           <t>03-Jan-2020</t>
         </is>
       </c>
-      <c r="F2" s="77" t="inlineStr">
+      <c r="F2" s="75" t="inlineStr">
         <is>
           <t>Rollover/Conversion To New:</t>
         </is>
       </c>
-      <c r="G2" s="77" t="inlineStr">
+      <c r="G2" s="75" t="inlineStr">
         <is>
           <t>23,600,000.00</t>
         </is>
       </c>
-      <c r="H2" s="77" t="inlineStr">
+      <c r="H2" s="75" t="inlineStr">
         <is>
           <t>60002342</t>
         </is>
       </c>
-      <c r="I2" s="77" t="inlineStr">
+      <c r="I2" s="75" t="inlineStr">
         <is>
           <t>0.92000%</t>
         </is>
       </c>
-      <c r="J2" s="77" t="inlineStr">
+      <c r="J2" s="75" t="inlineStr">
         <is>
           <t>27,392.05</t>
         </is>
       </c>
-      <c r="K2" s="77" t="inlineStr">
+      <c r="K2" s="75" t="inlineStr">
         <is>
           <t>1,992.40</t>
         </is>
@@ -3685,7 +3862,7 @@
           <t>None</t>
         </is>
       </c>
-      <c r="M2" s="74" t="inlineStr">
+      <c r="M2" s="72" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -3696,7 +3873,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="9" t="n"/>
@@ -3769,8 +3945,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="64"/>
-    <col width="9.140625" customWidth="1" style="31" min="65" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="66"/>
+    <col width="9.140625" customWidth="1" style="31" min="67" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">
@@ -4233,7 +4409,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1" s="76">
+    <row r="3" ht="30" customHeight="1" s="74">
       <c r="C3" s="29" t="n"/>
       <c r="D3" s="29" t="n"/>
       <c r="E3" s="29" t="n"/>
@@ -4305,25 +4481,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
-    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="27" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="23.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="20.7109375" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="18" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
-    <col width="32" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="27" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="6" max="6"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="18" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="74" min="15" max="15"/>
+    <col width="32" bestFit="1" customWidth="1" style="74" min="16" max="16"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="74" min="17" max="17"/>
+    <col width="24.42578125" bestFit="1" customWidth="1" style="74" min="18" max="18"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4544,23 +4720,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
-    <col width="27.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" style="76" min="6" max="7"/>
-    <col width="15.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="19.140625" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="27.5703125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="74" min="6" max="7"/>
+    <col width="15.7109375" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="19.140625" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="74" min="15" max="15"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="74" min="16" max="16"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="74" min="17" max="17"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="74" min="18" max="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4771,25 +4947,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
-    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="32.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="27" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="23.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="20.7109375" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="18" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
-    <col width="19.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
-    <col width="32" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
-    <col width="24.42578125" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="27" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="6" max="6"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="23.140625" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="20.7109375" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="18" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="74" min="15" max="15"/>
+    <col width="32" bestFit="1" customWidth="1" style="74" min="16" max="16"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="74" min="17" max="17"/>
+    <col width="24.42578125" bestFit="1" customWidth="1" style="74" min="18" max="18"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5010,60 +5186,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" bestFit="1" customWidth="1" style="76" min="1" max="1"/>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="17.85546875" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="22.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
-    <col width="22" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
-    <col width="27.42578125" bestFit="1" customWidth="1" style="76" min="15" max="15"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="76" min="16" max="16"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="17" max="17"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" style="76" min="18" max="18"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="19" max="19"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="76" min="20" max="20"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="76" min="21" max="21"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="76" min="22" max="22"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="23" max="23"/>
-    <col width="27.42578125" bestFit="1" customWidth="1" style="76" min="24" max="24"/>
-    <col width="30.42578125" bestFit="1" customWidth="1" style="76" min="25" max="25"/>
-    <col width="16.7109375" bestFit="1" customWidth="1" style="76" min="26" max="26"/>
-    <col width="22.5703125" bestFit="1" customWidth="1" style="76" min="27" max="27"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="76" min="28" max="28"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="29" max="29"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="30" max="30"/>
-    <col width="38.5703125" bestFit="1" customWidth="1" style="76" min="31" max="31"/>
-    <col width="39.140625" bestFit="1" customWidth="1" style="76" min="32" max="32"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="33" max="33"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="34" max="34"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="35" max="35"/>
-    <col width="18.85546875" bestFit="1" customWidth="1" style="76" min="36" max="36"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="37" max="37"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="38" max="38"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="76" min="39" max="39"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="40" max="40"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="41" max="41"/>
-    <col width="38.5703125" bestFit="1" customWidth="1" style="76" min="42" max="42"/>
-    <col width="39.140625" bestFit="1" customWidth="1" style="76" min="43" max="43"/>
-    <col width="18.28515625" bestFit="1" customWidth="1" style="76" min="44" max="44"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="45" max="45"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="76" min="46" max="46"/>
-    <col width="18.85546875" bestFit="1" customWidth="1" style="76" min="47" max="47"/>
-    <col width="21.7109375" bestFit="1" customWidth="1" style="76" min="48" max="48"/>
-    <col width="24.7109375" bestFit="1" customWidth="1" style="76" min="49" max="49"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="76" min="50" max="50"/>
-    <col width="23.42578125" bestFit="1" customWidth="1" style="76" min="51" max="51"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="76" min="52" max="52"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="76" min="53" max="53"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="76" min="54" max="54"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="74" min="1" max="1"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="22.42578125" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="21.85546875" bestFit="1" customWidth="1" style="74" min="6" max="6"/>
+    <col width="22" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="31.140625" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="74" min="15" max="15"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="74" min="16" max="16"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="74" min="17" max="17"/>
+    <col width="31.85546875" bestFit="1" customWidth="1" style="74" min="18" max="18"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="74" min="19" max="19"/>
+    <col width="25.140625" bestFit="1" customWidth="1" style="74" min="20" max="20"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" style="74" min="21" max="21"/>
+    <col width="31.140625" bestFit="1" customWidth="1" style="74" min="22" max="22"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="74" min="23" max="23"/>
+    <col width="27.42578125" bestFit="1" customWidth="1" style="74" min="24" max="24"/>
+    <col width="30.42578125" bestFit="1" customWidth="1" style="74" min="25" max="25"/>
+    <col width="16.7109375" bestFit="1" customWidth="1" style="74" min="26" max="26"/>
+    <col width="22.5703125" bestFit="1" customWidth="1" style="74" min="27" max="27"/>
+    <col width="39.85546875" bestFit="1" customWidth="1" style="74" min="28" max="28"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="74" min="29" max="29"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="74" min="30" max="30"/>
+    <col width="38.5703125" bestFit="1" customWidth="1" style="74" min="31" max="31"/>
+    <col width="39.140625" bestFit="1" customWidth="1" style="74" min="32" max="32"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="74" min="33" max="33"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="74" min="34" max="34"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="74" min="35" max="35"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="74" min="36" max="36"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="37" max="37"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="38" max="38"/>
+    <col width="39.85546875" bestFit="1" customWidth="1" style="74" min="39" max="39"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="74" min="40" max="40"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="74" min="41" max="41"/>
+    <col width="38.5703125" bestFit="1" customWidth="1" style="74" min="42" max="42"/>
+    <col width="39.140625" bestFit="1" customWidth="1" style="74" min="43" max="43"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="74" min="44" max="44"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="74" min="45" max="45"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="74" min="46" max="46"/>
+    <col width="18.85546875" bestFit="1" customWidth="1" style="74" min="47" max="47"/>
+    <col width="21.7109375" bestFit="1" customWidth="1" style="74" min="48" max="48"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="74" min="49" max="49"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="74" min="50" max="50"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="74" min="51" max="51"/>
+    <col width="29.28515625" bestFit="1" customWidth="1" style="74" min="52" max="52"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" style="74" min="53" max="53"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="74" min="54" max="54"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5616,19 +5792,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="36.28515625" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="26.28515625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="18.42578125" customWidth="1" style="76" min="6" max="6"/>
-    <col width="27.28515625" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="20" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="26.28515625" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="34.85546875" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="22" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="18.42578125" customWidth="1" style="74" min="6" max="6"/>
+    <col width="27.28515625" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="20" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="34.85546875" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="22" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5795,9 +5971,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="32.140625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5863,19 +6039,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="38.140625" bestFit="1" customWidth="1" style="76" min="2" max="2"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" style="76" min="3" max="3"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="76" min="4" max="4"/>
-    <col width="26" bestFit="1" customWidth="1" style="76" min="5" max="5"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="76" min="6" max="6"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="76" min="7" max="7"/>
-    <col width="21" bestFit="1" customWidth="1" style="76" min="8" max="8"/>
-    <col width="49.42578125" bestFit="1" customWidth="1" style="76" min="9" max="9"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="10" max="10"/>
-    <col width="24" bestFit="1" customWidth="1" style="76" min="11" max="11"/>
-    <col width="16.42578125" bestFit="1" customWidth="1" style="76" min="12" max="12"/>
-    <col width="22.85546875" bestFit="1" customWidth="1" style="76" min="13" max="13"/>
-    <col width="24" bestFit="1" customWidth="1" style="76" min="14" max="14"/>
+    <col width="38.140625" bestFit="1" customWidth="1" style="74" min="2" max="2"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="74" min="3" max="3"/>
+    <col width="32.140625" bestFit="1" customWidth="1" style="74" min="4" max="4"/>
+    <col width="26" bestFit="1" customWidth="1" style="74" min="5" max="5"/>
+    <col width="36.140625" bestFit="1" customWidth="1" style="74" min="6" max="6"/>
+    <col width="33.140625" bestFit="1" customWidth="1" style="74" min="7" max="7"/>
+    <col width="21" bestFit="1" customWidth="1" style="74" min="8" max="8"/>
+    <col width="49.42578125" bestFit="1" customWidth="1" style="74" min="9" max="9"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="74" min="10" max="10"/>
+    <col width="24" bestFit="1" customWidth="1" style="74" min="11" max="11"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="74" min="12" max="12"/>
+    <col width="22.85546875" bestFit="1" customWidth="1" style="74" min="13" max="13"/>
+    <col width="24" bestFit="1" customWidth="1" style="74" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6023,7 +6199,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="71" t="inlineStr">
+      <c r="D3" s="69" t="inlineStr">
         <is>
           <t>Should be 27-Dec-2019</t>
         </is>

</xml_diff>

<commit_message>
GDE-9411 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -1537,11 +1537,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BO4"/>
+  <dimension ref="A1:BO5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I24" sqref="I24"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1611,8 +1611,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="135"/>
-    <col width="9.140625" customWidth="1" style="52" min="136" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="136"/>
+    <col width="9.140625" customWidth="1" style="52" min="137" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2652,6 +2652,241 @@
         </is>
       </c>
       <c r="BO4" s="59" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="74">
+      <c r="A5" s="76" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" s="53" t="inlineStr">
+        <is>
+          <t>Loan Repricing Rate Setting Notice - Combine A &amp; B</t>
+        </is>
+      </c>
+      <c r="C5" s="61" t="n"/>
+      <c r="D5" s="67" t="inlineStr">
+        <is>
+          <t>CH EDU Limited 1710818</t>
+        </is>
+      </c>
+      <c r="E5" s="60" t="n"/>
+      <c r="F5" s="60" t="n"/>
+      <c r="G5" s="67" t="inlineStr">
+        <is>
+          <t>Linda Chu</t>
+        </is>
+      </c>
+      <c r="H5" s="63" t="inlineStr">
+        <is>
+          <t>LOANIQ01</t>
+        </is>
+      </c>
+      <c r="I5" s="67" t="inlineStr">
+        <is>
+          <t>G(EN1FAD</t>
+        </is>
+      </c>
+      <c r="J5" s="67" t="inlineStr">
+        <is>
+          <t>LIQ-G(EN1FAD-G4EN1D8I-2</t>
+        </is>
+      </c>
+      <c r="K5" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-26 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="L5" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-16 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="M5" s="63" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" s="63" t="inlineStr">
+        <is>
+          <t>Deal Level Loan Repricing Rate Setting Notice</t>
+        </is>
+      </c>
+      <c r="O5" s="64" t="inlineStr">
+        <is>
+          <t>Notice Identifier</t>
+        </is>
+      </c>
+      <c r="P5" s="64" t="inlineStr">
+        <is>
+          <t>CBA Email with PDF Attachment</t>
+        </is>
+      </c>
+      <c r="Q5" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-21 13:26:36.352</t>
+        </is>
+      </c>
+      <c r="R5" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-21 13:26:36.352</t>
+        </is>
+      </c>
+      <c r="S5" s="64" t="inlineStr">
+        <is>
+          <t>Legal Name</t>
+        </is>
+      </c>
+      <c r="T5" s="64" t="inlineStr">
+        <is>
+          <t>C:\Users\u720589\AppData\Local\Temp\</t>
+        </is>
+      </c>
+      <c r="U5" s="64" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
+        </is>
+      </c>
+      <c r="V5" s="64" t="inlineStr">
+        <is>
+          <t>API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="W5" s="65" t="inlineStr">
+        <is>
+          <t>TEMP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="X5" s="65" t="inlineStr">
+        <is>
+          <t>INPUT_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Y5" s="65" t="inlineStr">
+        <is>
+          <t>EXP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Z5" s="65" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
+        </is>
+      </c>
+      <c r="AA5" s="65" t="inlineStr">
+        <is>
+          <t>correlationId</t>
+        </is>
+      </c>
+      <c r="AB5" s="65" t="inlineStr">
+        <is>
+          <t>API_COR_RESPONSE_TC2</t>
+        </is>
+      </c>
+      <c r="AC5" s="60" t="n"/>
+      <c r="AD5" s="65" t="inlineStr">
+        <is>
+          <t>SENT</t>
+        </is>
+      </c>
+      <c r="AE5" s="65" t="n"/>
+      <c r="AF5" s="66" t="n"/>
+      <c r="AG5" s="60" t="n"/>
+      <c r="AH5" s="64" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="AI5" s="60" t="n"/>
+      <c r="AJ5" s="63" t="inlineStr">
+        <is>
+          <t>FEE INVOICE</t>
+        </is>
+      </c>
+      <c r="AK5" s="60" t="n"/>
+      <c r="AL5" s="61" t="inlineStr">
+        <is>
+          <t>10.000000%</t>
+        </is>
+      </c>
+      <c r="AM5" s="61" t="inlineStr">
+        <is>
+          <t>5.000000%</t>
+        </is>
+      </c>
+      <c r="AN5" s="61" t="inlineStr">
+        <is>
+          <t>15.000000%</t>
+        </is>
+      </c>
+      <c r="AO5" s="61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AP5" s="60" t="n"/>
+      <c r="AQ5" s="60" t="n"/>
+      <c r="AR5" s="62" t="n"/>
+      <c r="AS5" s="61" t="inlineStr">
+        <is>
+          <t>27-May-2020</t>
+        </is>
+      </c>
+      <c r="AT5" s="61" t="inlineStr">
+        <is>
+          <t>28-Jun-2021</t>
+        </is>
+      </c>
+      <c r="AU5" s="61" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="AV5" s="61" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="AW5" s="61" t="n"/>
+      <c r="AX5" s="61" t="n"/>
+      <c r="AY5" s="61" t="n"/>
+      <c r="AZ5" s="61" t="n"/>
+      <c r="BA5" s="61" t="n"/>
+      <c r="BB5" s="61" t="n"/>
+      <c r="BC5" s="61" t="n"/>
+      <c r="BD5" s="61" t="n"/>
+      <c r="BE5" s="61" t="n"/>
+      <c r="BF5" s="61" t="n"/>
+      <c r="BG5" s="61" t="n"/>
+      <c r="BH5" s="61" t="n"/>
+      <c r="BI5" s="61" t="n"/>
+      <c r="BJ5" s="73" t="inlineStr">
+        <is>
+          <t>27-Dec-2019</t>
+        </is>
+      </c>
+      <c r="BK5" s="73" t="inlineStr">
+        <is>
+          <t>275,750.00</t>
+        </is>
+      </c>
+      <c r="BL5" s="73" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BM5" s="73" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BN5" s="73" t="inlineStr">
+        <is>
+          <t>Establishment/Extension Fee</t>
+        </is>
+      </c>
+      <c r="BO5" s="59" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
@@ -3378,8 +3613,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="29"/>
-    <col width="8.7109375" customWidth="1" style="72" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="30"/>
+    <col width="8.7109375" customWidth="1" style="72" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3469,8 +3704,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="30"/>
-    <col width="8.7109375" customWidth="1" style="72" min="31" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="31"/>
+    <col width="8.7109375" customWidth="1" style="72" min="32" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3581,8 +3816,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="34"/>
-    <col width="8.7109375" customWidth="1" style="72" min="35" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="35"/>
+    <col width="8.7109375" customWidth="1" style="72" min="36" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3725,8 +3960,8 @@
     <col width="18.28515625" bestFit="1" customWidth="1" style="72" min="12" max="12"/>
     <col width="23.85546875" bestFit="1" customWidth="1" style="72" min="13" max="13"/>
     <col width="17.5703125" bestFit="1" customWidth="1" style="72" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="72" min="15" max="34"/>
-    <col width="8.7109375" customWidth="1" style="72" min="35" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="15" max="35"/>
+    <col width="8.7109375" customWidth="1" style="72" min="36" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3945,8 +4180,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="66"/>
-    <col width="9.140625" customWidth="1" style="31" min="67" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="67"/>
+    <col width="9.140625" customWidth="1" style="31" min="68" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9413 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -1539,9 +1539,9 @@
   </sheetPr>
   <dimension ref="A1:BO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1611,8 +1611,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="136"/>
-    <col width="9.140625" customWidth="1" style="52" min="137" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="137"/>
+    <col width="9.140625" customWidth="1" style="52" min="138" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2905,10 +2905,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3587,6 +3587,131 @@
       </c>
       <c r="AA5" s="73" t="n"/>
     </row>
+    <row r="6" s="74">
+      <c r="A6" s="37" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="35" t="inlineStr">
+        <is>
+          <t>Create Drawdown for Capitalization Facility - Outstanding C</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>60002504</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="G6" s="37" t="inlineStr">
+        <is>
+          <t>750,000.00</t>
+        </is>
+      </c>
+      <c r="H6" s="37" t="inlineStr">
+        <is>
+          <t>15-Jan-2020</t>
+        </is>
+      </c>
+      <c r="I6" s="37" t="inlineStr">
+        <is>
+          <t>29-Aug-2023</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>to the adjusted due date</t>
+        </is>
+      </c>
+      <c r="M6" s="37" t="inlineStr">
+        <is>
+          <t>03-Feb-2020</t>
+        </is>
+      </c>
+      <c r="N6" s="73" t="n"/>
+      <c r="O6" s="73" t="n"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="Q6" s="37" t="inlineStr">
+        <is>
+          <t>750,000.00</t>
+        </is>
+      </c>
+      <c r="R6" s="37" t="inlineStr">
+        <is>
+          <t>750,000.00</t>
+        </is>
+      </c>
+      <c r="S6" s="37" t="inlineStr">
+        <is>
+          <t>750,000.00</t>
+        </is>
+      </c>
+      <c r="T6" s="37" t="inlineStr">
+        <is>
+          <t>750,000.00</t>
+        </is>
+      </c>
+      <c r="U6" s="37" t="inlineStr">
+        <is>
+          <t>0.901500%</t>
+        </is>
+      </c>
+      <c r="V6" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="W6" s="37" t="inlineStr">
+        <is>
+          <t>1.626500%</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AA6" s="73" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3613,8 +3738,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="30"/>
-    <col width="8.7109375" customWidth="1" style="72" min="31" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="31"/>
+    <col width="8.7109375" customWidth="1" style="72" min="32" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3704,8 +3829,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="31"/>
-    <col width="8.7109375" customWidth="1" style="72" min="32" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="32"/>
+    <col width="8.7109375" customWidth="1" style="72" min="33" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3816,8 +3941,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="35"/>
-    <col width="8.7109375" customWidth="1" style="72" min="36" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="36"/>
+    <col width="8.7109375" customWidth="1" style="72" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3960,8 +4085,8 @@
     <col width="18.28515625" bestFit="1" customWidth="1" style="72" min="12" max="12"/>
     <col width="23.85546875" bestFit="1" customWidth="1" style="72" min="13" max="13"/>
     <col width="17.5703125" bestFit="1" customWidth="1" style="72" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="72" min="15" max="35"/>
-    <col width="8.7109375" customWidth="1" style="72" min="36" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="72" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4180,8 +4305,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="67"/>
-    <col width="9.140625" customWidth="1" style="31" min="68" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="68"/>
+    <col width="9.140625" customWidth="1" style="31" min="69" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9416 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -346,6 +346,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1611,8 +1613,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="138"/>
-    <col width="9.140625" customWidth="1" style="52" min="139" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="142"/>
+    <col width="9.140625" customWidth="1" style="52" min="143" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2907,8 +2909,8 @@
   </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3712,7 +3714,7 @@
       </c>
       <c r="AA6" s="73" t="n"/>
     </row>
-    <row r="7" s="74">
+    <row r="7">
       <c r="A7" s="37" t="inlineStr">
         <is>
           <t>6</t>
@@ -3863,8 +3865,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="32"/>
-    <col width="8.7109375" customWidth="1" style="72" min="33" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="36"/>
+    <col width="8.7109375" customWidth="1" style="72" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3954,8 +3956,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="33"/>
-    <col width="8.7109375" customWidth="1" style="72" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="37"/>
+    <col width="8.7109375" customWidth="1" style="72" min="38" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4066,8 +4068,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="37"/>
-    <col width="8.7109375" customWidth="1" style="72" min="38" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="41"/>
+    <col width="8.7109375" customWidth="1" style="72" min="42" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4191,27 +4193,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
-    <col width="33.42578125" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
-    <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
-    <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
-    <col width="24.28515625" customWidth="1" style="72" min="5" max="8"/>
-    <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
-    <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
-    <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
+    <col width="6.140625" bestFit="1" customWidth="1" style="72" min="1" max="1"/>
+    <col width="26.28515625" bestFit="1" customWidth="1" style="72" min="2" max="2"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" style="72" min="3" max="3"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
+    <col width="14" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
+    <col width="24.7109375" bestFit="1" customWidth="1" style="72" min="6" max="6"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" style="72" min="8" max="8"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="72" min="9" max="11"/>
     <col width="18.28515625" bestFit="1" customWidth="1" style="72" min="12" max="12"/>
     <col width="23.85546875" bestFit="1" customWidth="1" style="72" min="13" max="13"/>
     <col width="17.5703125" bestFit="1" customWidth="1" style="72" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="72" min="15" max="37"/>
-    <col width="8.7109375" customWidth="1" style="72" min="38" max="16384"/>
+    <col width="21" bestFit="1" customWidth="1" style="72" min="15" max="16"/>
+    <col width="15" bestFit="1" customWidth="1" style="72" min="17" max="17"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="72" min="18" max="18"/>
+    <col width="26" bestFit="1" customWidth="1" style="72" min="19" max="19"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" style="72" min="20" max="20"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="72" min="21" max="21"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="72" min="22" max="22"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="72" min="23" max="23"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="72" min="24" max="24"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="72" min="25" max="25"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" style="72" min="26" max="26"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="27" max="27"/>
+    <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
+    <col width="8.7109375" customWidth="1" style="72" min="29" max="41"/>
+    <col width="8.7109375" customWidth="1" style="72" min="42" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4285,6 +4301,76 @@
           <t>Outstanding_Type</t>
         </is>
       </c>
+      <c r="O1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_1_IntAmt</t>
+        </is>
+      </c>
+      <c r="P1" s="71" t="inlineStr">
+        <is>
+          <t>Outstanding_2_IntAmt</t>
+        </is>
+      </c>
+      <c r="Q1" s="71" t="inlineStr">
+        <is>
+          <t>Repricing_Date</t>
+        </is>
+      </c>
+      <c r="R1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanGlobalOriginal</t>
+        </is>
+      </c>
+      <c r="S1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanGlobalCurrent</t>
+        </is>
+      </c>
+      <c r="T1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanHostBankGross</t>
+        </is>
+      </c>
+      <c r="U1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanHostBankNet</t>
+        </is>
+      </c>
+      <c r="V1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanCurrentBaseRate</t>
+        </is>
+      </c>
+      <c r="W1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanSpread</t>
+        </is>
+      </c>
+      <c r="X1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_LoanAllInRate</t>
+        </is>
+      </c>
+      <c r="Y1" s="68" t="inlineStr">
+        <is>
+          <t>Loan_PaymentMode</t>
+        </is>
+      </c>
+      <c r="Z1" s="68" t="inlineStr">
+        <is>
+          <t>Expctd_Loan_IntCycleFrequency</t>
+        </is>
+      </c>
+      <c r="AA1" s="68" t="inlineStr">
+        <is>
+          <t>Pricing_Option</t>
+        </is>
+      </c>
+      <c r="AB1" s="68" t="inlineStr">
+        <is>
+          <t>Loan_RepricingFrequency</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -4355,6 +4441,154 @@
       <c r="N2" t="inlineStr">
         <is>
           <t>Loan</t>
+        </is>
+      </c>
+      <c r="O2" s="78" t="n"/>
+      <c r="P2" s="78" t="n"/>
+      <c r="Q2" s="78" t="n"/>
+      <c r="R2" s="78" t="n"/>
+      <c r="S2" s="78" t="n"/>
+      <c r="T2" s="78" t="n"/>
+      <c r="U2" s="78" t="n"/>
+      <c r="V2" s="78" t="n"/>
+      <c r="W2" s="78" t="n"/>
+      <c r="X2" s="78" t="n"/>
+      <c r="Y2" s="78" t="n"/>
+      <c r="Z2" s="78" t="n"/>
+      <c r="AA2" s="78" t="n"/>
+      <c r="AB2" s="73" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Combine Outstanding AB &amp; C</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="E3" s="75" t="inlineStr">
+        <is>
+          <t>03-Feb-2020</t>
+        </is>
+      </c>
+      <c r="F3" s="75" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion To New:</t>
+        </is>
+      </c>
+      <c r="G3" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="H3" s="75" t="inlineStr">
+        <is>
+          <t>60002636</t>
+        </is>
+      </c>
+      <c r="I3" s="75" t="inlineStr">
+        <is>
+          <t>0.84620%</t>
+        </is>
+      </c>
+      <c r="J3" s="79" t="n"/>
+      <c r="K3" s="79" t="n"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M3" s="72" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="O3" s="75" t="inlineStr">
+        <is>
+          <t>635.00</t>
+        </is>
+      </c>
+      <c r="P3" s="75" t="inlineStr">
+        <is>
+          <t>32,972.11</t>
+        </is>
+      </c>
+      <c r="Q3" s="75" t="inlineStr">
+        <is>
+          <t>04-Mar-2020</t>
+        </is>
+      </c>
+      <c r="R3" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="S3" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="T3" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="U3" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="V3" s="75" t="inlineStr">
+        <is>
+          <t>0.846200%</t>
+        </is>
+      </c>
+      <c r="W3" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="X3" s="37" t="inlineStr">
+        <is>
+          <t>1.571200%</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>1 Months</t>
         </is>
       </c>
     </row>
@@ -4430,8 +4664,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="69"/>
-    <col width="9.140625" customWidth="1" style="31" min="70" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="73"/>
+    <col width="9.140625" customWidth="1" style="31" min="74" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9418 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -1613,8 +1613,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="142"/>
-    <col width="9.140625" customWidth="1" style="52" min="143" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="143"/>
+    <col width="9.140625" customWidth="1" style="52" min="144" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2907,10 +2907,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3839,6 +3839,131 @@
       </c>
       <c r="AA7" s="73" t="n"/>
     </row>
+    <row r="8" s="74">
+      <c r="A8" s="37" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" s="35" t="inlineStr">
+        <is>
+          <t>Create Drawdown for Capitalization Facility - Outstanding E</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>60002652</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="G8" s="37" t="inlineStr">
+        <is>
+          <t>14,000,000.00</t>
+        </is>
+      </c>
+      <c r="H8" s="37" t="inlineStr">
+        <is>
+          <t>19-Feb-2020</t>
+        </is>
+      </c>
+      <c r="I8" s="37" t="inlineStr">
+        <is>
+          <t>29-Aug-2023</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>to the adjusted due date</t>
+        </is>
+      </c>
+      <c r="M8" s="37" t="inlineStr">
+        <is>
+          <t>04-Mar-2020</t>
+        </is>
+      </c>
+      <c r="N8" s="73" t="n"/>
+      <c r="O8" s="73" t="n"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="Q8" s="37" t="inlineStr">
+        <is>
+          <t>14,000,000.00</t>
+        </is>
+      </c>
+      <c r="R8" s="37" t="inlineStr">
+        <is>
+          <t>14,000,000.00</t>
+        </is>
+      </c>
+      <c r="S8" s="37" t="inlineStr">
+        <is>
+          <t>14,000,000.00</t>
+        </is>
+      </c>
+      <c r="T8" s="37" t="inlineStr">
+        <is>
+          <t>14,000,000.00</t>
+        </is>
+      </c>
+      <c r="U8" s="37" t="inlineStr">
+        <is>
+          <t>0.855000%</t>
+        </is>
+      </c>
+      <c r="V8" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="W8" s="37" t="inlineStr">
+        <is>
+          <t>1.580000%</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="AA8" s="73" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3865,8 +3990,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="36"/>
-    <col width="8.7109375" customWidth="1" style="72" min="37" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="37"/>
+    <col width="8.7109375" customWidth="1" style="72" min="38" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -3956,8 +4081,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="37"/>
-    <col width="8.7109375" customWidth="1" style="72" min="38" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="38"/>
+    <col width="8.7109375" customWidth="1" style="72" min="39" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4068,8 +4193,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="41"/>
-    <col width="8.7109375" customWidth="1" style="72" min="42" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="42"/>
+    <col width="8.7109375" customWidth="1" style="72" min="43" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4195,7 +4320,7 @@
   </sheetPr>
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -4226,8 +4351,8 @@
     <col width="31.28515625" bestFit="1" customWidth="1" style="72" min="26" max="26"/>
     <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="27" max="27"/>
     <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
-    <col width="8.7109375" customWidth="1" style="72" min="29" max="41"/>
-    <col width="8.7109375" customWidth="1" style="72" min="42" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="29" max="42"/>
+    <col width="8.7109375" customWidth="1" style="72" min="43" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4664,8 +4789,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="73"/>
-    <col width="9.140625" customWidth="1" style="31" min="74" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="74"/>
+    <col width="9.140625" customWidth="1" style="31" min="75" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9539 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="5" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -348,6 +348,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1613,8 +1614,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="144"/>
-    <col width="9.140625" customWidth="1" style="52" min="145" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="148"/>
+    <col width="9.140625" customWidth="1" style="52" min="149" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2909,8 +2910,8 @@
   </sheetPr>
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3964,7 +3965,7 @@
       </c>
       <c r="AA8" s="73" t="n"/>
     </row>
-    <row r="9" s="74">
+    <row r="9">
       <c r="A9" s="37" t="inlineStr">
         <is>
           <t>8</t>
@@ -4115,8 +4116,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="38"/>
-    <col width="8.7109375" customWidth="1" style="72" min="39" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="42"/>
+    <col width="8.7109375" customWidth="1" style="72" min="43" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4206,8 +4207,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="39"/>
-    <col width="8.7109375" customWidth="1" style="72" min="40" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="43"/>
+    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4355,8 +4356,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="43"/>
-    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="47"/>
+    <col width="8.7109375" customWidth="1" style="72" min="48" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4480,10 +4481,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -4501,20 +4502,21 @@
     <col width="23.85546875" bestFit="1" customWidth="1" style="72" min="13" max="13"/>
     <col width="17.5703125" bestFit="1" customWidth="1" style="72" min="14" max="14"/>
     <col width="21" bestFit="1" customWidth="1" style="72" min="15" max="16"/>
-    <col width="15" bestFit="1" customWidth="1" style="72" min="17" max="17"/>
-    <col width="26.5703125" bestFit="1" customWidth="1" style="72" min="18" max="18"/>
-    <col width="26" bestFit="1" customWidth="1" style="72" min="19" max="19"/>
-    <col width="26.7109375" bestFit="1" customWidth="1" style="72" min="20" max="20"/>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="72" min="21" max="21"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="72" min="22" max="22"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="72" min="23" max="23"/>
-    <col width="21.42578125" bestFit="1" customWidth="1" style="72" min="24" max="24"/>
-    <col width="19.85546875" bestFit="1" customWidth="1" style="72" min="25" max="25"/>
-    <col width="31.28515625" bestFit="1" customWidth="1" style="72" min="26" max="26"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="27" max="27"/>
-    <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
-    <col width="8.7109375" customWidth="1" style="72" min="29" max="43"/>
-    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
+    <col width="21" customWidth="1" style="72" min="17" max="17"/>
+    <col width="15" bestFit="1" customWidth="1" style="72" min="18" max="18"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" style="72" min="19" max="19"/>
+    <col width="26" bestFit="1" customWidth="1" style="72" min="20" max="20"/>
+    <col width="26.7109375" bestFit="1" customWidth="1" style="72" min="21" max="21"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="72" min="22" max="22"/>
+    <col width="28.5703125" bestFit="1" customWidth="1" style="72" min="23" max="23"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" style="72" min="24" max="24"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="72" min="25" max="25"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" style="72" min="26" max="26"/>
+    <col width="31.28515625" bestFit="1" customWidth="1" style="72" min="27" max="27"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
+    <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="29" max="29"/>
+    <col width="8.7109375" customWidth="1" style="72" min="30" max="48"/>
+    <col width="8.7109375" customWidth="1" style="72" min="49" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4600,60 +4602,65 @@
       </c>
       <c r="Q1" s="71" t="inlineStr">
         <is>
+          <t>Outstanding_3_IntAmt</t>
+        </is>
+      </c>
+      <c r="R1" s="71" t="inlineStr">
+        <is>
           <t>Repricing_Date</t>
         </is>
       </c>
-      <c r="R1" s="68" t="inlineStr">
+      <c r="S1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalOriginal</t>
         </is>
       </c>
-      <c r="S1" s="68" t="inlineStr">
+      <c r="T1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanGlobalCurrent</t>
         </is>
       </c>
-      <c r="T1" s="68" t="inlineStr">
+      <c r="U1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankGross</t>
         </is>
       </c>
-      <c r="U1" s="68" t="inlineStr">
+      <c r="V1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanHostBankNet</t>
         </is>
       </c>
-      <c r="V1" s="68" t="inlineStr">
+      <c r="W1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanCurrentBaseRate</t>
         </is>
       </c>
-      <c r="W1" s="68" t="inlineStr">
+      <c r="X1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanSpread</t>
         </is>
       </c>
-      <c r="X1" s="68" t="inlineStr">
+      <c r="Y1" s="68" t="inlineStr">
         <is>
           <t>Expctd_LoanAllInRate</t>
         </is>
       </c>
-      <c r="Y1" s="68" t="inlineStr">
+      <c r="Z1" s="68" t="inlineStr">
         <is>
           <t>Loan_PaymentMode</t>
         </is>
       </c>
-      <c r="Z1" s="68" t="inlineStr">
+      <c r="AA1" s="68" t="inlineStr">
         <is>
           <t>Expctd_Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="AA1" s="68" t="inlineStr">
+      <c r="AB1" s="68" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="AB1" s="68" t="inlineStr">
+      <c r="AC1" s="68" t="inlineStr">
         <is>
           <t>Loan_RepricingFrequency</t>
         </is>
@@ -4743,7 +4750,8 @@
       <c r="Y2" s="78" t="n"/>
       <c r="Z2" s="78" t="n"/>
       <c r="AA2" s="78" t="n"/>
-      <c r="AB2" s="73" t="n"/>
+      <c r="AB2" s="78" t="n"/>
+      <c r="AC2" s="73" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -4818,71 +4826,211 @@
           <t>32,972.11</t>
         </is>
       </c>
-      <c r="Q3" s="75" t="inlineStr">
+      <c r="Q3" s="79" t="n"/>
+      <c r="R3" s="75" t="inlineStr">
         <is>
           <t>04-Mar-2020</t>
         </is>
       </c>
-      <c r="R3" s="75" t="inlineStr">
+      <c r="S3" s="75" t="inlineStr">
         <is>
           <t>24,350,000.00</t>
         </is>
       </c>
-      <c r="S3" s="75" t="inlineStr">
+      <c r="T3" s="75" t="inlineStr">
         <is>
           <t>24,350,000.00</t>
         </is>
       </c>
-      <c r="T3" s="75" t="inlineStr">
+      <c r="U3" s="75" t="inlineStr">
         <is>
           <t>24,350,000.00</t>
         </is>
       </c>
-      <c r="U3" s="75" t="inlineStr">
+      <c r="V3" s="75" t="inlineStr">
         <is>
           <t>24,350,000.00</t>
         </is>
       </c>
-      <c r="V3" s="75" t="inlineStr">
+      <c r="W3" s="75" t="inlineStr">
         <is>
           <t>0.846200%</t>
         </is>
       </c>
-      <c r="W3" s="37" t="inlineStr">
+      <c r="X3" s="37" t="inlineStr">
         <is>
           <t>0.725000%</t>
         </is>
       </c>
-      <c r="X3" s="37" t="inlineStr">
+      <c r="Y3" s="37" t="inlineStr">
         <is>
           <t>1.571200%</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>Pay in Arrears</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>1 Months</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n"/>
-      <c r="B4" s="9" t="n"/>
-      <c r="C4" s="9" t="n"/>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Combine Outstanding D, E &amp; F</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="E4" s="75" t="inlineStr">
+        <is>
+          <t>04-Mar-2020</t>
+        </is>
+      </c>
+      <c r="F4" s="80" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion to New:</t>
+        </is>
+      </c>
+      <c r="G4" s="80" t="inlineStr">
+        <is>
+          <t>86,100,000.00</t>
+        </is>
+      </c>
+      <c r="H4" s="75" t="inlineStr">
+        <is>
+          <t>60002816</t>
+        </is>
+      </c>
+      <c r="I4" s="75" t="inlineStr">
+        <is>
+          <t>0.62860%</t>
+        </is>
+      </c>
+      <c r="J4" s="79" t="n"/>
+      <c r="K4" s="79" t="n"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M4" s="72" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="O4" s="75" t="inlineStr">
+        <is>
+          <t>297,821.86</t>
+        </is>
+      </c>
+      <c r="P4" s="75" t="inlineStr">
+        <is>
+          <t>8,484.38</t>
+        </is>
+      </c>
+      <c r="Q4" s="75" t="inlineStr">
+        <is>
+          <t>311.67</t>
+        </is>
+      </c>
+      <c r="R4" s="75" t="inlineStr">
+        <is>
+          <t>20-Mar-2020</t>
+        </is>
+      </c>
+      <c r="S4" s="75" t="inlineStr">
+        <is>
+          <t>86,100,000.00</t>
+        </is>
+      </c>
+      <c r="T4" s="75" t="inlineStr">
+        <is>
+          <t>86,100,000.00</t>
+        </is>
+      </c>
+      <c r="U4" s="75" t="inlineStr">
+        <is>
+          <t>86,100,000.00</t>
+        </is>
+      </c>
+      <c r="V4" s="75" t="inlineStr">
+        <is>
+          <t>86,100,000.00</t>
+        </is>
+      </c>
+      <c r="W4" s="75" t="inlineStr">
+        <is>
+          <t>0.628600%</t>
+        </is>
+      </c>
+      <c r="X4" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="Y4" s="37" t="inlineStr">
+        <is>
+          <t>1.353600%</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="O5" s="75" t="n"/>
+      <c r="P5" s="75" t="n"/>
+      <c r="Q5" s="75" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4951,8 +5099,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="75"/>
-    <col width="9.140625" customWidth="1" style="31" min="76" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="79"/>
+    <col width="9.140625" customWidth="1" style="31" min="80" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9540 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -1614,8 +1614,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="148"/>
-    <col width="9.140625" customWidth="1" style="52" min="149" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="149"/>
+    <col width="9.140625" customWidth="1" style="52" min="150" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -4116,8 +4116,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="42"/>
-    <col width="8.7109375" customWidth="1" style="72" min="43" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="43"/>
+    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4207,8 +4207,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="43"/>
-    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="44"/>
+    <col width="8.7109375" customWidth="1" style="72" min="45" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4356,8 +4356,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="47"/>
-    <col width="8.7109375" customWidth="1" style="72" min="48" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="48"/>
+    <col width="8.7109375" customWidth="1" style="72" min="49" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4481,10 +4481,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -4515,8 +4515,9 @@
     <col width="31.28515625" bestFit="1" customWidth="1" style="72" min="27" max="27"/>
     <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
     <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="29" max="29"/>
-    <col width="8.7109375" customWidth="1" style="72" min="30" max="48"/>
-    <col width="8.7109375" customWidth="1" style="72" min="49" max="16384"/>
+    <col width="14" customWidth="1" style="72" min="30" max="30"/>
+    <col width="8.7109375" customWidth="1" style="72" min="31" max="49"/>
+    <col width="8.7109375" customWidth="1" style="72" min="50" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4665,6 +4666,11 @@
           <t>Loan_RepricingFrequency</t>
         </is>
       </c>
+      <c r="AD1" s="71" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -4707,7 +4713,7 @@
           <t>60002342</t>
         </is>
       </c>
-      <c r="I2" s="75" t="inlineStr">
+      <c r="I2" s="79" t="inlineStr">
         <is>
           <t>0.92000%</t>
         </is>
@@ -4752,6 +4758,7 @@
       <c r="AA2" s="78" t="n"/>
       <c r="AB2" s="78" t="n"/>
       <c r="AC2" s="73" t="n"/>
+      <c r="AD2" s="78" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -4794,7 +4801,7 @@
           <t>60002636</t>
         </is>
       </c>
-      <c r="I3" s="75" t="inlineStr">
+      <c r="I3" s="79" t="inlineStr">
         <is>
           <t>0.84620%</t>
         </is>
@@ -4887,6 +4894,7 @@
           <t>1 Months</t>
         </is>
       </c>
+      <c r="AD3" s="78" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -4929,7 +4937,7 @@
           <t>60002816</t>
         </is>
       </c>
-      <c r="I4" s="75" t="inlineStr">
+      <c r="I4" s="79" t="inlineStr">
         <is>
           <t>0.62860%</t>
         </is>
@@ -5026,11 +5034,143 @@
           <t>1 Months</t>
         </is>
       </c>
+      <c r="AD4" s="78" t="n"/>
     </row>
     <row r="5">
-      <c r="O5" s="75" t="n"/>
-      <c r="P5" s="75" t="n"/>
-      <c r="Q5" s="75" t="n"/>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rollover Outstanding ABC</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Comprehensive Repricing</t>
+        </is>
+      </c>
+      <c r="E5" s="75" t="inlineStr">
+        <is>
+          <t>04-Mar-2020</t>
+        </is>
+      </c>
+      <c r="F5" s="75" t="inlineStr">
+        <is>
+          <t>Rollover/Conversion To New:</t>
+        </is>
+      </c>
+      <c r="G5" s="80" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="H5" s="75" t="inlineStr">
+        <is>
+          <t>60002857</t>
+        </is>
+      </c>
+      <c r="I5" s="75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J5" s="79" t="n"/>
+      <c r="K5" s="79" t="n"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M5" s="72" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="O5" s="75" t="inlineStr">
+        <is>
+          <t>31,445.52</t>
+        </is>
+      </c>
+      <c r="P5" s="79" t="n"/>
+      <c r="Q5" s="79" t="n"/>
+      <c r="R5" s="75" t="inlineStr">
+        <is>
+          <t>20-Mar-2020</t>
+        </is>
+      </c>
+      <c r="S5" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="T5" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="U5" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="V5" s="75" t="inlineStr">
+        <is>
+          <t>24,350,000.00</t>
+        </is>
+      </c>
+      <c r="W5" s="75" t="inlineStr">
+        <is>
+          <t>0.628600%</t>
+        </is>
+      </c>
+      <c r="X5" s="37" t="inlineStr">
+        <is>
+          <t>0.725000%</t>
+        </is>
+      </c>
+      <c r="Y5" s="37" t="inlineStr">
+        <is>
+          <t>1.353600%</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Pay in Arrears</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>BBSY - Bid</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>1 Months</t>
+        </is>
+      </c>
+      <c r="AD5" s="72" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5099,8 +5239,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="79"/>
-    <col width="9.140625" customWidth="1" style="31" min="80" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="80"/>
+    <col width="9.140625" customWidth="1" style="31" min="81" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9541 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -1540,17 +1540,17 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BO5"/>
+  <dimension ref="A1:BO6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I22" sqref="I22"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6.5703125" customWidth="1" style="54" min="1" max="1"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="54" min="2" max="2"/>
+    <col width="50.140625" bestFit="1" customWidth="1" style="54" min="2" max="2"/>
     <col width="27.42578125" bestFit="1" customWidth="1" style="52" min="3" max="3"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="54" min="4" max="4"/>
     <col width="29.28515625" bestFit="1" customWidth="1" style="52" min="5" max="5"/>
@@ -1614,8 +1614,8 @@
     <col width="9.7109375" bestFit="1" customWidth="1" style="52" min="65" max="65"/>
     <col width="26" bestFit="1" customWidth="1" style="52" min="66" max="66"/>
     <col width="36.28515625" bestFit="1" customWidth="1" style="52" min="67" max="67"/>
-    <col width="9.140625" customWidth="1" style="52" min="68" max="149"/>
-    <col width="9.140625" customWidth="1" style="52" min="150" max="16384"/>
+    <col width="9.140625" customWidth="1" style="52" min="68" max="151"/>
+    <col width="9.140625" customWidth="1" style="52" min="152" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.15" customHeight="1" s="74">
@@ -2890,6 +2890,241 @@
         </is>
       </c>
       <c r="BO5" s="59" t="inlineStr">
+        <is>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="74">
+      <c r="A6" s="76" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" s="53" t="inlineStr">
+        <is>
+          <t>Loan Repricing Intent Notice for Rollover Outstanding ABC</t>
+        </is>
+      </c>
+      <c r="C6" s="61" t="n"/>
+      <c r="D6" s="67" t="inlineStr">
+        <is>
+          <t>CH EDU Limited 1710818</t>
+        </is>
+      </c>
+      <c r="E6" s="60" t="n"/>
+      <c r="F6" s="60" t="n"/>
+      <c r="G6" s="67" t="inlineStr">
+        <is>
+          <t>Linda Chu</t>
+        </is>
+      </c>
+      <c r="H6" s="63" t="inlineStr">
+        <is>
+          <t>LOANIQ01</t>
+        </is>
+      </c>
+      <c r="I6" s="67" t="inlineStr">
+        <is>
+          <t>?RENV04J</t>
+        </is>
+      </c>
+      <c r="J6" s="67" t="inlineStr">
+        <is>
+          <t>LIQ-?RENV04J-?!ENUYZJ-6</t>
+        </is>
+      </c>
+      <c r="K6" s="67" t="inlineStr">
+        <is>
+          <t>2021-02-10 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="L6" s="67" t="inlineStr">
+        <is>
+          <t>2021-01-31 00:00:00.000</t>
+        </is>
+      </c>
+      <c r="M6" s="63" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="63" t="inlineStr">
+        <is>
+          <t>Repricing Intent Notice</t>
+        </is>
+      </c>
+      <c r="O6" s="64" t="inlineStr">
+        <is>
+          <t>Notice Identifier</t>
+        </is>
+      </c>
+      <c r="P6" s="64" t="inlineStr">
+        <is>
+          <t>CBA Email with PDF Attachment</t>
+        </is>
+      </c>
+      <c r="Q6" s="67" t="inlineStr">
+        <is>
+          <t>2021-02-05 09:35:34.840</t>
+        </is>
+      </c>
+      <c r="R6" s="67" t="inlineStr">
+        <is>
+          <t>2021-02-05 09:35:34.840</t>
+        </is>
+      </c>
+      <c r="S6" s="64" t="inlineStr">
+        <is>
+          <t>Legal Name</t>
+        </is>
+      </c>
+      <c r="T6" s="64" t="inlineStr">
+        <is>
+          <t>C:\Users\u720589\AppData\Local\Temp\</t>
+        </is>
+      </c>
+      <c r="U6" s="64" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Input\Correspondence\</t>
+        </is>
+      </c>
+      <c r="V6" s="64" t="inlineStr">
+        <is>
+          <t>API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="W6" s="65" t="inlineStr">
+        <is>
+          <t>TEMP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="X6" s="65" t="inlineStr">
+        <is>
+          <t>INPUT_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Y6" s="65" t="inlineStr">
+        <is>
+          <t>EXP_API_COR_TC02</t>
+        </is>
+      </c>
+      <c r="Z6" s="65" t="inlineStr">
+        <is>
+          <t>\DataSet\LoanIQ_DataSet\EU_Entity\API_EU\Output\Correspondence\</t>
+        </is>
+      </c>
+      <c r="AA6" s="65" t="inlineStr">
+        <is>
+          <t>correlationId</t>
+        </is>
+      </c>
+      <c r="AB6" s="65" t="inlineStr">
+        <is>
+          <t>API_COR_RESPONSE_TC2</t>
+        </is>
+      </c>
+      <c r="AC6" s="60" t="n"/>
+      <c r="AD6" s="65" t="inlineStr">
+        <is>
+          <t>SENT</t>
+        </is>
+      </c>
+      <c r="AE6" s="65" t="n"/>
+      <c r="AF6" s="66" t="n"/>
+      <c r="AG6" s="60" t="n"/>
+      <c r="AH6" s="64" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="AI6" s="60" t="n"/>
+      <c r="AJ6" s="63" t="inlineStr">
+        <is>
+          <t>FEE INVOICE</t>
+        </is>
+      </c>
+      <c r="AK6" s="60" t="n"/>
+      <c r="AL6" s="61" t="inlineStr">
+        <is>
+          <t>10.000000%</t>
+        </is>
+      </c>
+      <c r="AM6" s="61" t="inlineStr">
+        <is>
+          <t>5.000000%</t>
+        </is>
+      </c>
+      <c r="AN6" s="61" t="inlineStr">
+        <is>
+          <t>15.000000%</t>
+        </is>
+      </c>
+      <c r="AO6" s="61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AP6" s="60" t="n"/>
+      <c r="AQ6" s="60" t="n"/>
+      <c r="AR6" s="62" t="n"/>
+      <c r="AS6" s="61" t="inlineStr">
+        <is>
+          <t>27-May-2020</t>
+        </is>
+      </c>
+      <c r="AT6" s="61" t="inlineStr">
+        <is>
+          <t>28-Jun-2021</t>
+        </is>
+      </c>
+      <c r="AU6" s="61" t="inlineStr">
+        <is>
+          <t>10,000.00</t>
+        </is>
+      </c>
+      <c r="AV6" s="61" t="inlineStr">
+        <is>
+          <t>25-May-2020</t>
+        </is>
+      </c>
+      <c r="AW6" s="61" t="n"/>
+      <c r="AX6" s="61" t="n"/>
+      <c r="AY6" s="61" t="n"/>
+      <c r="AZ6" s="61" t="n"/>
+      <c r="BA6" s="61" t="n"/>
+      <c r="BB6" s="61" t="n"/>
+      <c r="BC6" s="61" t="n"/>
+      <c r="BD6" s="61" t="n"/>
+      <c r="BE6" s="61" t="n"/>
+      <c r="BF6" s="61" t="n"/>
+      <c r="BG6" s="61" t="n"/>
+      <c r="BH6" s="61" t="n"/>
+      <c r="BI6" s="61" t="n"/>
+      <c r="BJ6" s="73" t="inlineStr">
+        <is>
+          <t>27-Dec-2019</t>
+        </is>
+      </c>
+      <c r="BK6" s="73" t="inlineStr">
+        <is>
+          <t>275,750.00</t>
+        </is>
+      </c>
+      <c r="BL6" s="73" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+      <c r="BM6" s="73" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="BN6" s="73" t="inlineStr">
+        <is>
+          <t>Establishment/Extension Fee</t>
+        </is>
+      </c>
+      <c r="BO6" s="59" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
@@ -4116,8 +4351,8 @@
     <col width="29.42578125" customWidth="1" style="72" min="3" max="3"/>
     <col width="24.28515625" bestFit="1" customWidth="1" style="72" min="4" max="4"/>
     <col width="20.5703125" customWidth="1" style="72" min="5" max="5"/>
-    <col width="8.7109375" customWidth="1" style="72" min="6" max="43"/>
-    <col width="8.7109375" customWidth="1" style="72" min="44" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="6" max="45"/>
+    <col width="8.7109375" customWidth="1" style="72" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4207,8 +4442,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="5" max="5"/>
     <col width="30.140625" customWidth="1" style="72" min="6" max="6"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="7" max="7"/>
-    <col width="8.7109375" customWidth="1" style="72" min="8" max="44"/>
-    <col width="8.7109375" customWidth="1" style="72" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="8" max="46"/>
+    <col width="8.7109375" customWidth="1" style="72" min="47" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4356,8 +4591,8 @@
     <col width="30.140625" bestFit="1" customWidth="1" style="72" min="9" max="9"/>
     <col width="30.140625" customWidth="1" style="72" min="10" max="10"/>
     <col width="24" bestFit="1" customWidth="1" style="72" min="11" max="11"/>
-    <col width="8.7109375" customWidth="1" style="72" min="12" max="48"/>
-    <col width="8.7109375" customWidth="1" style="72" min="49" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="12" max="50"/>
+    <col width="8.7109375" customWidth="1" style="72" min="51" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -4483,8 +4718,8 @@
   </sheetPr>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -4516,8 +4751,8 @@
     <col width="14.5703125" bestFit="1" customWidth="1" style="72" min="28" max="28"/>
     <col width="25.28515625" bestFit="1" customWidth="1" style="72" min="29" max="29"/>
     <col width="14" customWidth="1" style="72" min="30" max="30"/>
-    <col width="8.7109375" customWidth="1" style="72" min="31" max="49"/>
-    <col width="8.7109375" customWidth="1" style="72" min="50" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="72" min="31" max="51"/>
+    <col width="8.7109375" customWidth="1" style="72" min="52" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="71">
@@ -5239,8 +5474,8 @@
     <col width="24" bestFit="1" customWidth="1" style="31" min="44" max="44"/>
     <col width="13.140625" bestFit="1" customWidth="1" style="31" min="45" max="45"/>
     <col width="11.5703125" bestFit="1" customWidth="1" style="31" min="46" max="46"/>
-    <col width="9.140625" customWidth="1" style="31" min="47" max="80"/>
-    <col width="9.140625" customWidth="1" style="31" min="81" max="16384"/>
+    <col width="9.140625" customWidth="1" style="31" min="47" max="82"/>
+    <col width="9.140625" customWidth="1" style="31" min="83" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customFormat="1" customHeight="1" s="22">

</xml_diff>

<commit_message>
GDE-9544 Combine Loan YZ
Added new locator
Add new high level keyword and test suite
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A6A5CC-A4CC-4BD0-9D2A-E1EF46F46ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C937C739-AD0F-4F69-A498-52955BAE5504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="753">
   <si>
     <t>rowid</t>
   </si>
@@ -2229,6 +2229,72 @@
   </si>
   <si>
     <t>Fee_Comment</t>
+  </si>
+  <si>
+    <t>Commitment Change Notice - Revolver Facility</t>
+  </si>
+  <si>
+    <t>;$EOH2X0</t>
+  </si>
+  <si>
+    <t>LIQ-;$EOH2X0-;CEOH1Q8-3</t>
+  </si>
+  <si>
+    <t>2021-02-22 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-02-12 00:00:00.000</t>
+  </si>
+  <si>
+    <t>Commitment Change</t>
+  </si>
+  <si>
+    <t>2021-02-17 18:56:43.269</t>
+  </si>
+  <si>
+    <t>API_COR_CHEDU_REV_COMCNGE</t>
+  </si>
+  <si>
+    <t>TEMP_API_COR__CHEDU_REV_COMCNGE</t>
+  </si>
+  <si>
+    <t>INPUT_API_COR__CHEDU_REV_COMCNGE</t>
+  </si>
+  <si>
+    <t>EXP_API_COR__CHEDU_REV_COMCNGE</t>
+  </si>
+  <si>
+    <t>API_COR_RESPONSE_CHEDU_REV_COMCNGE</t>
+  </si>
+  <si>
+    <t>Combine Outstanding Y &amp; Z</t>
+  </si>
+  <si>
+    <t>36,775,750.00</t>
+  </si>
+  <si>
+    <t>60003092</t>
+  </si>
+  <si>
+    <t>2,006.00</t>
+  </si>
+  <si>
+    <t>260,851.61</t>
+  </si>
+  <si>
+    <t>16-Jun-2020</t>
+  </si>
+  <si>
+    <t>37,038,607.61</t>
+  </si>
+  <si>
+    <t>0.643300%</t>
+  </si>
+  <si>
+    <t>2.643300%</t>
+  </si>
+  <si>
+    <t>InterestCapitalization_Status</t>
   </si>
 </sst>
 </file>
@@ -2472,7 +2538,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2595,6 +2661,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -3507,11 +3577,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO9"/>
+  <dimension ref="A1:BO10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K21" sqref="K21"/>
+      <selection pane="topRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4943,6 +5013,131 @@
       <c r="BA9" s="61"/>
       <c r="BB9" s="61"/>
     </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A10" s="76" t="s">
+        <v>712</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>731</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="67" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" s="63" t="s">
+        <v>426</v>
+      </c>
+      <c r="I10" s="67" t="s">
+        <v>732</v>
+      </c>
+      <c r="J10" s="67" t="s">
+        <v>733</v>
+      </c>
+      <c r="K10" s="67" t="s">
+        <v>734</v>
+      </c>
+      <c r="L10" s="67" t="s">
+        <v>735</v>
+      </c>
+      <c r="M10" s="63">
+        <v>5</v>
+      </c>
+      <c r="N10" s="63" t="s">
+        <v>736</v>
+      </c>
+      <c r="O10" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="P10" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q10" s="67" t="s">
+        <v>737</v>
+      </c>
+      <c r="R10" s="67" t="s">
+        <v>737</v>
+      </c>
+      <c r="S10" s="64" t="s">
+        <v>434</v>
+      </c>
+      <c r="T10" s="64" t="s">
+        <v>694</v>
+      </c>
+      <c r="U10" s="64" t="s">
+        <v>436</v>
+      </c>
+      <c r="V10" s="64" t="s">
+        <v>738</v>
+      </c>
+      <c r="W10" s="81" t="s">
+        <v>739</v>
+      </c>
+      <c r="X10" s="81" t="s">
+        <v>740</v>
+      </c>
+      <c r="Y10" s="81" t="s">
+        <v>741</v>
+      </c>
+      <c r="Z10" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA10" s="81" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB10" s="81" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="81" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE10" s="65"/>
+      <c r="AF10" s="66"/>
+      <c r="AG10" s="60"/>
+      <c r="AH10" s="64" t="s">
+        <v>445</v>
+      </c>
+      <c r="AI10" s="60"/>
+      <c r="AJ10" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK10" s="60"/>
+      <c r="AL10" s="61"/>
+      <c r="AM10" s="61"/>
+      <c r="AN10" s="61"/>
+      <c r="AO10" s="61"/>
+      <c r="AP10" s="60"/>
+      <c r="AQ10" s="60"/>
+      <c r="AR10" s="62"/>
+      <c r="AS10" s="61"/>
+      <c r="AT10" s="61"/>
+      <c r="AU10" s="61"/>
+      <c r="AV10" s="61"/>
+      <c r="AW10" s="61"/>
+      <c r="AX10" s="61"/>
+      <c r="AY10" s="61"/>
+      <c r="AZ10" s="61"/>
+      <c r="BA10" s="61"/>
+      <c r="BB10" s="92"/>
+      <c r="BC10" s="92"/>
+      <c r="BD10" s="92"/>
+      <c r="BE10" s="92"/>
+      <c r="BF10" s="92"/>
+      <c r="BG10" s="92"/>
+      <c r="BH10" s="92"/>
+      <c r="BI10" s="92"/>
+      <c r="BJ10" s="92"/>
+      <c r="BK10" s="92"/>
+      <c r="BL10" s="92"/>
+      <c r="BM10" s="92"/>
+      <c r="BN10" s="92"/>
+      <c r="BO10" s="92"/>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -4954,8 +5149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6182,10 +6377,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6217,11 +6412,12 @@
     <col min="28" max="28" width="14.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="25.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" style="72" customWidth="1"/>
-    <col min="31" max="54" width="8.7109375" style="72" customWidth="1"/>
+    <col min="31" max="31" width="27.42578125" style="72" bestFit="1" customWidth="1"/>
+    <col min="32" max="54" width="8.7109375" style="72" customWidth="1"/>
     <col min="55" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="71" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
@@ -6312,8 +6508,11 @@
       <c r="AD1" s="71" t="s">
         <v>105</v>
       </c>
+      <c r="AE1" s="71" t="s">
+        <v>752</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -6372,8 +6571,9 @@
       <c r="AB2" s="78"/>
       <c r="AC2" s="73"/>
       <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>456</v>
       </c>
@@ -6456,8 +6656,9 @@
         <v>560</v>
       </c>
       <c r="AD3" s="78"/>
+      <c r="AE3" s="78"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>469</v>
       </c>
@@ -6542,8 +6743,9 @@
         <v>560</v>
       </c>
       <c r="AD4" s="78"/>
+      <c r="AE4" s="78"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>482</v>
       </c>
@@ -6625,6 +6827,92 @@
       </c>
       <c r="AD5" s="72" t="s">
         <v>105</v>
+      </c>
+      <c r="AE5" s="78"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>743</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>633</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>542</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>649</v>
+      </c>
+      <c r="G6" s="75" t="s">
+        <v>744</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>745</v>
+      </c>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" s="72" t="s">
+        <v>544</v>
+      </c>
+      <c r="N6" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="O6" s="75" t="s">
+        <v>746</v>
+      </c>
+      <c r="P6" s="75" t="s">
+        <v>747</v>
+      </c>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="75" t="s">
+        <v>748</v>
+      </c>
+      <c r="S6" s="75" t="s">
+        <v>749</v>
+      </c>
+      <c r="T6" s="75" t="s">
+        <v>749</v>
+      </c>
+      <c r="U6" s="75" t="s">
+        <v>749</v>
+      </c>
+      <c r="V6" s="75" t="s">
+        <v>749</v>
+      </c>
+      <c r="W6" s="75" t="s">
+        <v>750</v>
+      </c>
+      <c r="X6" s="37" t="s">
+        <v>546</v>
+      </c>
+      <c r="Y6" s="37" t="s">
+        <v>751</v>
+      </c>
+      <c r="Z6" s="74" t="s">
+        <v>548</v>
+      </c>
+      <c r="AA6" s="72" t="s">
+        <v>549</v>
+      </c>
+      <c r="AB6" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC6" s="72" t="s">
+        <v>540</v>
+      </c>
+      <c r="AD6" s="78"/>
+      <c r="AE6" s="93" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -8603,7 +8891,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GDE-9545 Repricing Intent notice
Updated noticeid locator
Updated test suite and keyword
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C937C739-AD0F-4F69-A498-52955BAE5504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C5AB6-5A15-43E3-A5FF-53EC993C5937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="764">
   <si>
     <t>rowid</t>
   </si>
@@ -2295,6 +2295,39 @@
   </si>
   <si>
     <t>InterestCapitalization_Status</t>
+  </si>
+  <si>
+    <t>Loan Repricing Intent Notice for Rollover Outstanding YZ</t>
+  </si>
+  <si>
+    <t>-TEOL0PB</t>
+  </si>
+  <si>
+    <t>LIQ--TEOL0PB--PEOKZGH-2</t>
+  </si>
+  <si>
+    <t>2021-02-24 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-02-14 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-02-19 13:11:24.243</t>
+  </si>
+  <si>
+    <t>API_COR_CHEDU_YZ_IN</t>
+  </si>
+  <si>
+    <t>TEMP_API_COR__CHEDU_YZ_IN</t>
+  </si>
+  <si>
+    <t>INPUT_API_COR__CHEDU_YZ_IN</t>
+  </si>
+  <si>
+    <t>EXP_API_COR__CHEDU_YZ_IN</t>
+  </si>
+  <si>
+    <t>API_COR_RESPONSE__CHEDU_YZ_IN</t>
   </si>
 </sst>
 </file>
@@ -3577,11 +3610,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO10"/>
+  <dimension ref="A1:BO11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E21" sqref="E21"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5138,6 +5171,131 @@
       <c r="BN10" s="92"/>
       <c r="BO10" s="92"/>
     </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>753</v>
+      </c>
+      <c r="C11" s="61"/>
+      <c r="D11" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="67" t="s">
+        <v>425</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>426</v>
+      </c>
+      <c r="I11" s="67" t="s">
+        <v>754</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>755</v>
+      </c>
+      <c r="K11" s="67" t="s">
+        <v>756</v>
+      </c>
+      <c r="L11" s="67" t="s">
+        <v>757</v>
+      </c>
+      <c r="M11" s="63">
+        <v>5</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>475</v>
+      </c>
+      <c r="O11" s="64" t="s">
+        <v>432</v>
+      </c>
+      <c r="P11" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" s="74" t="s">
+        <v>758</v>
+      </c>
+      <c r="R11" s="74" t="s">
+        <v>758</v>
+      </c>
+      <c r="S11" s="64" t="s">
+        <v>434</v>
+      </c>
+      <c r="T11" s="64" t="s">
+        <v>694</v>
+      </c>
+      <c r="U11" s="64" t="s">
+        <v>436</v>
+      </c>
+      <c r="V11" s="64" t="s">
+        <v>759</v>
+      </c>
+      <c r="W11" s="81" t="s">
+        <v>760</v>
+      </c>
+      <c r="X11" s="81" t="s">
+        <v>761</v>
+      </c>
+      <c r="Y11" s="81" t="s">
+        <v>762</v>
+      </c>
+      <c r="Z11" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="AA11" s="81" t="s">
+        <v>442</v>
+      </c>
+      <c r="AB11" s="81" t="s">
+        <v>763</v>
+      </c>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="81" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE11" s="65"/>
+      <c r="AF11" s="66"/>
+      <c r="AG11" s="60"/>
+      <c r="AH11" s="64" t="s">
+        <v>445</v>
+      </c>
+      <c r="AI11" s="60"/>
+      <c r="AJ11" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="AK11" s="60"/>
+      <c r="AL11" s="61"/>
+      <c r="AM11" s="61"/>
+      <c r="AN11" s="61"/>
+      <c r="AO11" s="61"/>
+      <c r="AP11" s="60"/>
+      <c r="AQ11" s="60"/>
+      <c r="AR11" s="62"/>
+      <c r="AS11" s="61"/>
+      <c r="AT11" s="61"/>
+      <c r="AU11" s="61"/>
+      <c r="AV11" s="61"/>
+      <c r="AW11" s="61"/>
+      <c r="AX11" s="61"/>
+      <c r="AY11" s="61"/>
+      <c r="AZ11" s="61"/>
+      <c r="BA11" s="61"/>
+      <c r="BB11" s="61"/>
+      <c r="BC11" s="61"/>
+      <c r="BD11" s="61"/>
+      <c r="BE11" s="61"/>
+      <c r="BF11" s="61"/>
+      <c r="BG11" s="61"/>
+      <c r="BH11" s="61"/>
+      <c r="BI11" s="61"/>
+      <c r="BJ11" s="61"/>
+      <c r="BK11" s="61"/>
+      <c r="BL11" s="61"/>
+      <c r="BM11" s="61"/>
+      <c r="BN11" s="61"/>
+      <c r="BO11" s="61"/>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -6379,7 +6537,7 @@
   </sheetPr>
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -7498,8 +7656,8 @@
   </sheetPr>
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9059,12 +9217,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9182,15 +9337,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35928E82-1B5C-4072-91D4-469BBF0DE967}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14162CA4-C7CC-4D04-ACED-BB502ABB2A36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9212,10 +9371,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14162CA4-C7CC-4D04-ACED-BB502ABB2A36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35928E82-1B5C-4072-91D4-469BBF0DE967}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GDE-9557 Rate setting notice
Updated test suites and data sets
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2E3FFF-0459-44F1-884D-B05C73EA99D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FE897E-1A18-4963-B62A-48DF0F2DFD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="842">
   <si>
     <t>rowid</t>
   </si>
@@ -1872,6 +1872,33 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>Loan Repricing Rate Setting Notice for Rollover Outstanding W</t>
+  </si>
+  <si>
+    <t>H;EOZJNJ</t>
+  </si>
+  <si>
+    <t>LIQ-H;EOZJNJ-HEEOZHQP-2</t>
+  </si>
+  <si>
+    <t>2021-03-02 16:54:41.567</t>
+  </si>
+  <si>
+    <t>API_COR_CHEDU_W_RSN</t>
+  </si>
+  <si>
+    <t>TEMP_API_COR__CHEDU_W_RSN</t>
+  </si>
+  <si>
+    <t>INPUT_API_COR__CHEDU_W_RSN</t>
+  </si>
+  <si>
+    <t>EXP_API_COR__CHEDU_W_RSN</t>
+  </si>
+  <si>
+    <t>API_COR_RESPONSE__CHEDU_W_RSN</t>
   </si>
   <si>
     <t>16</t>
@@ -3828,7 +3855,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <selection pane="topRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,8 +3925,8 @@
     <col min="65" max="65" width="9.7109375" style="52" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="26" style="52" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="36.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="68" max="160" width="9.140625" style="52" customWidth="1"/>
-    <col min="161" max="16384" width="9.140625" style="52"/>
+    <col min="68" max="161" width="9.140625" style="52" customWidth="1"/>
+    <col min="162" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6095,10 +6122,132 @@
       <c r="A16" s="76" t="s">
         <v>611</v>
       </c>
+      <c r="B16" s="53" t="s">
+        <v>612</v>
+      </c>
+      <c r="C16" s="61"/>
+      <c r="D16" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="67" t="s">
+        <v>422</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>423</v>
+      </c>
+      <c r="I16" s="67" t="s">
+        <v>613</v>
+      </c>
+      <c r="J16" s="67" t="s">
+        <v>614</v>
+      </c>
+      <c r="K16" s="67" t="s">
+        <v>603</v>
+      </c>
+      <c r="L16" s="67" t="s">
+        <v>604</v>
+      </c>
+      <c r="M16" s="63">
+        <v>5</v>
+      </c>
+      <c r="N16" s="63" t="s">
+        <v>485</v>
+      </c>
+      <c r="O16" s="64" t="s">
+        <v>429</v>
+      </c>
+      <c r="P16" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q16" s="67" t="s">
+        <v>615</v>
+      </c>
+      <c r="R16" s="67" t="s">
+        <v>615</v>
+      </c>
+      <c r="S16" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="T16" s="64" t="s">
+        <v>524</v>
+      </c>
+      <c r="U16" s="64" t="s">
+        <v>433</v>
+      </c>
+      <c r="V16" s="64" t="s">
+        <v>616</v>
+      </c>
+      <c r="W16" s="81" t="s">
+        <v>617</v>
+      </c>
+      <c r="X16" s="81" t="s">
+        <v>618</v>
+      </c>
+      <c r="Y16" s="81" t="s">
+        <v>619</v>
+      </c>
+      <c r="Z16" s="81" t="s">
+        <v>438</v>
+      </c>
+      <c r="AA16" s="81" t="s">
+        <v>439</v>
+      </c>
+      <c r="AB16" s="81" t="s">
+        <v>620</v>
+      </c>
+      <c r="AC16" s="60"/>
+      <c r="AD16" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="AE16" s="65"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="60"/>
+      <c r="AH16" s="64" t="s">
+        <v>442</v>
+      </c>
+      <c r="AI16" s="60"/>
+      <c r="AJ16" s="63" t="s">
+        <v>443</v>
+      </c>
+      <c r="AK16" s="60"/>
+      <c r="AL16" s="61"/>
+      <c r="AM16" s="61"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="61"/>
+      <c r="AP16" s="60"/>
+      <c r="AQ16" s="60"/>
+      <c r="AR16" s="62"/>
+      <c r="AS16" s="61"/>
+      <c r="AT16" s="61"/>
+      <c r="AU16" s="61"/>
+      <c r="AV16" s="61"/>
+      <c r="AW16" s="61"/>
+      <c r="AX16" s="61"/>
+      <c r="AY16" s="61"/>
+      <c r="AZ16" s="61"/>
+      <c r="BA16" s="61"/>
+      <c r="BB16" s="61"/>
+      <c r="BC16" s="61"/>
+      <c r="BD16" s="61"/>
+      <c r="BE16" s="61"/>
+      <c r="BF16" s="61"/>
+      <c r="BG16" s="61"/>
+      <c r="BH16" s="61"/>
+      <c r="BI16" s="61"/>
+      <c r="BJ16" s="61"/>
+      <c r="BK16" s="61"/>
+      <c r="BL16" s="61"/>
+      <c r="BM16" s="61"/>
+      <c r="BN16" s="61"/>
+      <c r="BO16" s="59" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
-        <v>612</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -6159,16 +6308,16 @@
         <v>362</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="E1" s="68" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="F1" s="68" t="s">
-        <v>615</v>
+        <v>624</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
       <c r="H1" s="68" t="s">
         <v>400</v>
@@ -6177,13 +6326,13 @@
         <v>401</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="K1" s="68" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="M1" s="68" t="s">
         <v>404</v>
@@ -6195,43 +6344,43 @@
         <v>343</v>
       </c>
       <c r="P1" s="68" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="Q1" s="68" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="R1" s="68" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="S1" s="68" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
       <c r="T1" s="68" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="U1" s="68" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="V1" s="68" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="W1" s="68" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="X1" s="68" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="Y1" s="68" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="Z1" s="68" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="AA1" s="68" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="AB1" s="68" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -6239,7 +6388,7 @@
         <v>72</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="C2" s="93">
         <v>60002878</v>
@@ -6263,25 +6412,25 @@
         <v>217</v>
       </c>
       <c r="J2" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="K2" t="s">
         <v>105</v>
       </c>
       <c r="L2" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="N2" t="s">
         <v>354</v>
       </c>
       <c r="O2" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="P2" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q2" s="37" t="s">
         <v>350</v>
@@ -6296,19 +6445,19 @@
         <v>350</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="V2" s="37" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="X2" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y2" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="Z2" t="s">
         <v>105</v>
@@ -6321,7 +6470,7 @@
         <v>453</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
       <c r="C3" s="93">
         <v>60002979</v>
@@ -6336,61 +6485,61 @@
         <v>113</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="I3" s="37" t="s">
         <v>217</v>
       </c>
       <c r="J3" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="K3" t="s">
         <v>105</v>
       </c>
       <c r="L3" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="N3" s="73"/>
       <c r="O3" s="73"/>
       <c r="P3" s="73"/>
       <c r="Q3" s="37" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="R3" s="37" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="T3" s="37" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="U3" s="37" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="V3" s="37" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="W3" s="37" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="X3" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y3" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="Z3" t="s">
         <v>105</v>
       </c>
       <c r="AA3" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="AB3" s="73"/>
     </row>
@@ -6399,10 +6548,10 @@
         <v>466</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="C4" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
       <c r="D4" t="s">
         <v>218</v>
@@ -6414,57 +6563,57 @@
         <v>113</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="I4" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J4" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="K4" t="s">
         <v>105</v>
       </c>
       <c r="L4" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="N4" s="73"/>
       <c r="O4" s="73"/>
       <c r="P4" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q4" s="37" t="s">
+        <v>660</v>
+      </c>
+      <c r="R4" s="37" t="s">
+        <v>660</v>
+      </c>
+      <c r="S4" s="37" t="s">
+        <v>660</v>
+      </c>
+      <c r="T4" s="37" t="s">
+        <v>660</v>
+      </c>
+      <c r="U4" s="37" t="s">
+        <v>664</v>
+      </c>
+      <c r="V4" s="37" t="s">
+        <v>665</v>
+      </c>
+      <c r="W4" s="37" t="s">
+        <v>666</v>
+      </c>
+      <c r="X4" t="s">
         <v>651</v>
       </c>
-      <c r="R4" s="37" t="s">
-        <v>651</v>
-      </c>
-      <c r="S4" s="37" t="s">
-        <v>651</v>
-      </c>
-      <c r="T4" s="37" t="s">
-        <v>651</v>
-      </c>
-      <c r="U4" s="37" t="s">
-        <v>655</v>
-      </c>
-      <c r="V4" s="37" t="s">
-        <v>656</v>
-      </c>
-      <c r="W4" s="37" t="s">
-        <v>657</v>
-      </c>
-      <c r="X4" t="s">
-        <v>642</v>
-      </c>
       <c r="Y4" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="Z4" t="s">
         <v>105</v>
@@ -6477,10 +6626,10 @@
         <v>479</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>659</v>
+        <v>668</v>
       </c>
       <c r="C5" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="D5" t="s">
         <v>218</v>
@@ -6492,57 +6641,57 @@
         <v>113</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J5" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="K5" t="s">
         <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="N5" s="73"/>
       <c r="O5" s="73"/>
       <c r="P5" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="R5" s="37" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="S5" s="37" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="T5" s="37" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="U5" s="37" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="V5" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="W5" s="37" t="s">
-        <v>663</v>
+        <v>672</v>
       </c>
       <c r="X5" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y5" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="Z5" t="s">
         <v>105</v>
@@ -6555,10 +6704,10 @@
         <v>492</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>664</v>
+        <v>673</v>
       </c>
       <c r="C6" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="D6" t="s">
         <v>218</v>
@@ -6570,57 +6719,57 @@
         <v>113</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
       <c r="I6" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J6" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="K6" t="s">
         <v>105</v>
       </c>
       <c r="L6" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="N6" s="73"/>
       <c r="O6" s="73"/>
       <c r="P6" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q6" s="37" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="R6" s="37" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="S6" s="37" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="T6" s="37" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="U6" s="37" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="V6" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="W6" s="37" t="s">
-        <v>670</v>
+        <v>679</v>
       </c>
       <c r="X6" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y6" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="Z6" t="s">
         <v>105</v>
@@ -6633,10 +6782,10 @@
         <v>504</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="C7" t="s">
-        <v>672</v>
+        <v>681</v>
       </c>
       <c r="D7" t="s">
         <v>218</v>
@@ -6648,57 +6797,57 @@
         <v>113</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="I7" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J7" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="K7" t="s">
         <v>105</v>
       </c>
       <c r="L7" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="N7" s="73"/>
       <c r="O7" s="73"/>
       <c r="P7" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q7" s="37" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="R7" s="37" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="T7" s="37" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="V7" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="W7" s="37" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="X7" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y7" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="Z7" t="s">
         <v>105</v>
@@ -6711,10 +6860,10 @@
         <v>516</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="C8" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="D8" t="s">
         <v>218</v>
@@ -6726,57 +6875,57 @@
         <v>113</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="I8" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J8" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="K8" t="s">
         <v>105</v>
       </c>
       <c r="L8" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="N8" s="73"/>
       <c r="O8" s="73"/>
       <c r="P8" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q8" s="37" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="S8" s="37" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="T8" s="37" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="U8" s="37" t="s">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="V8" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="W8" s="37" t="s">
-        <v>682</v>
+        <v>691</v>
       </c>
       <c r="X8" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y8" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="Z8" t="s">
         <v>105</v>
@@ -6789,10 +6938,10 @@
         <v>530</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="C9" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="D9" t="s">
         <v>218</v>
@@ -6804,57 +6953,57 @@
         <v>113</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="I9" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J9" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="K9" t="s">
         <v>105</v>
       </c>
       <c r="L9" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
       <c r="P9" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q9" s="37" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="S9" s="37" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="T9" s="37" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="U9" s="37" t="s">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="V9" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="W9" s="37" t="s">
-        <v>682</v>
+        <v>691</v>
       </c>
       <c r="X9" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y9" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="Z9" t="s">
         <v>105</v>
@@ -6867,10 +7016,10 @@
         <v>541</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>687</v>
+        <v>696</v>
       </c>
       <c r="C10" s="83" t="s">
-        <v>688</v>
+        <v>697</v>
       </c>
       <c r="D10" t="s">
         <v>218</v>
@@ -6882,7 +7031,7 @@
         <v>113</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="H10" s="37" t="s">
         <v>247</v>
@@ -6891,52 +7040,52 @@
         <v>217</v>
       </c>
       <c r="J10" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="K10" t="s">
         <v>105</v>
       </c>
       <c r="L10" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="N10" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="O10" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="P10" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="S10" s="37" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="U10" s="37" t="s">
-        <v>692</v>
+        <v>701</v>
       </c>
       <c r="V10" s="37" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="W10" s="37" t="s">
-        <v>693</v>
+        <v>702</v>
       </c>
       <c r="X10" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="Y10" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="Z10" t="s">
         <v>105</v>
@@ -6970,8 +7119,8 @@
     <col min="3" max="3" width="29.42578125" style="72" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="72" customWidth="1"/>
-    <col min="6" max="54" width="8.7109375" style="72" customWidth="1"/>
-    <col min="55" max="16384" width="8.7109375" style="72"/>
+    <col min="6" max="55" width="8.7109375" style="72" customWidth="1"/>
+    <col min="56" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -6982,13 +7131,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>694</v>
+        <v>703</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>695</v>
+        <v>704</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>696</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6996,16 +7145,16 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="C2" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7039,8 +7188,8 @@
     <col min="5" max="5" width="30.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" style="72" customWidth="1"/>
     <col min="7" max="7" width="24" style="72" bestFit="1" customWidth="1"/>
-    <col min="8" max="55" width="8.7109375" style="72" customWidth="1"/>
-    <col min="56" max="16384" width="8.7109375" style="72"/>
+    <col min="8" max="56" width="8.7109375" style="72" customWidth="1"/>
+    <col min="57" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7051,16 +7200,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>700</v>
+        <v>709</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>701</v>
+        <v>710</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="G1" s="71" t="s">
         <v>164</v>
@@ -7071,19 +7220,19 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="C2" t="s">
         <v>189</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>706</v>
+        <v>715</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="G2" s="75" t="s">
         <v>250</v>
@@ -7094,22 +7243,22 @@
         <v>453</v>
       </c>
       <c r="B3" t="s">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="C3" t="s">
         <v>189</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>709</v>
+        <v>718</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>706</v>
+        <v>715</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7158,8 +7307,8 @@
     <col min="20" max="20" width="22.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22.7109375" style="72" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27.42578125" style="72" bestFit="1" customWidth="1"/>
-    <col min="23" max="59" width="8.7109375" style="72" customWidth="1"/>
-    <col min="60" max="16384" width="8.7109375" style="72"/>
+    <col min="23" max="60" width="8.7109375" style="72" customWidth="1"/>
+    <col min="61" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7173,34 +7322,34 @@
         <v>339</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>710</v>
+        <v>719</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>714</v>
+        <v>723</v>
       </c>
       <c r="I1" s="71" t="s">
         <v>417</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>717</v>
+        <v>726</v>
       </c>
       <c r="M1" s="71" t="s">
-        <v>718</v>
+        <v>727</v>
       </c>
       <c r="N1" s="71" t="s">
         <v>342</v>
@@ -7212,10 +7361,10 @@
         <v>346</v>
       </c>
       <c r="Q1" s="71" t="s">
-        <v>719</v>
+        <v>728</v>
       </c>
       <c r="R1" s="71" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
       <c r="S1" s="89" t="s">
         <v>347</v>
@@ -7224,10 +7373,10 @@
         <v>348</v>
       </c>
       <c r="U1" s="71" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -7235,7 +7384,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="C2" t="s">
         <v>187</v>
@@ -7253,13 +7402,13 @@
         <v>248</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>248</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="K2" s="90"/>
       <c r="L2" s="91"/>
@@ -7279,7 +7428,7 @@
         <v>453</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="C3" s="72" t="s">
         <v>186</v>
@@ -7297,37 +7446,37 @@
         <v>248</v>
       </c>
       <c r="H3" s="85" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="I3" s="75" t="s">
         <v>248</v>
       </c>
       <c r="J3" s="85" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="K3" s="85" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="L3" s="85" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="M3" s="85" t="s">
         <v>447</v>
       </c>
       <c r="N3" s="72" t="s">
-        <v>725</v>
+        <v>734</v>
       </c>
       <c r="O3" s="72" t="s">
-        <v>726</v>
+        <v>735</v>
       </c>
       <c r="P3" t="s">
         <v>358</v>
       </c>
       <c r="Q3" s="85" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="R3" s="86" t="s">
-        <v>727</v>
+        <v>736</v>
       </c>
       <c r="S3" s="87" t="s">
         <v>359</v>
@@ -7336,7 +7485,7 @@
         <v>357</v>
       </c>
       <c r="U3" s="72" t="s">
-        <v>725</v>
+        <v>734</v>
       </c>
       <c r="V3" s="91"/>
     </row>
@@ -7345,7 +7494,7 @@
         <v>466</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="C4" s="72" t="s">
         <v>186</v>
@@ -7357,34 +7506,34 @@
         <v>247</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>728</v>
+        <v>737</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="H4" s="85" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="I4" s="75" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="J4" s="85" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="K4" s="85" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="L4" s="85" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="M4" s="85" t="s">
         <v>447</v>
       </c>
       <c r="N4" s="72" t="s">
-        <v>730</v>
+        <v>739</v>
       </c>
       <c r="O4" s="72" t="s">
-        <v>731</v>
+        <v>740</v>
       </c>
       <c r="P4" s="91"/>
       <c r="Q4" s="91"/>
@@ -7403,7 +7552,7 @@
       <c r="D5" s="84"/>
       <c r="F5" s="75"/>
       <c r="R5" s="88" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
     </row>
   </sheetData>
@@ -7457,8 +7606,8 @@
     <col min="33" max="34" width="23.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="78.140625" style="72" bestFit="1" customWidth="1"/>
-    <col min="37" max="60" width="8.7109375" style="72" customWidth="1"/>
-    <col min="61" max="16384" width="8.7109375" style="72"/>
+    <col min="37" max="61" width="8.7109375" style="72" customWidth="1"/>
+    <col min="62" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7469,100 +7618,100 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>733</v>
+        <v>742</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>734</v>
+        <v>743</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>417</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>735</v>
+        <v>744</v>
       </c>
       <c r="G1" s="77" t="s">
-        <v>736</v>
+        <v>745</v>
       </c>
       <c r="H1" s="77" t="s">
-        <v>737</v>
+        <v>746</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>738</v>
+        <v>747</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>739</v>
+        <v>748</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="L1" s="68" t="s">
+        <v>639</v>
+      </c>
+      <c r="M1" s="71" t="s">
+        <v>629</v>
+      </c>
+      <c r="N1" s="68" t="s">
+        <v>622</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>750</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>751</v>
+      </c>
+      <c r="Q1" s="71" t="s">
+        <v>752</v>
+      </c>
+      <c r="R1" s="71" t="s">
+        <v>753</v>
+      </c>
+      <c r="S1" s="68" t="s">
         <v>630</v>
       </c>
-      <c r="M1" s="71" t="s">
-        <v>620</v>
-      </c>
-      <c r="N1" s="68" t="s">
-        <v>613</v>
-      </c>
-      <c r="O1" s="71" t="s">
-        <v>741</v>
-      </c>
-      <c r="P1" s="71" t="s">
-        <v>742</v>
-      </c>
-      <c r="Q1" s="71" t="s">
-        <v>743</v>
-      </c>
-      <c r="R1" s="71" t="s">
-        <v>744</v>
-      </c>
-      <c r="S1" s="68" t="s">
-        <v>621</v>
-      </c>
       <c r="T1" s="68" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="U1" s="68" t="s">
+        <v>632</v>
+      </c>
+      <c r="V1" s="68" t="s">
+        <v>633</v>
+      </c>
+      <c r="W1" s="68" t="s">
+        <v>634</v>
+      </c>
+      <c r="X1" s="68" t="s">
+        <v>635</v>
+      </c>
+      <c r="Y1" s="68" t="s">
+        <v>636</v>
+      </c>
+      <c r="Z1" s="68" t="s">
+        <v>637</v>
+      </c>
+      <c r="AA1" s="68" t="s">
+        <v>638</v>
+      </c>
+      <c r="AB1" s="68" t="s">
         <v>623</v>
       </c>
-      <c r="V1" s="68" t="s">
-        <v>624</v>
-      </c>
-      <c r="W1" s="68" t="s">
-        <v>625</v>
-      </c>
-      <c r="X1" s="68" t="s">
+      <c r="AC1" s="68" t="s">
         <v>626</v>
-      </c>
-      <c r="Y1" s="68" t="s">
-        <v>627</v>
-      </c>
-      <c r="Z1" s="68" t="s">
-        <v>628</v>
-      </c>
-      <c r="AA1" s="68" t="s">
-        <v>629</v>
-      </c>
-      <c r="AB1" s="68" t="s">
-        <v>614</v>
-      </c>
-      <c r="AC1" s="68" t="s">
-        <v>617</v>
       </c>
       <c r="AD1" s="71" t="s">
         <v>105</v>
       </c>
       <c r="AE1" s="71" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="AF1" s="71" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="AG1" s="71" t="s">
-        <v>746</v>
+        <v>755</v>
       </c>
       <c r="AH1" s="71" t="s">
-        <v>747</v>
+        <v>756</v>
       </c>
       <c r="AI1" s="71" t="s">
         <v>342</v>
@@ -7576,40 +7725,40 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>748</v>
+        <v>757</v>
       </c>
       <c r="C2" t="s">
         <v>218</v>
       </c>
       <c r="D2" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="G2" s="75" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>752</v>
+        <v>761</v>
       </c>
       <c r="I2" s="79" t="s">
-        <v>753</v>
+        <v>762</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="K2" s="75" t="s">
-        <v>755</v>
+        <v>764</v>
       </c>
       <c r="L2" t="s">
         <v>105</v>
       </c>
       <c r="M2" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N2" t="s">
         <v>218</v>
@@ -7639,28 +7788,28 @@
         <v>453</v>
       </c>
       <c r="B3" t="s">
-        <v>756</v>
+        <v>765</v>
       </c>
       <c r="C3" t="s">
         <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E3" s="75" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="F3" s="75" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="I3" s="79" t="s">
-        <v>759</v>
+        <v>768</v>
       </c>
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
@@ -7668,53 +7817,53 @@
         <v>105</v>
       </c>
       <c r="M3" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N3" t="s">
         <v>218</v>
       </c>
       <c r="O3" s="75" t="s">
-        <v>760</v>
+        <v>769</v>
       </c>
       <c r="P3" s="75" t="s">
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="Q3" s="79"/>
       <c r="R3" s="75" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="S3" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="T3" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="U3" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="W3" s="75" t="s">
-        <v>762</v>
+        <v>771</v>
       </c>
       <c r="X3" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="Y3" s="37" t="s">
-        <v>763</v>
+        <v>772</v>
       </c>
       <c r="Z3" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA3" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="AB3" t="s">
         <v>177</v>
       </c>
       <c r="AC3" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="AD3" s="78"/>
       <c r="AE3" s="78"/>
@@ -7726,28 +7875,28 @@
         <v>466</v>
       </c>
       <c r="B4" t="s">
-        <v>764</v>
+        <v>773</v>
       </c>
       <c r="C4" t="s">
         <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="F4" s="80" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="H4" s="75" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="I4" s="79" t="s">
-        <v>768</v>
+        <v>777</v>
       </c>
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
@@ -7755,55 +7904,55 @@
         <v>105</v>
       </c>
       <c r="M4" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N4" t="s">
         <v>218</v>
       </c>
       <c r="O4" s="75" t="s">
-        <v>769</v>
+        <v>778</v>
       </c>
       <c r="P4" s="75" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="Q4" s="75" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="R4" s="75" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="S4" s="75" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="T4" s="75" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="U4" s="75" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="V4" s="75" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="W4" s="75" t="s">
-        <v>773</v>
+        <v>782</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="Z4" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA4" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="AB4" t="s">
         <v>177</v>
       </c>
       <c r="AC4" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="AD4" s="78"/>
       <c r="AE4" s="78"/>
@@ -7815,25 +7964,25 @@
         <v>479</v>
       </c>
       <c r="B5" t="s">
-        <v>775</v>
+        <v>784</v>
       </c>
       <c r="C5" t="s">
         <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="G5" s="80" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>776</v>
+        <v>785</v>
       </c>
       <c r="I5" s="75" t="s">
         <v>105</v>
@@ -7844,51 +7993,51 @@
         <v>105</v>
       </c>
       <c r="M5" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N5" t="s">
         <v>218</v>
       </c>
       <c r="O5" s="75" t="s">
-        <v>777</v>
+        <v>786</v>
       </c>
       <c r="P5" s="79"/>
       <c r="Q5" s="79"/>
       <c r="R5" s="75" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="S5" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="T5" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="U5" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="V5" s="75" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="W5" s="75" t="s">
-        <v>773</v>
+        <v>782</v>
       </c>
       <c r="X5" s="37" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="Z5" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA5" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="AB5" t="s">
         <v>177</v>
       </c>
       <c r="AC5" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="AD5" s="72" t="s">
         <v>105</v>
@@ -7902,25 +8051,25 @@
         <v>492</v>
       </c>
       <c r="B6" s="72" t="s">
-        <v>778</v>
+        <v>787</v>
       </c>
       <c r="C6" t="s">
         <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E6" s="75" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="F6" s="75" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>779</v>
+        <v>788</v>
       </c>
       <c r="H6" t="s">
-        <v>780</v>
+        <v>789</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
@@ -7929,53 +8078,53 @@
         <v>105</v>
       </c>
       <c r="M6" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N6" t="s">
         <v>218</v>
       </c>
       <c r="O6" s="75" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="P6" s="75" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="Q6" s="79"/>
       <c r="R6" s="75" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="S6" s="75" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="T6" s="75" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="U6" s="75" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="V6" s="75" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="W6" s="75" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="X6" s="37" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="Y6" s="37" t="s">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="Z6" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA6" s="72" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="AB6" t="s">
         <v>177</v>
       </c>
       <c r="AC6" s="72" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="AD6" s="78"/>
       <c r="AE6" s="92" t="s">
@@ -7989,25 +8138,25 @@
         <v>504</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="H7" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="I7" s="72" t="s">
         <v>105</v>
@@ -8018,58 +8167,58 @@
         <v>105</v>
       </c>
       <c r="M7" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="O7" s="75" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="P7" s="78"/>
       <c r="Q7" s="78"/>
       <c r="R7" s="75" t="s">
-        <v>791</v>
+        <v>800</v>
       </c>
       <c r="S7" s="95" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="T7" s="95" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="U7" s="95" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="V7" s="95" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="W7" s="75" t="s">
-        <v>792</v>
+        <v>801</v>
       </c>
       <c r="X7" s="37" t="s">
-        <v>793</v>
+        <v>802</v>
       </c>
       <c r="Y7" s="37" t="s">
-        <v>794</v>
+        <v>803</v>
       </c>
       <c r="Z7" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA7" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="AB7" t="s">
         <v>177</v>
       </c>
       <c r="AC7" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="AD7" s="72" t="s">
         <v>105</v>
       </c>
       <c r="AE7" s="78"/>
       <c r="AF7" s="75" t="s">
-        <v>795</v>
+        <v>804</v>
       </c>
       <c r="AG7" s="72" t="s">
         <v>118</v>
@@ -8085,25 +8234,25 @@
         <v>516</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="C8" s="72" t="s">
         <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="H8" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
       <c r="I8" s="72" t="s">
         <v>105</v>
@@ -8114,51 +8263,51 @@
         <v>105</v>
       </c>
       <c r="M8" s="72" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="N8" s="72" t="s">
         <v>218</v>
       </c>
       <c r="O8" s="75" t="s">
-        <v>799</v>
+        <v>808</v>
       </c>
       <c r="P8" s="78"/>
       <c r="Q8" s="78"/>
       <c r="R8" s="75" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="S8" s="95" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="T8" s="95" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="U8" s="95" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="V8" s="95" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="W8" s="75" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="X8" s="37" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="Y8" s="37" t="s">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="Z8" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="AA8" s="72" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="AB8" t="s">
         <v>177</v>
       </c>
       <c r="AC8" s="72" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="AD8" s="78"/>
       <c r="AE8" s="78"/>
@@ -8166,10 +8315,10 @@
       <c r="AG8" s="78"/>
       <c r="AH8" s="78"/>
       <c r="AI8" s="72" t="s">
-        <v>804</v>
+        <v>813</v>
       </c>
       <c r="AJ8" s="72" t="s">
-        <v>805</v>
+        <v>814</v>
       </c>
     </row>
   </sheetData>
@@ -8218,8 +8367,8 @@
     <col min="28" max="28" width="14.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="25.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" style="72" customWidth="1"/>
-    <col min="31" max="60" width="8.7109375" style="72" customWidth="1"/>
-    <col min="61" max="16384" width="8.7109375" style="72"/>
+    <col min="31" max="61" width="8.7109375" style="72" customWidth="1"/>
+    <col min="62" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -8230,25 +8379,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>808</v>
+        <v>817</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>809</v>
+        <v>818</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>810</v>
+        <v>819</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>811</v>
+        <v>820</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>812</v>
+        <v>821</v>
       </c>
       <c r="L1" s="68"/>
       <c r="N1" s="68"/>
@@ -8269,19 +8418,19 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>813</v>
+        <v>822</v>
       </c>
       <c r="C2" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>815</v>
+        <v>824</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>816</v>
+        <v>825</v>
       </c>
       <c r="G2" s="75">
         <v>1</v>
@@ -8312,22 +8461,22 @@
         <v>453</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="75" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="F3" s="78"/>
       <c r="G3" s="75">
         <v>1</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
       <c r="I3" s="75" t="s">
-        <v>819</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -8405,8 +8554,8 @@
     <col min="54" max="54" width="12.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="55" max="56" width="18.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="57" max="58" width="17.5703125" style="72" bestFit="1" customWidth="1"/>
-    <col min="59" max="64" width="8.7109375" style="72" customWidth="1"/>
-    <col min="65" max="16384" width="8.7109375" style="72"/>
+    <col min="59" max="65" width="8.7109375" style="72" customWidth="1"/>
+    <col min="66" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -8417,13 +8566,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>822</v>
+        <v>831</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>223</v>
@@ -8567,10 +8716,10 @@
         <v>302</v>
       </c>
       <c r="BA1" s="71" t="s">
-        <v>823</v>
+        <v>832</v>
       </c>
       <c r="BB1" s="71" t="s">
-        <v>824</v>
+        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:58" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8578,16 +8727,16 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="E2" s="82" t="s">
-        <v>826</v>
+        <v>835</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>240</v>
@@ -8632,7 +8781,7 @@
         <v>308</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
       <c r="U2" t="s">
         <v>109</v>
@@ -8659,7 +8808,7 @@
         <v>308</v>
       </c>
       <c r="AC2" s="44" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
       <c r="AD2" t="s">
         <v>312</v>
@@ -8695,7 +8844,7 @@
         <v>313</v>
       </c>
       <c r="AO2" s="44" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
       <c r="AP2" t="s">
         <v>109</v>
@@ -8728,13 +8877,13 @@
         <v>313</v>
       </c>
       <c r="AZ2" s="44" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
       <c r="BA2" s="72" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="BB2" s="75" t="s">
-        <v>793</v>
+        <v>802</v>
       </c>
       <c r="BC2" s="75"/>
       <c r="BD2" s="75"/>
@@ -8754,8 +8903,8 @@
   </sheetPr>
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8806,8 +8955,8 @@
     <col min="44" max="44" width="24" style="31" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="47" max="91" width="9.140625" style="31" customWidth="1"/>
-    <col min="92" max="16384" width="9.140625" style="31"/>
+    <col min="47" max="92" width="9.140625" style="31" customWidth="1"/>
+    <col min="93" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8964,10 +9113,10 @@
         <v>169</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>113</v>
@@ -9152,8 +9301,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9249,7 +9398,7 @@
         <v>212</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>213</v>

</xml_diff>

<commit_message>
GDE-9558 Fee Payment Notice
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_CH_EDU_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FE897E-1A18-4963-B62A-48DF0F2DFD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA1F1A0-AD54-46CA-B4F7-775CF5E7AF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="853">
   <si>
     <t>rowid</t>
   </si>
@@ -1904,6 +1904,36 @@
     <t>16</t>
   </si>
   <si>
+    <t>HUEOZGF3</t>
+  </si>
+  <si>
+    <t>LIQ-HUEOZGF3-HUEOZG9G-2</t>
+  </si>
+  <si>
+    <t>2021-03-08 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-02-26 00:00:00.000</t>
+  </si>
+  <si>
+    <t>2021-03-03 18:13:54.186</t>
+  </si>
+  <si>
+    <t>API_COR_CHEDU_CFEE_IN</t>
+  </si>
+  <si>
+    <t>TEMP_API_COR_CHEDU_CFEE_IN</t>
+  </si>
+  <si>
+    <t>INPUT_API_COR_CHEDU_CFEE_IN</t>
+  </si>
+  <si>
+    <t>EXP_API_COR_CHEDU_CFEE_IN</t>
+  </si>
+  <si>
+    <t>API_COR_RESPONSE_CHEDU_CFEE_IN</t>
+  </si>
+  <si>
     <t>Outstanding_Type</t>
   </si>
   <si>
@@ -2553,6 +2583,9 @@
   </si>
   <si>
     <t>Global Current  X Rate (0.7%)</t>
+  </si>
+  <si>
+    <t>Commitment Fee Payment Intent Notice</t>
   </si>
   <si>
     <t>CH EDU BILAT DEAL AUD 158.2M 17DEC191610</t>
@@ -3855,7 +3888,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J21" sqref="J21"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3925,8 +3958,8 @@
     <col min="65" max="65" width="9.7109375" style="52" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="26" style="52" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="36.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="68" max="161" width="9.140625" style="52" customWidth="1"/>
-    <col min="162" max="16384" width="9.140625" style="52"/>
+    <col min="68" max="162" width="9.140625" style="52" customWidth="1"/>
+    <col min="163" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6245,9 +6278,131 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="76" t="s">
         <v>621</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>849</v>
+      </c>
+      <c r="C17" s="61"/>
+      <c r="D17" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="67" t="s">
+        <v>422</v>
+      </c>
+      <c r="H17" s="63" t="s">
+        <v>423</v>
+      </c>
+      <c r="I17" s="67" t="s">
+        <v>622</v>
+      </c>
+      <c r="J17" s="67" t="s">
+        <v>623</v>
+      </c>
+      <c r="K17" s="67" t="s">
+        <v>624</v>
+      </c>
+      <c r="L17" s="67" t="s">
+        <v>625</v>
+      </c>
+      <c r="M17" s="63">
+        <v>5</v>
+      </c>
+      <c r="N17" s="63" t="s">
+        <v>459</v>
+      </c>
+      <c r="O17" s="64" t="s">
+        <v>429</v>
+      </c>
+      <c r="P17" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="67" t="s">
+        <v>626</v>
+      </c>
+      <c r="R17" s="67" t="s">
+        <v>626</v>
+      </c>
+      <c r="S17" s="64" t="s">
+        <v>431</v>
+      </c>
+      <c r="T17" s="64" t="s">
+        <v>524</v>
+      </c>
+      <c r="U17" s="64" t="s">
+        <v>433</v>
+      </c>
+      <c r="V17" s="64" t="s">
+        <v>627</v>
+      </c>
+      <c r="W17" s="81" t="s">
+        <v>628</v>
+      </c>
+      <c r="X17" s="81" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y17" s="81" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z17" s="81" t="s">
+        <v>438</v>
+      </c>
+      <c r="AA17" s="81" t="s">
+        <v>439</v>
+      </c>
+      <c r="AB17" s="81" t="s">
+        <v>631</v>
+      </c>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="AE17" s="65"/>
+      <c r="AF17" s="66"/>
+      <c r="AG17" s="60"/>
+      <c r="AH17" s="64" t="s">
+        <v>442</v>
+      </c>
+      <c r="AI17" s="60"/>
+      <c r="AJ17" s="63" t="s">
+        <v>443</v>
+      </c>
+      <c r="AK17" s="60"/>
+      <c r="AL17" s="61"/>
+      <c r="AM17" s="61"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="61"/>
+      <c r="AP17" s="60"/>
+      <c r="AQ17" s="60"/>
+      <c r="AR17" s="62"/>
+      <c r="AS17" s="61"/>
+      <c r="AT17" s="61"/>
+      <c r="AU17" s="61"/>
+      <c r="AV17" s="61"/>
+      <c r="AW17" s="61"/>
+      <c r="AX17" s="61"/>
+      <c r="AY17" s="61"/>
+      <c r="AZ17" s="61"/>
+      <c r="BA17" s="61"/>
+      <c r="BB17" s="61"/>
+      <c r="BC17" s="61"/>
+      <c r="BD17" s="61"/>
+      <c r="BE17" s="61"/>
+      <c r="BF17" s="61"/>
+      <c r="BG17" s="61"/>
+      <c r="BH17" s="61"/>
+      <c r="BI17" s="61"/>
+      <c r="BJ17" s="61"/>
+      <c r="BK17" s="61"/>
+      <c r="BL17" s="61"/>
+      <c r="BM17" s="61"/>
+      <c r="BN17" s="61"/>
+      <c r="BO17" s="59" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6308,16 +6463,16 @@
         <v>362</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="E1" s="68" t="s">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="F1" s="68" t="s">
-        <v>624</v>
+        <v>634</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>625</v>
+        <v>635</v>
       </c>
       <c r="H1" s="68" t="s">
         <v>400</v>
@@ -6326,13 +6481,13 @@
         <v>401</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="K1" s="68" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="M1" s="68" t="s">
         <v>404</v>
@@ -6344,43 +6499,43 @@
         <v>343</v>
       </c>
       <c r="P1" s="68" t="s">
-        <v>629</v>
+        <v>639</v>
       </c>
       <c r="Q1" s="68" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="R1" s="68" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="S1" s="68" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="T1" s="68" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="U1" s="68" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="V1" s="68" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="W1" s="68" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
       <c r="X1" s="68" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="Y1" s="68" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="Z1" s="68" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="AA1" s="68" t="s">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="AB1" s="68" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -6388,7 +6543,7 @@
         <v>72</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>642</v>
+        <v>652</v>
       </c>
       <c r="C2" s="93">
         <v>60002878</v>
@@ -6412,25 +6567,25 @@
         <v>217</v>
       </c>
       <c r="J2" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="K2" t="s">
         <v>105</v>
       </c>
       <c r="L2" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="N2" t="s">
         <v>354</v>
       </c>
       <c r="O2" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="P2" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q2" s="37" t="s">
         <v>350</v>
@@ -6445,19 +6600,19 @@
         <v>350</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="V2" s="37" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="X2" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y2" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="Z2" t="s">
         <v>105</v>
@@ -6470,7 +6625,7 @@
         <v>453</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>653</v>
+        <v>663</v>
       </c>
       <c r="C3" s="93">
         <v>60002979</v>
@@ -6485,61 +6640,61 @@
         <v>113</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="I3" s="37" t="s">
         <v>217</v>
       </c>
       <c r="J3" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="K3" t="s">
         <v>105</v>
       </c>
       <c r="L3" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="N3" s="73"/>
       <c r="O3" s="73"/>
       <c r="P3" s="73"/>
       <c r="Q3" s="37" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="R3" s="37" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="S3" s="37" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="T3" s="37" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="U3" s="37" t="s">
-        <v>656</v>
+        <v>666</v>
       </c>
       <c r="V3" s="37" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="W3" s="37" t="s">
-        <v>657</v>
+        <v>667</v>
       </c>
       <c r="X3" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y3" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="Z3" t="s">
         <v>105</v>
       </c>
       <c r="AA3" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="AB3" s="73"/>
     </row>
@@ -6548,10 +6703,10 @@
         <v>466</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="C4" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="D4" t="s">
         <v>218</v>
@@ -6563,57 +6718,57 @@
         <v>113</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="I4" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J4" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="K4" t="s">
         <v>105</v>
       </c>
       <c r="L4" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="N4" s="73"/>
       <c r="O4" s="73"/>
       <c r="P4" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q4" s="37" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="R4" s="37" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="S4" s="37" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="U4" s="37" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="V4" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="W4" s="37" t="s">
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="X4" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y4" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="Z4" t="s">
         <v>105</v>
@@ -6626,10 +6781,10 @@
         <v>479</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>668</v>
+        <v>678</v>
       </c>
       <c r="C5" t="s">
-        <v>669</v>
+        <v>679</v>
       </c>
       <c r="D5" t="s">
         <v>218</v>
@@ -6641,57 +6796,57 @@
         <v>113</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J5" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="K5" t="s">
         <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="N5" s="73"/>
       <c r="O5" s="73"/>
       <c r="P5" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="R5" s="37" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="S5" s="37" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="T5" s="37" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="U5" s="37" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="V5" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="W5" s="37" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="X5" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y5" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="Z5" t="s">
         <v>105</v>
@@ -6704,10 +6859,10 @@
         <v>492</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>673</v>
+        <v>683</v>
       </c>
       <c r="C6" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="D6" t="s">
         <v>218</v>
@@ -6719,57 +6874,57 @@
         <v>113</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>675</v>
+        <v>685</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="I6" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J6" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="K6" t="s">
         <v>105</v>
       </c>
       <c r="L6" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>677</v>
+        <v>687</v>
       </c>
       <c r="N6" s="73"/>
       <c r="O6" s="73"/>
       <c r="P6" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q6" s="37" t="s">
+        <v>685</v>
+      </c>
+      <c r="R6" s="37" t="s">
+        <v>685</v>
+      </c>
+      <c r="S6" s="37" t="s">
+        <v>685</v>
+      </c>
+      <c r="T6" s="37" t="s">
+        <v>685</v>
+      </c>
+      <c r="U6" s="37" t="s">
+        <v>688</v>
+      </c>
+      <c r="V6" s="37" t="s">
         <v>675</v>
       </c>
-      <c r="R6" s="37" t="s">
-        <v>675</v>
-      </c>
-      <c r="S6" s="37" t="s">
-        <v>675</v>
-      </c>
-      <c r="T6" s="37" t="s">
-        <v>675</v>
-      </c>
-      <c r="U6" s="37" t="s">
-        <v>678</v>
-      </c>
-      <c r="V6" s="37" t="s">
-        <v>665</v>
-      </c>
       <c r="W6" s="37" t="s">
-        <v>679</v>
+        <v>689</v>
       </c>
       <c r="X6" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y6" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="Z6" t="s">
         <v>105</v>
@@ -6782,10 +6937,10 @@
         <v>504</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>680</v>
+        <v>690</v>
       </c>
       <c r="C7" t="s">
-        <v>681</v>
+        <v>691</v>
       </c>
       <c r="D7" t="s">
         <v>218</v>
@@ -6797,57 +6952,57 @@
         <v>113</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="I7" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J7" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="K7" t="s">
         <v>105</v>
       </c>
       <c r="L7" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="N7" s="73"/>
       <c r="O7" s="73"/>
       <c r="P7" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q7" s="37" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="R7" s="37" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="T7" s="37" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>684</v>
+        <v>694</v>
       </c>
       <c r="V7" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="W7" s="37" t="s">
-        <v>685</v>
+        <v>695</v>
       </c>
       <c r="X7" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y7" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="Z7" t="s">
         <v>105</v>
@@ -6860,10 +7015,10 @@
         <v>516</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>686</v>
+        <v>696</v>
       </c>
       <c r="C8" t="s">
-        <v>687</v>
+        <v>697</v>
       </c>
       <c r="D8" t="s">
         <v>218</v>
@@ -6875,57 +7030,57 @@
         <v>113</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>689</v>
+        <v>699</v>
       </c>
       <c r="I8" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J8" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="K8" t="s">
         <v>105</v>
       </c>
       <c r="L8" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="N8" s="73"/>
       <c r="O8" s="73"/>
       <c r="P8" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q8" s="37" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="S8" s="37" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="T8" s="37" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="U8" s="37" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="V8" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="W8" s="37" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
       <c r="X8" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y8" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="Z8" t="s">
         <v>105</v>
@@ -6938,10 +7093,10 @@
         <v>530</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>692</v>
+        <v>702</v>
       </c>
       <c r="C9" t="s">
-        <v>693</v>
+        <v>703</v>
       </c>
       <c r="D9" t="s">
         <v>218</v>
@@ -6953,57 +7108,57 @@
         <v>113</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>695</v>
+        <v>705</v>
       </c>
       <c r="I9" s="37" t="s">
         <v>258</v>
       </c>
       <c r="J9" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="K9" t="s">
         <v>105</v>
       </c>
       <c r="L9" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
       <c r="P9" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q9" s="37" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="S9" s="37" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="T9" s="37" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="U9" s="37" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="V9" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="W9" s="37" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
       <c r="X9" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y9" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="Z9" t="s">
         <v>105</v>
@@ -7016,10 +7171,10 @@
         <v>541</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c r="C10" s="83" t="s">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="D10" t="s">
         <v>218</v>
@@ -7031,7 +7186,7 @@
         <v>113</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="H10" s="37" t="s">
         <v>247</v>
@@ -7040,52 +7195,52 @@
         <v>217</v>
       </c>
       <c r="J10" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="K10" t="s">
         <v>105</v>
       </c>
       <c r="L10" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="N10" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="O10" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="P10" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="S10" s="37" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="U10" s="37" t="s">
-        <v>701</v>
+        <v>711</v>
       </c>
       <c r="V10" s="37" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="W10" s="37" t="s">
-        <v>702</v>
+        <v>712</v>
       </c>
       <c r="X10" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="Y10" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="Z10" t="s">
         <v>105</v>
@@ -7119,8 +7274,8 @@
     <col min="3" max="3" width="29.42578125" style="72" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="72" customWidth="1"/>
-    <col min="6" max="55" width="8.7109375" style="72" customWidth="1"/>
-    <col min="56" max="16384" width="8.7109375" style="72"/>
+    <col min="6" max="56" width="8.7109375" style="72" customWidth="1"/>
+    <col min="57" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7131,13 +7286,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>703</v>
+        <v>713</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>705</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7145,16 +7300,16 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>706</v>
+        <v>716</v>
       </c>
       <c r="C2" t="s">
-        <v>706</v>
+        <v>716</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7188,8 +7343,8 @@
     <col min="5" max="5" width="30.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.140625" style="72" customWidth="1"/>
     <col min="7" max="7" width="24" style="72" bestFit="1" customWidth="1"/>
-    <col min="8" max="56" width="8.7109375" style="72" customWidth="1"/>
-    <col min="57" max="16384" width="8.7109375" style="72"/>
+    <col min="8" max="57" width="8.7109375" style="72" customWidth="1"/>
+    <col min="58" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7200,16 +7355,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>710</v>
+        <v>720</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>711</v>
+        <v>721</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>712</v>
+        <v>722</v>
       </c>
       <c r="G1" s="71" t="s">
         <v>164</v>
@@ -7220,19 +7375,19 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>713</v>
+        <v>723</v>
       </c>
       <c r="C2" t="s">
         <v>189</v>
       </c>
       <c r="D2" s="75" t="s">
-        <v>714</v>
+        <v>724</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>716</v>
+        <v>726</v>
       </c>
       <c r="G2" s="75" t="s">
         <v>250</v>
@@ -7243,22 +7398,22 @@
         <v>453</v>
       </c>
       <c r="B3" t="s">
-        <v>717</v>
+        <v>727</v>
       </c>
       <c r="C3" t="s">
         <v>189</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>718</v>
+        <v>728</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>716</v>
+        <v>726</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>695</v>
+        <v>705</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7307,8 +7462,8 @@
     <col min="20" max="20" width="22.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22.7109375" style="72" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27.42578125" style="72" bestFit="1" customWidth="1"/>
-    <col min="23" max="60" width="8.7109375" style="72" customWidth="1"/>
-    <col min="61" max="16384" width="8.7109375" style="72"/>
+    <col min="23" max="61" width="8.7109375" style="72" customWidth="1"/>
+    <col min="62" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7322,34 +7477,34 @@
         <v>339</v>
       </c>
       <c r="D1" s="71" t="s">
-        <v>719</v>
+        <v>729</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>721</v>
+        <v>731</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>722</v>
+        <v>732</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>723</v>
+        <v>733</v>
       </c>
       <c r="I1" s="71" t="s">
         <v>417</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
       <c r="L1" s="71" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
       <c r="M1" s="71" t="s">
-        <v>727</v>
+        <v>737</v>
       </c>
       <c r="N1" s="71" t="s">
         <v>342</v>
@@ -7361,10 +7516,10 @@
         <v>346</v>
       </c>
       <c r="Q1" s="71" t="s">
-        <v>728</v>
+        <v>738</v>
       </c>
       <c r="R1" s="71" t="s">
-        <v>729</v>
+        <v>739</v>
       </c>
       <c r="S1" s="89" t="s">
         <v>347</v>
@@ -7373,10 +7528,10 @@
         <v>348</v>
       </c>
       <c r="U1" s="71" t="s">
-        <v>730</v>
+        <v>740</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -7384,7 +7539,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>731</v>
+        <v>741</v>
       </c>
       <c r="C2" t="s">
         <v>187</v>
@@ -7402,13 +7557,13 @@
         <v>248</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>732</v>
+        <v>742</v>
       </c>
       <c r="I2" s="75" t="s">
         <v>248</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>732</v>
+        <v>742</v>
       </c>
       <c r="K2" s="90"/>
       <c r="L2" s="91"/>
@@ -7428,7 +7583,7 @@
         <v>453</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>733</v>
+        <v>743</v>
       </c>
       <c r="C3" s="72" t="s">
         <v>186</v>
@@ -7446,37 +7601,37 @@
         <v>248</v>
       </c>
       <c r="H3" s="85" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="I3" s="75" t="s">
         <v>248</v>
       </c>
       <c r="J3" s="85" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="K3" s="85" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="L3" s="85" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="M3" s="85" t="s">
         <v>447</v>
       </c>
       <c r="N3" s="72" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="O3" s="72" t="s">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="P3" t="s">
         <v>358</v>
       </c>
       <c r="Q3" s="85" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="R3" s="86" t="s">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="S3" s="87" t="s">
         <v>359</v>
@@ -7485,7 +7640,7 @@
         <v>357</v>
       </c>
       <c r="U3" s="72" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="V3" s="91"/>
     </row>
@@ -7494,7 +7649,7 @@
         <v>466</v>
       </c>
       <c r="B4" s="72" t="s">
-        <v>733</v>
+        <v>743</v>
       </c>
       <c r="C4" s="72" t="s">
         <v>186</v>
@@ -7506,34 +7661,34 @@
         <v>247</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>737</v>
+        <v>747</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="H4" s="85" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="I4" s="75" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="J4" s="85" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="K4" s="85" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="L4" s="85" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="M4" s="85" t="s">
         <v>447</v>
       </c>
       <c r="N4" s="72" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="O4" s="72" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="P4" s="91"/>
       <c r="Q4" s="91"/>
@@ -7552,7 +7707,7 @@
       <c r="D5" s="84"/>
       <c r="F5" s="75"/>
       <c r="R5" s="88" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
     </row>
   </sheetData>
@@ -7606,8 +7761,8 @@
     <col min="33" max="34" width="23.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19.140625" style="72" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="78.140625" style="72" bestFit="1" customWidth="1"/>
-    <col min="37" max="61" width="8.7109375" style="72" customWidth="1"/>
-    <col min="62" max="16384" width="8.7109375" style="72"/>
+    <col min="37" max="62" width="8.7109375" style="72" customWidth="1"/>
+    <col min="63" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -7618,100 +7773,100 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>417</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
       <c r="G1" s="77" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
       <c r="H1" s="77" t="s">
-        <v>746</v>
+        <v>756</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>747</v>
+        <v>757</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>748</v>
+        <v>758</v>
       </c>
       <c r="K1" s="71" t="s">
-        <v>749</v>
+        <v>759</v>
       </c>
       <c r="L1" s="68" t="s">
+        <v>649</v>
+      </c>
+      <c r="M1" s="71" t="s">
         <v>639</v>
       </c>
-      <c r="M1" s="71" t="s">
-        <v>629</v>
-      </c>
       <c r="N1" s="68" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="O1" s="71" t="s">
-        <v>750</v>
+        <v>760</v>
       </c>
       <c r="P1" s="71" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="Q1" s="71" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="R1" s="71" t="s">
-        <v>753</v>
+        <v>763</v>
       </c>
       <c r="S1" s="68" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="T1" s="68" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="U1" s="68" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="V1" s="68" t="s">
+        <v>643</v>
+      </c>
+      <c r="W1" s="68" t="s">
+        <v>644</v>
+      </c>
+      <c r="X1" s="68" t="s">
+        <v>645</v>
+      </c>
+      <c r="Y1" s="68" t="s">
+        <v>646</v>
+      </c>
+      <c r="Z1" s="68" t="s">
+        <v>647</v>
+      </c>
+      <c r="AA1" s="68" t="s">
+        <v>648</v>
+      </c>
+      <c r="AB1" s="68" t="s">
         <v>633</v>
       </c>
-      <c r="W1" s="68" t="s">
-        <v>634</v>
-      </c>
-      <c r="X1" s="68" t="s">
-        <v>635</v>
-      </c>
-      <c r="Y1" s="68" t="s">
+      <c r="AC1" s="68" t="s">
         <v>636</v>
-      </c>
-      <c r="Z1" s="68" t="s">
-        <v>637</v>
-      </c>
-      <c r="AA1" s="68" t="s">
-        <v>638</v>
-      </c>
-      <c r="AB1" s="68" t="s">
-        <v>623</v>
-      </c>
-      <c r="AC1" s="68" t="s">
-        <v>626</v>
       </c>
       <c r="AD1" s="71" t="s">
         <v>105</v>
       </c>
       <c r="AE1" s="71" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="AF1" s="71" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="AG1" s="71" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="AH1" s="71" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
       <c r="AI1" s="71" t="s">
         <v>342</v>
@@ -7725,40 +7880,40 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="C2" t="s">
         <v>218</v>
       </c>
       <c r="D2" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="G2" s="75" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="H2" s="75" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="I2" s="79" t="s">
-        <v>762</v>
+        <v>772</v>
       </c>
       <c r="J2" s="75" t="s">
-        <v>763</v>
+        <v>773</v>
       </c>
       <c r="K2" s="75" t="s">
-        <v>764</v>
+        <v>774</v>
       </c>
       <c r="L2" t="s">
         <v>105</v>
       </c>
       <c r="M2" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N2" t="s">
         <v>218</v>
@@ -7788,28 +7943,28 @@
         <v>453</v>
       </c>
       <c r="B3" t="s">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="C3" t="s">
         <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E3" s="75" t="s">
-        <v>677</v>
+        <v>687</v>
       </c>
       <c r="F3" s="75" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="I3" s="79" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="J3" s="79"/>
       <c r="K3" s="79"/>
@@ -7817,53 +7972,53 @@
         <v>105</v>
       </c>
       <c r="M3" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N3" t="s">
         <v>218</v>
       </c>
       <c r="O3" s="75" t="s">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c r="P3" s="75" t="s">
-        <v>770</v>
+        <v>780</v>
       </c>
       <c r="Q3" s="79"/>
       <c r="R3" s="75" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="S3" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="T3" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="U3" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="V3" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="W3" s="75" t="s">
-        <v>771</v>
+        <v>781</v>
       </c>
       <c r="X3" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="Y3" s="37" t="s">
-        <v>772</v>
+        <v>782</v>
       </c>
       <c r="Z3" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA3" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="AB3" t="s">
         <v>177</v>
       </c>
       <c r="AC3" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="AD3" s="78"/>
       <c r="AE3" s="78"/>
@@ -7875,28 +8030,28 @@
         <v>466</v>
       </c>
       <c r="B4" t="s">
-        <v>773</v>
+        <v>783</v>
       </c>
       <c r="C4" t="s">
         <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="F4" s="80" t="s">
-        <v>774</v>
+        <v>784</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="H4" s="75" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="I4" s="79" t="s">
-        <v>777</v>
+        <v>787</v>
       </c>
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
@@ -7904,55 +8059,55 @@
         <v>105</v>
       </c>
       <c r="M4" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N4" t="s">
         <v>218</v>
       </c>
       <c r="O4" s="75" t="s">
-        <v>778</v>
+        <v>788</v>
       </c>
       <c r="P4" s="75" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
       <c r="Q4" s="75" t="s">
-        <v>780</v>
+        <v>790</v>
       </c>
       <c r="R4" s="75" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="S4" s="75" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="T4" s="75" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="U4" s="75" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="V4" s="75" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="W4" s="75" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
       <c r="X4" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>783</v>
+        <v>793</v>
       </c>
       <c r="Z4" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA4" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="AB4" t="s">
         <v>177</v>
       </c>
       <c r="AC4" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="AD4" s="78"/>
       <c r="AE4" s="78"/>
@@ -7964,25 +8119,25 @@
         <v>479</v>
       </c>
       <c r="B5" t="s">
-        <v>784</v>
+        <v>794</v>
       </c>
       <c r="C5" t="s">
         <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="G5" s="80" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>785</v>
+        <v>795</v>
       </c>
       <c r="I5" s="75" t="s">
         <v>105</v>
@@ -7993,51 +8148,51 @@
         <v>105</v>
       </c>
       <c r="M5" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N5" t="s">
         <v>218</v>
       </c>
       <c r="O5" s="75" t="s">
-        <v>786</v>
+        <v>796</v>
       </c>
       <c r="P5" s="79"/>
       <c r="Q5" s="79"/>
       <c r="R5" s="75" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="S5" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="T5" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="U5" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="V5" s="75" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="W5" s="75" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
       <c r="X5" s="37" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>783</v>
+        <v>793</v>
       </c>
       <c r="Z5" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA5" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="AB5" t="s">
         <v>177</v>
       </c>
       <c r="AC5" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="AD5" s="72" t="s">
         <v>105</v>
@@ -8051,25 +8206,25 @@
         <v>492</v>
       </c>
       <c r="B6" s="72" t="s">
-        <v>787</v>
+        <v>797</v>
       </c>
       <c r="C6" t="s">
         <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E6" s="75" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="F6" s="75" t="s">
-        <v>774</v>
+        <v>784</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>788</v>
+        <v>798</v>
       </c>
       <c r="H6" t="s">
-        <v>789</v>
+        <v>799</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
@@ -8078,53 +8233,53 @@
         <v>105</v>
       </c>
       <c r="M6" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N6" t="s">
         <v>218</v>
       </c>
       <c r="O6" s="75" t="s">
-        <v>790</v>
+        <v>800</v>
       </c>
       <c r="P6" s="75" t="s">
-        <v>791</v>
+        <v>801</v>
       </c>
       <c r="Q6" s="79"/>
       <c r="R6" s="75" t="s">
-        <v>792</v>
+        <v>802</v>
       </c>
       <c r="S6" s="75" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
       <c r="T6" s="75" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
       <c r="U6" s="75" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
       <c r="V6" s="75" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
       <c r="W6" s="75" t="s">
-        <v>794</v>
+        <v>804</v>
       </c>
       <c r="X6" s="37" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="Y6" s="37" t="s">
-        <v>795</v>
+        <v>805</v>
       </c>
       <c r="Z6" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA6" s="72" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="AB6" t="s">
         <v>177</v>
       </c>
       <c r="AC6" s="72" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="AD6" s="78"/>
       <c r="AE6" s="92" t="s">
@@ -8138,25 +8293,25 @@
         <v>504</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>796</v>
+        <v>806</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="H7" t="s">
-        <v>798</v>
+        <v>808</v>
       </c>
       <c r="I7" s="72" t="s">
         <v>105</v>
@@ -8167,58 +8322,58 @@
         <v>105</v>
       </c>
       <c r="M7" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N7" s="72" t="s">
         <v>218</v>
       </c>
       <c r="O7" s="75" t="s">
-        <v>799</v>
+        <v>809</v>
       </c>
       <c r="P7" s="78"/>
       <c r="Q7" s="78"/>
       <c r="R7" s="75" t="s">
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="S7" s="95" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="T7" s="95" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="U7" s="95" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="V7" s="95" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="W7" s="75" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="X7" s="37" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
       <c r="Y7" s="37" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
       <c r="Z7" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA7" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="AB7" t="s">
         <v>177</v>
       </c>
       <c r="AC7" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="AD7" s="72" t="s">
         <v>105</v>
       </c>
       <c r="AE7" s="78"/>
       <c r="AF7" s="75" t="s">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="AG7" s="72" t="s">
         <v>118</v>
@@ -8234,25 +8389,25 @@
         <v>516</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>805</v>
+        <v>815</v>
       </c>
       <c r="C8" s="72" t="s">
         <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>806</v>
+        <v>816</v>
       </c>
       <c r="H8" t="s">
-        <v>807</v>
+        <v>817</v>
       </c>
       <c r="I8" s="72" t="s">
         <v>105</v>
@@ -8263,51 +8418,51 @@
         <v>105</v>
       </c>
       <c r="M8" s="72" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="N8" s="72" t="s">
         <v>218</v>
       </c>
       <c r="O8" s="75" t="s">
-        <v>808</v>
+        <v>818</v>
       </c>
       <c r="P8" s="78"/>
       <c r="Q8" s="78"/>
       <c r="R8" s="75" t="s">
-        <v>792</v>
+        <v>802</v>
       </c>
       <c r="S8" s="95" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
       <c r="T8" s="95" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
       <c r="U8" s="95" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
       <c r="V8" s="95" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
       <c r="W8" s="75" t="s">
-        <v>810</v>
+        <v>820</v>
       </c>
       <c r="X8" s="37" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="Y8" s="37" t="s">
-        <v>811</v>
+        <v>821</v>
       </c>
       <c r="Z8" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="AA8" s="72" t="s">
-        <v>812</v>
+        <v>822</v>
       </c>
       <c r="AB8" t="s">
         <v>177</v>
       </c>
       <c r="AC8" s="72" t="s">
-        <v>812</v>
+        <v>822</v>
       </c>
       <c r="AD8" s="78"/>
       <c r="AE8" s="78"/>
@@ -8315,10 +8470,10 @@
       <c r="AG8" s="78"/>
       <c r="AH8" s="78"/>
       <c r="AI8" s="72" t="s">
-        <v>813</v>
+        <v>823</v>
       </c>
       <c r="AJ8" s="72" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>
@@ -8367,8 +8522,8 @@
     <col min="28" max="28" width="14.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="25.28515625" style="72" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" style="72" customWidth="1"/>
-    <col min="31" max="61" width="8.7109375" style="72" customWidth="1"/>
-    <col min="62" max="16384" width="8.7109375" style="72"/>
+    <col min="31" max="62" width="8.7109375" style="72" customWidth="1"/>
+    <col min="63" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -8379,25 +8534,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>816</v>
+        <v>826</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="F1" s="71" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="H1" s="71" t="s">
-        <v>820</v>
+        <v>830</v>
       </c>
       <c r="I1" s="71" t="s">
-        <v>821</v>
+        <v>831</v>
       </c>
       <c r="L1" s="68"/>
       <c r="N1" s="68"/>
@@ -8418,19 +8573,19 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>822</v>
+        <v>832</v>
       </c>
       <c r="C2" t="s">
-        <v>823</v>
+        <v>833</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="F2" s="75" t="s">
-        <v>825</v>
+        <v>835</v>
       </c>
       <c r="G2" s="75">
         <v>1</v>
@@ -8461,22 +8616,22 @@
         <v>453</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>826</v>
+        <v>836</v>
       </c>
       <c r="C3" s="78"/>
       <c r="D3" s="78"/>
       <c r="E3" s="75" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="F3" s="78"/>
       <c r="G3" s="75">
         <v>1</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>827</v>
+        <v>837</v>
       </c>
       <c r="I3" s="75" t="s">
-        <v>828</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -8554,8 +8709,8 @@
     <col min="54" max="54" width="12.85546875" style="72" bestFit="1" customWidth="1"/>
     <col min="55" max="56" width="18.5703125" style="72" bestFit="1" customWidth="1"/>
     <col min="57" max="58" width="17.5703125" style="72" bestFit="1" customWidth="1"/>
-    <col min="59" max="65" width="8.7109375" style="72" customWidth="1"/>
-    <col min="66" max="16384" width="8.7109375" style="72"/>
+    <col min="59" max="66" width="8.7109375" style="72" customWidth="1"/>
+    <col min="67" max="16384" width="8.7109375" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="71" customFormat="1" x14ac:dyDescent="0.2">
@@ -8566,13 +8721,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>829</v>
+        <v>839</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>830</v>
+        <v>840</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>831</v>
+        <v>841</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>223</v>
@@ -8716,10 +8871,10 @@
         <v>302</v>
       </c>
       <c r="BA1" s="71" t="s">
-        <v>832</v>
+        <v>842</v>
       </c>
       <c r="BB1" s="71" t="s">
-        <v>833</v>
+        <v>843</v>
       </c>
     </row>
     <row r="2" spans="1:58" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8727,16 +8882,16 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>834</v>
+        <v>844</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="E2" s="82" t="s">
-        <v>835</v>
+        <v>845</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>240</v>
@@ -8781,7 +8936,7 @@
         <v>308</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
       <c r="U2" t="s">
         <v>109</v>
@@ -8808,7 +8963,7 @@
         <v>308</v>
       </c>
       <c r="AC2" s="44" t="s">
-        <v>837</v>
+        <v>847</v>
       </c>
       <c r="AD2" t="s">
         <v>312</v>
@@ -8844,7 +8999,7 @@
         <v>313</v>
       </c>
       <c r="AO2" s="44" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
       <c r="AP2" t="s">
         <v>109</v>
@@ -8877,13 +9032,13 @@
         <v>313</v>
       </c>
       <c r="AZ2" s="44" t="s">
-        <v>837</v>
+        <v>847</v>
       </c>
       <c r="BA2" s="72" t="s">
-        <v>838</v>
+        <v>848</v>
       </c>
       <c r="BB2" s="75" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
       <c r="BC2" s="75"/>
       <c r="BD2" s="75"/>
@@ -8903,8 +9058,8 @@
   </sheetPr>
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8955,8 +9110,8 @@
     <col min="44" max="44" width="24" style="31" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="11.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="47" max="92" width="9.140625" style="31" customWidth="1"/>
-    <col min="93" max="16384" width="9.140625" style="31"/>
+    <col min="47" max="93" width="9.140625" style="31" customWidth="1"/>
+    <col min="94" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" s="22" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9113,10 +9268,10 @@
         <v>169</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>839</v>
+        <v>850</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>840</v>
+        <v>851</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>113</v>
@@ -9301,8 +9456,8 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9398,7 +9553,7 @@
         <v>212</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>841</v>
+        <v>852</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>213</v>

</xml_diff>